<commit_message>
N balance returning in excel but not full array, needs debugging
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6285738-474F-4009-BCCA-3CD019B14CCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACE8B6-7C59-494E-A3FD-F3236842350E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <definedName name="Type">CropCoefficients!$E$3:$E$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="281">
   <si>
     <t>EndUse</t>
   </si>
@@ -883,6 +884,9 @@
   </si>
   <si>
     <t>Oat Grain General</t>
+  </si>
+  <si>
+    <t>InitialN</t>
   </si>
 </sst>
 </file>
@@ -952,7 +956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1066,11 +1070,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1115,36 +1160,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2538,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2548,9 +2585,9 @@
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -2575,7 +2612,7 @@
       <c r="N1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="36" t="s">
         <v>248</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -2585,9 +2622,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
       <c r="A2" s="26">
-        <f>K8</f>
+        <f>K9</f>
         <v>44929</v>
       </c>
       <c r="B2">
@@ -2597,22 +2634,12 @@
         <v>12</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="H2" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="30" t="str">
-        <f>H2&amp;I2</f>
-        <v>PriorCropName</v>
-      </c>
-      <c r="K2" s="31" t="str">
-        <f>L2</f>
-        <v>Annual ryegrass Fodder General</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>275</v>
+      <c r="J2" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="K2" s="41">
+        <f>IF(L2="",50,L2)</f>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
         <v>32</v>
@@ -2627,7 +2654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="26">
         <f>A2+1</f>
         <v>44930</v>
@@ -2643,22 +2670,23 @@
       <c r="G3">
         <v>7</v>
       </c>
-      <c r="H3" s="32" t="str">
-        <f>H2</f>
-        <v>Prior</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="J3" s="34" t="str">
-        <f t="shared" ref="J3:J13" si="0">H3&amp;I3</f>
-        <v>PriorSaleableYield</v>
-      </c>
-      <c r="K3" s="35">
-        <f>IF(L3="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G3,FALSE),L3)</f>
-        <v>5</v>
-      </c>
-      <c r="L3" s="43"/>
+      <c r="H3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" t="s">
+        <v>270</v>
+      </c>
+      <c r="J3" s="29" t="str">
+        <f>H3&amp;I3</f>
+        <v>PriorCropName</v>
+      </c>
+      <c r="K3" s="30" t="str">
+        <f>L3</f>
+        <v>Annual ryegrass Fodder General</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>275</v>
+      </c>
       <c r="N3" t="s">
         <v>123</v>
       </c>
@@ -2674,7 +2702,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="26">
-        <f t="shared" ref="A4:A33" si="1">A3+1</f>
+        <f t="shared" ref="A4:A33" si="0">A3+1</f>
         <v>44931</v>
       </c>
       <c r="B4">
@@ -2688,20 +2716,20 @@
       <c r="G4">
         <v>8</v>
       </c>
-      <c r="H4" s="32" t="str">
-        <f t="shared" ref="H4:H13" si="2">H3</f>
+      <c r="H4" t="str">
+        <f>H3</f>
         <v>Prior</v>
       </c>
-      <c r="I4" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="J4" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>PriorUnits</v>
-      </c>
-      <c r="K4" s="35" t="str">
-        <f>IF(L4="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G4,FALSE),L4)</f>
-        <v>t/ha</v>
+      <c r="I4" t="s">
+        <v>256</v>
+      </c>
+      <c r="J4" s="31" t="str">
+        <f t="shared" ref="J4:J14" si="1">H4&amp;I4</f>
+        <v>PriorSaleableYield</v>
+      </c>
+      <c r="K4" s="32">
+        <f>IF(L4="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G3,FALSE),L4)</f>
+        <v>5</v>
       </c>
       <c r="L4" s="43"/>
       <c r="O4" t="s">
@@ -2713,34 +2741,34 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44932</v>
       </c>
       <c r="B5">
         <v>13.912023293050638</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C33" si="3">B5+C4</f>
+        <f t="shared" ref="C5:C33" si="2">B5+C4</f>
         <v>47.988434756431076</v>
       </c>
       <c r="E5" s="1"/>
       <c r="G5">
         <v>12</v>
       </c>
-      <c r="H5" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5:H14" si="3">H4</f>
         <v>Prior</v>
       </c>
-      <c r="I5" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="J5" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>PriorFieldLoss</v>
-      </c>
-      <c r="K5" s="35">
-        <f>IF(L5="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G5,FALSE),L5)</f>
-        <v>0</v>
+      <c r="I5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorUnits</v>
+      </c>
+      <c r="K5" s="32" t="str">
+        <f>IF(L5="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G4,FALSE),L5)</f>
+        <v>t/ha</v>
       </c>
       <c r="L5" s="43"/>
       <c r="O5" t="s">
@@ -2752,33 +2780,33 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44933</v>
       </c>
       <c r="B6">
         <v>4.1491642970301701</v>
       </c>
       <c r="C6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>52.137599053461244</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6">
         <v>11</v>
       </c>
-      <c r="H6" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
         <v>Prior</v>
       </c>
-      <c r="I6" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="J6" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>PriorDressingLoss</v>
-      </c>
-      <c r="K6" s="35">
-        <f>IF(L6="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G6,FALSE),L6)</f>
+      <c r="I6" t="s">
+        <v>258</v>
+      </c>
+      <c r="J6" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorFieldLoss</v>
+      </c>
+      <c r="K6" s="32">
+        <f>IF(L6="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G5,FALSE),L6)</f>
         <v>0</v>
       </c>
       <c r="L6" s="43"/>
@@ -2791,985 +2819,1005 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44934</v>
       </c>
       <c r="B7">
         <v>11.680823993463974</v>
       </c>
       <c r="C7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>63.818423046925219</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7">
         <v>15</v>
       </c>
-      <c r="H7" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
         <v>Prior</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="J7" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>PriorMoistureContent</v>
-      </c>
-      <c r="K7" s="35">
-        <f>IF(L7="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G7,FALSE),L7)</f>
-        <v>80</v>
+      <c r="I7" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorDressingLoss</v>
+      </c>
+      <c r="K7" s="32">
+        <f>IF(L7="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G6,FALSE),L7)</f>
+        <v>0</v>
       </c>
       <c r="L7" s="43"/>
       <c r="O7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1">
       <c r="A8" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44935</v>
       </c>
       <c r="B8">
         <v>11.289351844181724</v>
       </c>
       <c r="C8">
+        <f t="shared" si="2"/>
+        <v>75.107774891106942</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="H8" t="str">
         <f t="shared" si="3"/>
-        <v>75.107774891106942</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="H8" s="32" t="str">
-        <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="I8" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="J8" s="34" t="str">
+      <c r="I8" t="s">
+        <v>260</v>
+      </c>
+      <c r="J8" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorMoistureContent</v>
+      </c>
+      <c r="K8" s="32">
+        <f>IF(L8="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G7,FALSE),L8)</f>
+        <v>80</v>
+      </c>
+      <c r="L8" s="43"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A9" s="26">
         <f t="shared" si="0"/>
-        <v>PriorEstablishDate</v>
-      </c>
-      <c r="K8" s="36">
-        <f>L8</f>
-        <v>44929</v>
-      </c>
-      <c r="L8" s="51">
-        <v>44929</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="26">
-        <f t="shared" si="1"/>
         <v>44936</v>
       </c>
       <c r="B9">
         <v>13.934890823546613</v>
       </c>
       <c r="C9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>89.042665714653552</v>
       </c>
       <c r="E9" s="1"/>
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
         <v>Prior</v>
       </c>
-      <c r="I9" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="J9" s="34" t="str">
+      <c r="I9" t="s">
+        <v>261</v>
+      </c>
+      <c r="J9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorEstablishDate</v>
+      </c>
+      <c r="K9" s="33">
+        <f>L9</f>
+        <v>44929</v>
+      </c>
+      <c r="L9" s="44">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A10" s="26">
         <f t="shared" si="0"/>
-        <v>PriorEstablishStage</v>
-      </c>
-      <c r="K9" s="35" t="str">
-        <f>IF(L9="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G9,FALSE),L9)</f>
-        <v>Seed</v>
-      </c>
-      <c r="L9" s="43"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="26">
-        <f t="shared" si="1"/>
         <v>44937</v>
       </c>
       <c r="B10">
         <v>7.3816990790906738</v>
       </c>
       <c r="C10">
+        <f t="shared" si="2"/>
+        <v>96.424364793744232</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="H10" t="str">
         <f t="shared" si="3"/>
-        <v>96.424364793744232</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="H10" s="32" t="str">
-        <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="I10" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J10" s="34" t="str">
+      <c r="I10" t="s">
+        <v>262</v>
+      </c>
+      <c r="J10" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorEstablishStage</v>
+      </c>
+      <c r="K10" s="32" t="str">
+        <f>IF(L10="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G9,FALSE),L10)</f>
+        <v>Seed</v>
+      </c>
+      <c r="L10" s="43"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A11" s="26">
         <f t="shared" si="0"/>
-        <v>PriorHarvestDate</v>
-      </c>
-      <c r="K10" s="36">
-        <f>L10</f>
-        <v>44938</v>
-      </c>
-      <c r="L10" s="51">
-        <v>44938</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="26">
-        <f t="shared" si="1"/>
         <v>44938</v>
       </c>
       <c r="B11">
         <v>13.932559604705048</v>
       </c>
       <c r="C11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>110.35692439844928</v>
       </c>
       <c r="E11" s="1"/>
       <c r="G11">
         <v>5</v>
       </c>
-      <c r="H11" s="32" t="str">
-        <f t="shared" si="2"/>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
         <v>Prior</v>
       </c>
-      <c r="I11" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="J11" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>PriorHarvestStage</v>
-      </c>
-      <c r="K11" s="35" t="str">
-        <f>IF(L11="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G11,FALSE),L11)</f>
-        <v>EarlyReproductive</v>
-      </c>
-      <c r="L11" s="43"/>
+      <c r="I11" t="s">
+        <v>263</v>
+      </c>
+      <c r="J11" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorHarvestDate</v>
+      </c>
+      <c r="K11" s="33">
+        <f>L11</f>
+        <v>44938</v>
+      </c>
+      <c r="L11" s="44">
+        <v>44938</v>
+      </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44939</v>
       </c>
       <c r="B12">
         <v>5.3540880739901002</v>
       </c>
       <c r="C12">
+        <f t="shared" si="2"/>
+        <v>115.71101247243938</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="H12" t="str">
         <f t="shared" si="3"/>
-        <v>115.71101247243938</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="H12" s="32" t="str">
-        <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="I12" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="J12" s="34" t="str">
+      <c r="I12" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorHarvestStage</v>
+      </c>
+      <c r="K12" s="32" t="str">
+        <f>IF(L12="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G11,FALSE),L12)</f>
+        <v>EarlyReproductive</v>
+      </c>
+      <c r="L12" s="43"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="26">
         <f t="shared" si="0"/>
-        <v>PriorResidueTreatment</v>
-      </c>
-      <c r="K12" s="35" t="str">
-        <f>IF(L12="",P2,L12)</f>
-        <v>None</v>
-      </c>
-      <c r="L12" s="43"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A13" s="26">
-        <f t="shared" si="1"/>
         <v>44940</v>
       </c>
       <c r="B13">
         <v>13.363497784448709</v>
       </c>
       <c r="C13">
+        <f t="shared" si="2"/>
+        <v>129.07451025688809</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="H13" t="str">
         <f t="shared" si="3"/>
-        <v>129.07451025688809</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="H13" s="37" t="str">
-        <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="I13" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="J13" s="39" t="str">
+      <c r="I13" t="s">
+        <v>265</v>
+      </c>
+      <c r="J13" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorResidueTreatment</v>
+      </c>
+      <c r="K13" s="32" t="str">
+        <f>IF(L13="",P2,L13)</f>
+        <v>None</v>
+      </c>
+      <c r="L13" s="43"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A14" s="26">
         <f t="shared" si="0"/>
-        <v>PriorEstablishN</v>
-      </c>
-      <c r="K13" s="40">
-        <f>IF(L13="",0,L13)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="43"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="26">
-        <f t="shared" si="1"/>
         <v>44941</v>
       </c>
       <c r="B14">
         <v>6.6646938971593457</v>
       </c>
       <c r="C14">
+        <f t="shared" si="2"/>
+        <v>135.73920415404743</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="H14" t="str">
         <f t="shared" si="3"/>
-        <v>135.73920415404743</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="H14" s="44" t="s">
-        <v>273</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="J14" s="15" t="str">
-        <f>H14&amp;I14</f>
-        <v>CurrentCropName</v>
-      </c>
-      <c r="K14" s="45" t="str">
-        <f>L14</f>
-        <v>Potato Vegetable General</v>
-      </c>
-      <c r="L14" s="42" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>Prior</v>
+      </c>
+      <c r="I14" t="s">
+        <v>266</v>
+      </c>
+      <c r="J14" s="34" t="str">
+        <f t="shared" si="1"/>
+        <v>PriorEstablishN</v>
+      </c>
+      <c r="K14" s="35">
+        <f>IF(L14="",0,L14)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="43"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1">
       <c r="A15" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44942</v>
       </c>
       <c r="B15">
         <v>15.119829112109056</v>
       </c>
       <c r="C15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>150.85903326615647</v>
       </c>
       <c r="E15" s="1"/>
       <c r="G15">
         <v>7</v>
       </c>
-      <c r="H15" s="18" t="str">
-        <f>H14</f>
-        <v>Current</v>
-      </c>
-      <c r="I15" s="46" t="s">
-        <v>256</v>
-      </c>
-      <c r="J15" s="47" t="str">
-        <f t="shared" ref="J15:J25" si="4">H15&amp;I15</f>
-        <v>CurrentSaleableYield</v>
-      </c>
-      <c r="K15" s="19">
-        <f>IF(L15="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G15,FALSE),L15)</f>
-        <v>10</v>
-      </c>
-      <c r="L15" s="43">
-        <v>10</v>
+      <c r="H15" t="s">
+        <v>273</v>
+      </c>
+      <c r="I15" t="s">
+        <v>270</v>
+      </c>
+      <c r="J15" s="37" t="str">
+        <f>H15&amp;I15</f>
+        <v>CurrentCropName</v>
+      </c>
+      <c r="K15" s="38" t="str">
+        <f>L15</f>
+        <v>Potato Vegetable General</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44943</v>
       </c>
       <c r="B16">
         <v>10.605844567907475</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>161.46487783406394</v>
       </c>
       <c r="E16" s="1"/>
       <c r="G16">
         <v>8</v>
       </c>
-      <c r="H16" s="18" t="str">
-        <f t="shared" ref="H16:H25" si="5">H15</f>
+      <c r="H16" t="str">
+        <f>H15</f>
         <v>Current</v>
       </c>
-      <c r="I16" s="46" t="s">
-        <v>257</v>
-      </c>
-      <c r="J16" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>CurrentUnits</v>
-      </c>
-      <c r="K16" s="19" t="str">
-        <f>IF(L16="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G16,FALSE),L16)</f>
-        <v>kg/ha</v>
-      </c>
-      <c r="L16" s="43" t="s">
-        <v>268</v>
+      <c r="I16" t="s">
+        <v>256</v>
+      </c>
+      <c r="J16" s="18" t="str">
+        <f t="shared" ref="J16:J26" si="4">H16&amp;I16</f>
+        <v>CurrentSaleableYield</v>
+      </c>
+      <c r="K16" s="19">
+        <f>IF(L16="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G15,FALSE),L16)</f>
+        <v>10</v>
+      </c>
+      <c r="L16" s="43">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44944</v>
       </c>
       <c r="B17">
         <v>11.901756295522578</v>
       </c>
       <c r="C17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>173.36663412958652</v>
       </c>
       <c r="E17" s="1"/>
       <c r="G17">
         <v>12</v>
       </c>
-      <c r="H17" s="18" t="str">
-        <f t="shared" si="5"/>
+      <c r="H17" t="str">
+        <f t="shared" ref="H17:H26" si="5">H16</f>
         <v>Current</v>
       </c>
-      <c r="I17" s="46" t="s">
-        <v>258</v>
-      </c>
-      <c r="J17" s="47" t="str">
+      <c r="I17" t="s">
+        <v>257</v>
+      </c>
+      <c r="J17" s="18" t="str">
         <f t="shared" si="4"/>
-        <v>CurrentFieldLoss</v>
-      </c>
-      <c r="K17" s="19">
-        <f>IF(L17="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G17,FALSE),L17)</f>
-        <v>15</v>
-      </c>
-      <c r="L17" s="43">
-        <v>15</v>
+        <v>CurrentUnits</v>
+      </c>
+      <c r="K17" s="19" t="str">
+        <f>IF(L17="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G16,FALSE),L17)</f>
+        <v>kg/ha</v>
+      </c>
+      <c r="L17" s="43" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44945</v>
       </c>
       <c r="B18">
         <v>3.8939814164824327</v>
       </c>
       <c r="C18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>177.26061554606895</v>
       </c>
       <c r="E18" s="1"/>
       <c r="G18">
         <v>11</v>
       </c>
-      <c r="H18" s="18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I18" s="46" t="s">
-        <v>259</v>
-      </c>
-      <c r="J18" s="47" t="str">
+      <c r="I18" t="s">
+        <v>258</v>
+      </c>
+      <c r="J18" s="18" t="str">
         <f t="shared" si="4"/>
-        <v>CurrentDressingLoss</v>
+        <v>CurrentFieldLoss</v>
       </c>
       <c r="K18" s="19">
-        <f>IF(L18="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G18,FALSE),L18)</f>
-        <v>10</v>
+        <f>IF(L18="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G17,FALSE),L18)</f>
+        <v>15</v>
       </c>
       <c r="L18" s="43">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44946</v>
       </c>
       <c r="B19">
         <v>6.2562047514789443</v>
       </c>
       <c r="C19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>183.51682029754789</v>
       </c>
       <c r="E19" s="1"/>
       <c r="G19">
         <v>15</v>
       </c>
-      <c r="H19" s="18" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I19" s="46" t="s">
+      <c r="I19" t="s">
+        <v>259</v>
+      </c>
+      <c r="J19" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>CurrentDressingLoss</v>
+      </c>
+      <c r="K19" s="19">
+        <f>IF(L19="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G18,FALSE),L19)</f>
+        <v>10</v>
+      </c>
+      <c r="L19" s="43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A20" s="26">
+        <f t="shared" si="0"/>
+        <v>44947</v>
+      </c>
+      <c r="B20">
+        <v>5.2802002140493496</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>188.79702051159725</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="H20" t="str">
+        <f t="shared" si="5"/>
+        <v>Current</v>
+      </c>
+      <c r="I20" t="s">
         <v>260</v>
       </c>
-      <c r="J19" s="47" t="str">
+      <c r="J20" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentMoistureContent</v>
       </c>
-      <c r="K19" s="19">
-        <f>IF(L19="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G19,FALSE),L19)</f>
+      <c r="K20" s="19">
+        <f>IF(L20="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G19,FALSE),L20)</f>
         <v>72</v>
       </c>
-      <c r="L19" s="43">
+      <c r="L20" s="43">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="26">
-        <f t="shared" si="1"/>
-        <v>44947</v>
-      </c>
-      <c r="B20">
-        <v>5.2802002140493496</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="3"/>
-        <v>188.79702051159725</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="H20" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>Current</v>
-      </c>
-      <c r="I20" s="46" t="s">
-        <v>261</v>
-      </c>
-      <c r="J20" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>CurrentEstablishDate</v>
-      </c>
-      <c r="K20" s="48">
-        <f>L20</f>
-        <v>44941</v>
-      </c>
-      <c r="L20" s="51">
-        <v>44941</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44948</v>
       </c>
       <c r="B21">
         <v>14.049139077238873</v>
       </c>
       <c r="C21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>202.84615958883612</v>
       </c>
       <c r="E21" s="1"/>
       <c r="G21">
         <v>3</v>
       </c>
-      <c r="H21" s="18" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" t="s">
+        <v>261</v>
+      </c>
+      <c r="J21" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>CurrentEstablishDate</v>
+      </c>
+      <c r="K21" s="39">
+        <f>L21</f>
+        <v>44941</v>
+      </c>
+      <c r="L21" s="44">
+        <v>44941</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A22" s="26">
+        <f t="shared" si="0"/>
+        <v>44949</v>
+      </c>
+      <c r="B22">
+        <v>13.012433227854736</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>215.85859281669084</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="H22" t="str">
+        <f t="shared" si="5"/>
+        <v>Current</v>
+      </c>
+      <c r="I22" t="s">
         <v>262</v>
       </c>
-      <c r="J21" s="47" t="str">
+      <c r="J22" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishStage</v>
       </c>
-      <c r="K21" s="19" t="str">
-        <f>IF(L21="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G21,FALSE),L21)</f>
+      <c r="K22" s="19" t="str">
+        <f>IF(L22="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G21,FALSE),L22)</f>
         <v>Seedling</v>
       </c>
-      <c r="L21" s="43" t="s">
+      <c r="L22" s="43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="26">
-        <f t="shared" si="1"/>
-        <v>44949</v>
-      </c>
-      <c r="B22">
-        <v>13.012433227854736</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>215.85859281669084</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="H22" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>Current</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="J22" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>CurrentHarvestDate</v>
-      </c>
-      <c r="K22" s="48">
-        <f>L22</f>
-        <v>44947</v>
-      </c>
-      <c r="L22" s="51">
-        <v>44947</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1">
       <c r="A23" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44950</v>
       </c>
       <c r="B23">
         <v>18.45901588220935</v>
       </c>
       <c r="C23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>234.31760869890019</v>
       </c>
       <c r="E23" s="1"/>
       <c r="G23">
         <v>5</v>
       </c>
-      <c r="H23" s="18" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I23" s="46" t="s">
+      <c r="I23" t="s">
+        <v>263</v>
+      </c>
+      <c r="J23" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>CurrentHarvestDate</v>
+      </c>
+      <c r="K23" s="39">
+        <f>L23</f>
+        <v>44947</v>
+      </c>
+      <c r="L23" s="44">
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="26">
+        <f t="shared" si="0"/>
+        <v>44951</v>
+      </c>
+      <c r="B24">
+        <v>11.995492344501493</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>246.31310104340167</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="H24" t="str">
+        <f t="shared" si="5"/>
+        <v>Current</v>
+      </c>
+      <c r="I24" t="s">
         <v>264</v>
       </c>
-      <c r="J23" s="47" t="str">
+      <c r="J24" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentHarvestStage</v>
       </c>
-      <c r="K23" s="19" t="str">
-        <f>IF(L23="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G23,FALSE),L23)</f>
+      <c r="K24" s="19" t="str">
+        <f>IF(L24="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G23,FALSE),L24)</f>
         <v>Vegetative</v>
       </c>
-      <c r="L23" s="43" t="s">
+      <c r="L24" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="26">
-        <f t="shared" si="1"/>
-        <v>44951</v>
-      </c>
-      <c r="B24">
-        <v>11.995492344501493</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="3"/>
-        <v>246.31310104340167</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="H24" s="18" t="str">
+    <row r="25" spans="1:12">
+      <c r="A25" s="26">
+        <f t="shared" si="0"/>
+        <v>44952</v>
+      </c>
+      <c r="B25">
+        <v>14.89124712931573</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>261.2043481727174</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="H25" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I25" t="s">
         <v>265</v>
       </c>
-      <c r="J24" s="47" t="str">
+      <c r="J25" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentResidueTreatment</v>
       </c>
-      <c r="K24" s="19" t="str">
-        <f>IF(L24="",P2,L24)</f>
+      <c r="K25" s="19" t="str">
+        <f>IF(L25="",P2,L25)</f>
         <v>Incorporated</v>
       </c>
-      <c r="L24" s="43" t="s">
+      <c r="L25" s="43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A25" s="26">
-        <f t="shared" si="1"/>
-        <v>44952</v>
-      </c>
-      <c r="B25">
-        <v>14.89124712931573</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="3"/>
-        <v>261.2043481727174</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="H25" s="23" t="str">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A26" s="26">
+        <f t="shared" si="0"/>
+        <v>44953</v>
+      </c>
+      <c r="B26">
+        <v>10.598117463308858</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>271.80246563602628</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="H26" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I25" s="49" t="s">
+      <c r="I26" t="s">
         <v>266</v>
       </c>
-      <c r="J25" s="50" t="str">
+      <c r="J26" s="23" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishN</v>
       </c>
-      <c r="K25" s="24">
-        <f>IF(L25="",0,L25)</f>
+      <c r="K26" s="24">
+        <f>IF(L26="",0,L26)</f>
         <v>10</v>
       </c>
-      <c r="L25" s="43">
+      <c r="L26" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="26">
-        <f t="shared" si="1"/>
-        <v>44953</v>
-      </c>
-      <c r="B26">
-        <v>10.598117463308858</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="3"/>
-        <v>271.80246563602628</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="H26" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="J26" s="30" t="str">
-        <f>H26&amp;I26</f>
-        <v>FollowingCropName</v>
-      </c>
-      <c r="K26" s="31" t="str">
-        <f>L26</f>
-        <v>Oat Grain General</v>
-      </c>
-      <c r="L26" s="42" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1">
       <c r="A27" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44954</v>
       </c>
       <c r="B27">
         <v>18.08459347173163</v>
       </c>
       <c r="C27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>289.88705910775792</v>
       </c>
       <c r="E27" s="1"/>
       <c r="G27">
         <v>7</v>
       </c>
-      <c r="H27" s="32" t="str">
-        <f>H26</f>
-        <v>Following</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="J27" s="34" t="str">
-        <f t="shared" ref="J27:J37" si="6">H27&amp;I27</f>
-        <v>FollowingSaleableYield</v>
-      </c>
-      <c r="K27" s="35">
-        <f>IF(L27="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G27,FALSE),L27)</f>
-        <v>5</v>
-      </c>
-      <c r="L27" s="43"/>
+      <c r="H27" t="s">
+        <v>274</v>
+      </c>
+      <c r="I27" t="s">
+        <v>270</v>
+      </c>
+      <c r="J27" s="29" t="str">
+        <f>H27&amp;I27</f>
+        <v>FollowingCropName</v>
+      </c>
+      <c r="K27" s="30" t="str">
+        <f>L27</f>
+        <v>Oat Grain General</v>
+      </c>
+      <c r="L27" s="45" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44955</v>
       </c>
       <c r="B28">
         <v>14.79161849090584</v>
       </c>
       <c r="C28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>304.67867759866374</v>
       </c>
       <c r="E28" s="1"/>
       <c r="G28">
         <v>8</v>
       </c>
-      <c r="H28" s="32" t="str">
-        <f t="shared" ref="H28:H37" si="7">H27</f>
+      <c r="H28" t="str">
+        <f>H27</f>
         <v>Following</v>
       </c>
-      <c r="I28" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="J28" s="34" t="str">
-        <f t="shared" si="6"/>
-        <v>FollowingUnits</v>
-      </c>
-      <c r="K28" s="35" t="str">
-        <f>IF(L28="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G28,FALSE),L28)</f>
-        <v>t/ha</v>
+      <c r="I28" t="s">
+        <v>256</v>
+      </c>
+      <c r="J28" s="31" t="str">
+        <f t="shared" ref="J28:J38" si="6">H28&amp;I28</f>
+        <v>FollowingSaleableYield</v>
+      </c>
+      <c r="K28" s="32">
+        <f>IF(L28="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G27,FALSE),L28)</f>
+        <v>5</v>
       </c>
       <c r="L28" s="43"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44956</v>
       </c>
       <c r="B29">
         <v>17.933505589637022</v>
       </c>
       <c r="C29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>322.61218318830078</v>
       </c>
       <c r="E29" s="1"/>
       <c r="G29">
         <v>12</v>
       </c>
-      <c r="H29" s="32" t="str">
-        <f t="shared" si="7"/>
+      <c r="H29" t="str">
+        <f t="shared" ref="H29:H38" si="7">H28</f>
         <v>Following</v>
       </c>
-      <c r="I29" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="J29" s="34" t="str">
+      <c r="I29" t="s">
+        <v>257</v>
+      </c>
+      <c r="J29" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>FollowingFieldLoss</v>
-      </c>
-      <c r="K29" s="35">
-        <f>IF(L29="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G29,FALSE),L29)</f>
-        <v>0</v>
+        <v>FollowingUnits</v>
+      </c>
+      <c r="K29" s="32" t="str">
+        <f>IF(L29="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G28,FALSE),L29)</f>
+        <v>t/ha</v>
       </c>
       <c r="L29" s="43"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44957</v>
       </c>
       <c r="B30">
         <v>16.082282662694066</v>
       </c>
       <c r="C30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>338.69446585099485</v>
       </c>
       <c r="E30" s="1"/>
       <c r="G30">
         <v>11</v>
       </c>
-      <c r="H30" s="32" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I30" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="J30" s="34" t="str">
+      <c r="I30" t="s">
+        <v>258</v>
+      </c>
+      <c r="J30" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>FollowingDressingLoss</v>
-      </c>
-      <c r="K30" s="35">
-        <f>IF(L30="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G30,FALSE),L30)</f>
+        <v>FollowingFieldLoss</v>
+      </c>
+      <c r="K30" s="32">
+        <f>IF(L30="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G29,FALSE),L30)</f>
         <v>0</v>
       </c>
       <c r="L30" s="43"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44958</v>
       </c>
       <c r="B31">
         <v>20.828587685127982</v>
       </c>
       <c r="C31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>359.5230535361228</v>
       </c>
       <c r="E31" s="1"/>
       <c r="G31">
         <v>15</v>
       </c>
-      <c r="H31" s="32" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" t="s">
+        <v>259</v>
+      </c>
+      <c r="J31" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>FollowingDressingLoss</v>
+      </c>
+      <c r="K31" s="32">
+        <f>IF(L31="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G30,FALSE),L31)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="43"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A32" s="26">
+        <f t="shared" si="0"/>
+        <v>44959</v>
+      </c>
+      <c r="B32">
+        <v>13.76912650928467</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>373.29218004540746</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="H32" t="str">
+        <f t="shared" si="7"/>
+        <v>Following</v>
+      </c>
+      <c r="I32" t="s">
         <v>260</v>
       </c>
-      <c r="J31" s="34" t="str">
+      <c r="J32" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingMoistureContent</v>
       </c>
-      <c r="K31" s="35">
-        <f>IF(L31="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G31,FALSE),L31)</f>
+      <c r="K32" s="32">
+        <f>IF(L32="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G31,FALSE),L32)</f>
         <v>80</v>
       </c>
-      <c r="L31" s="43"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="26">
-        <f t="shared" si="1"/>
-        <v>44959</v>
-      </c>
-      <c r="B32">
-        <v>13.76912650928467</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="3"/>
-        <v>373.29218004540746</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="H32" s="32" t="str">
-        <f t="shared" si="7"/>
-        <v>Following</v>
-      </c>
-      <c r="I32" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="J32" s="34" t="str">
-        <f t="shared" si="6"/>
-        <v>FollowingEstablishDate</v>
-      </c>
-      <c r="K32" s="36">
-        <f>L32</f>
-        <v>44951</v>
-      </c>
-      <c r="L32" s="51">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="L32" s="43"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1">
       <c r="A33" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44960</v>
       </c>
       <c r="B33">
         <v>23.549644512826927</v>
       </c>
       <c r="C33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>396.84182455823441</v>
       </c>
       <c r="E33" s="1"/>
       <c r="G33">
         <v>3</v>
       </c>
-      <c r="H33" s="32" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="I33" t="s">
+        <v>261</v>
+      </c>
+      <c r="J33" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>FollowingEstablishDate</v>
+      </c>
+      <c r="K33" s="33">
+        <f>L33</f>
+        <v>44951</v>
+      </c>
+      <c r="L33" s="44">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A34" s="26"/>
+      <c r="E34" s="1"/>
+      <c r="H34" t="str">
+        <f t="shared" si="7"/>
+        <v>Following</v>
+      </c>
+      <c r="I34" t="s">
         <v>262</v>
       </c>
-      <c r="J33" s="34" t="str">
+      <c r="J34" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishStage</v>
       </c>
-      <c r="K33" s="35" t="str">
-        <f>IF(L33="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G33,FALSE),L33)</f>
+      <c r="K34" s="32" t="str">
+        <f>IF(L34="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G33,FALSE),L34)</f>
         <v>Seed</v>
       </c>
-      <c r="L33" s="43"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="26"/>
-      <c r="E34" s="1"/>
-      <c r="H34" s="32" t="str">
-        <f t="shared" si="7"/>
-        <v>Following</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J34" s="34" t="str">
-        <f t="shared" si="6"/>
-        <v>FollowingHarvestDate</v>
-      </c>
-      <c r="K34" s="36">
-        <f>L34</f>
-        <v>44959</v>
-      </c>
-      <c r="L34" s="51">
-        <f>A32</f>
-        <v>44959</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="L34" s="43"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" thickBot="1">
       <c r="A35" s="26"/>
       <c r="E35" s="1"/>
       <c r="G35">
         <v>5</v>
       </c>
-      <c r="H35" s="32" t="str">
+      <c r="H35" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I35" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="J35" s="34" t="str">
+      <c r="I35" t="s">
+        <v>263</v>
+      </c>
+      <c r="J35" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>FollowingHarvestStage</v>
-      </c>
-      <c r="K35" s="35" t="str">
-        <f>IF(L35="",VLOOKUP(K$2,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G35,FALSE),L35)</f>
-        <v>EarlyReproductive</v>
-      </c>
-      <c r="L35" s="43"/>
+        <v>FollowingHarvestDate</v>
+      </c>
+      <c r="K35" s="33">
+        <f>L35</f>
+        <v>44959</v>
+      </c>
+      <c r="L35" s="44">
+        <f>A32</f>
+        <v>44959</v>
+      </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="26"/>
       <c r="E36" s="1"/>
-      <c r="H36" s="32" t="str">
+      <c r="H36" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I36" s="33" t="s">
+      <c r="I36" t="s">
+        <v>264</v>
+      </c>
+      <c r="J36" s="31" t="str">
+        <f t="shared" si="6"/>
+        <v>FollowingHarvestStage</v>
+      </c>
+      <c r="K36" s="32" t="str">
+        <f>IF(L36="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G35,FALSE),L36)</f>
+        <v>EarlyReproductive</v>
+      </c>
+      <c r="L36" s="43"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="26"/>
+      <c r="E37" s="1"/>
+      <c r="H37" t="str">
+        <f t="shared" si="7"/>
+        <v>Following</v>
+      </c>
+      <c r="I37" t="s">
         <v>265</v>
       </c>
-      <c r="J36" s="34" t="str">
+      <c r="J37" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingResidueTreatment</v>
       </c>
-      <c r="K36" s="35" t="str">
-        <f>IF(L36="",P2,L36)</f>
+      <c r="K37" s="32" t="str">
+        <f>IF(L37="",P2,L37)</f>
         <v>None</v>
       </c>
-      <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A37" s="26"/>
-      <c r="E37" s="1"/>
-      <c r="H37" s="37" t="str">
+      <c r="L37" s="43"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1">
+      <c r="E38" s="1"/>
+      <c r="H38" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I37" s="38" t="s">
+      <c r="I38" t="s">
         <v>266</v>
       </c>
-      <c r="J37" s="39" t="str">
+      <c r="J38" s="34" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishN</v>
       </c>
-      <c r="K37" s="40">
-        <f>IF(L37="",0,L37)</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="43"/>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="E38" s="1"/>
+      <c r="K38" s="35">
+        <f>IF(L38="",0,L38)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="43"/>
     </row>
     <row r="39" spans="1:12">
+      <c r="A39" t="e">
+        <f t="array" ref="A39">_xll.GetDailyNBalance(C2:C33,J2:K38)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="B39" s="27"/>
     </row>
     <row r="40" spans="1:12">
@@ -3870,19 +3918,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:L12 K24:L24 K36:L36" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:L13 K25:L25 K37:L37" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
       <formula1>$P$2:$P$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11 L23 L35" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12 L24 L36" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
       <formula1>$O$2:$O$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9 L21 L33" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10 L22 L34" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
       <formula1>$N$2:$N$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4 L16 L28" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5 L17 L29" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
       <formula1>$Q$2:$Q$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L7 L17:L19 L29:L31" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L8 L18:L20 L30:L32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>
@@ -3907,7 +3955,7 @@
           <x14:formula1>
             <xm:f>CropCoefficients!$K$3:$K$78</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:L2 K14:L14 K26:L26</xm:sqref>
+          <xm:sqref>K3:L3 K15:L15 K27:L27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Basic N balance working now
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACE8B6-7C59-494E-A3FD-F3236842350E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED30C2C5-A6B9-4444-A77A-5A548BEB4F21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
@@ -1115,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1182,6 +1182,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,6 +1201,674 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'NBalance Test'!$A$2:$A$61</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>44929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44930</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44931</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44932</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44934</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44936</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44937</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44939</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44940</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44941</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44942</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44943</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44944</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44946</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44947</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44948</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44951</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44952</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44953</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44954</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44955</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44956</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44957</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'NBalance Test'!$B$2:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15783182418578878</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7235440432093423E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20235506135482084</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.764623288907412E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2106526484524287</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23504877557079729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33901731439190108</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.20415816274163623</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3359956809311733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.78047365225292076</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5414316932853449</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.49411391691496576</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4824885863887793</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.70799810604867464</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.43617634163370145</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.90771934575078106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.30344580387295927</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.94494045740038679</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0543760030125071</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5207555114147002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A770-4A0D-A5B2-F59D0663F47B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2095045328"/>
+        <c:axId val="2095034512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2095045328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2095034512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2095034512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2095045328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1680,6 +2349,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2235,7 +2944,564 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A475EFCB-712A-426E-A400-681BD0272A4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2573,1369 +3839,1827 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1">
-      <c r="B1" t="s">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A1" t="str">
+        <f t="array" ref="A1:C61">_xll.GetDailyNBalance(G3:G34,L2:M38)</f>
+        <v>Date</v>
+      </c>
+      <c r="B1" s="28" t="str">
+        <v>RootN</v>
+      </c>
+      <c r="C1" t="str">
+        <v>UptakeN</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" t="s">
+        <v>277</v>
+      </c>
+      <c r="N1" t="s">
+        <v>276</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A2" s="28">
+        <v>44929</v>
+      </c>
+      <c r="B2" s="46">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="I1" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="L2" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="M2" s="41">
+        <f>IF(N2="",50,N2)</f>
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" t="s">
+        <v>253</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="28">
+        <v>44930</v>
+      </c>
+      <c r="B3" s="46">
+        <v>0.15783182418578878</v>
+      </c>
+      <c r="C3" s="46">
+        <v>0</v>
+      </c>
+      <c r="E3" s="26">
+        <f>M9</f>
+        <v>44929</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>272</v>
+      </c>
+      <c r="K3" t="s">
+        <v>270</v>
+      </c>
+      <c r="L3" s="29" t="str">
+        <f>J3&amp;K3</f>
+        <v>PriorCropName</v>
+      </c>
+      <c r="M3" s="30" t="str">
+        <f>N3</f>
+        <v>Annual ryegrass Fodder General</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="P3" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s">
+        <v>249</v>
+      </c>
+      <c r="S3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="28">
+        <v>44931</v>
+      </c>
+      <c r="B4" s="46">
+        <v>9.7235440432093423E-2</v>
+      </c>
+      <c r="C4" s="46">
+        <v>0</v>
+      </c>
+      <c r="E4" s="26">
+        <f>E3+1</f>
+        <v>44930</v>
+      </c>
+      <c r="F4">
+        <v>14.387874318606862</v>
+      </c>
+      <c r="G4">
+        <f>F4+F3</f>
+        <v>26.387874318606862</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4" t="str">
+        <f>J3</f>
+        <v>Prior</v>
+      </c>
+      <c r="K4" t="s">
+        <v>256</v>
+      </c>
+      <c r="L4" s="31" t="str">
+        <f t="shared" ref="L4:L14" si="0">J4&amp;K4</f>
+        <v>PriorSaleableYield</v>
+      </c>
+      <c r="M4" s="32">
+        <f>IF(N4="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I4,FALSE),N4)</f>
+        <v>5</v>
+      </c>
+      <c r="N4" s="43"/>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="28">
+        <v>44932</v>
+      </c>
+      <c r="B5" s="46">
+        <v>0.20235506135482084</v>
+      </c>
+      <c r="C5" s="46">
+        <v>0</v>
+      </c>
+      <c r="E5" s="26">
+        <f t="shared" ref="E5:E34" si="1">E4+1</f>
+        <v>44931</v>
+      </c>
+      <c r="F5">
+        <v>7.6885371447735746</v>
+      </c>
+      <c r="G5">
+        <f>F5+G4</f>
+        <v>34.076411463380438</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ref="J5:J14" si="2">J4</f>
+        <v>Prior</v>
+      </c>
+      <c r="K5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="26">
-        <f>K9</f>
+      <c r="L5" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorUnits</v>
+      </c>
+      <c r="M5" s="32" t="str">
+        <f>IF(N5="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I5,FALSE),N5)</f>
+        <v>t/ha</v>
+      </c>
+      <c r="N5" s="43"/>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="28">
+        <v>44933</v>
+      </c>
+      <c r="B6" s="46">
+        <v>6.764623288907412E-2</v>
+      </c>
+      <c r="C6" s="46">
+        <v>0</v>
+      </c>
+      <c r="E6" s="26">
+        <f t="shared" si="1"/>
+        <v>44932</v>
+      </c>
+      <c r="F6">
+        <v>13.912023293050638</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G34" si="3">F6+G5</f>
+        <v>47.988434756431076</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K6" t="s">
+        <v>258</v>
+      </c>
+      <c r="L6" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorFieldLoss</v>
+      </c>
+      <c r="M6" s="32">
+        <f>IF(N6="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I6,FALSE),N6)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="43"/>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="28">
+        <v>44934</v>
+      </c>
+      <c r="B7" s="46">
+        <v>0.2106526484524287</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26">
+        <f t="shared" si="1"/>
+        <v>44933</v>
+      </c>
+      <c r="F7">
+        <v>4.1491642970301701</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>52.137599053461244</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L7" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorDressingLoss</v>
+      </c>
+      <c r="M7" s="32">
+        <f>IF(N7="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I7,FALSE),N7)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="43"/>
+      <c r="Q7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A8" s="28">
+        <v>44935</v>
+      </c>
+      <c r="B8" s="46">
+        <v>0.23504877557079729</v>
+      </c>
+      <c r="C8" s="46">
+        <v>0</v>
+      </c>
+      <c r="E8" s="26">
+        <f t="shared" si="1"/>
+        <v>44934</v>
+      </c>
+      <c r="F8">
+        <v>11.680823993463974</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>63.818423046925219</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K8" t="s">
+        <v>260</v>
+      </c>
+      <c r="L8" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorMoistureContent</v>
+      </c>
+      <c r="M8" s="32">
+        <f>IF(N8="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I8,FALSE),N8)</f>
+        <v>80</v>
+      </c>
+      <c r="N8" s="43"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A9" s="28">
+        <v>44936</v>
+      </c>
+      <c r="B9" s="46">
+        <v>0.33901731439190108</v>
+      </c>
+      <c r="C9" s="46">
+        <v>0</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" si="1"/>
+        <v>44935</v>
+      </c>
+      <c r="F9">
+        <v>11.289351844181724</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>75.107774891106942</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K9" t="s">
+        <v>261</v>
+      </c>
+      <c r="L9" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorEstablishDate</v>
+      </c>
+      <c r="M9" s="33">
+        <f>N9</f>
         <v>44929</v>
       </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="J2" s="40" t="s">
-        <v>280</v>
-      </c>
-      <c r="K2" s="41">
-        <f>IF(L2="",50,L2)</f>
+      <c r="N9" s="44">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A10" s="28">
+        <v>44937</v>
+      </c>
+      <c r="B10" s="46">
+        <v>0.20415816274163623</v>
+      </c>
+      <c r="C10" s="46">
+        <v>0</v>
+      </c>
+      <c r="E10" s="26">
+        <f t="shared" si="1"/>
+        <v>44936</v>
+      </c>
+      <c r="F10">
+        <v>13.934890823546613</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>89.042665714653552</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K10" t="s">
+        <v>262</v>
+      </c>
+      <c r="L10" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorEstablishStage</v>
+      </c>
+      <c r="M10" s="32" t="str">
+        <f>IF(N10="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I10,FALSE),N10)</f>
+        <v>Seed</v>
+      </c>
+      <c r="N10" s="43"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A11" s="28">
+        <v>44938</v>
+      </c>
+      <c r="B11" s="46">
+        <v>0</v>
+      </c>
+      <c r="C11" s="46">
+        <v>0</v>
+      </c>
+      <c r="E11" s="26">
+        <f t="shared" si="1"/>
+        <v>44937</v>
+      </c>
+      <c r="F11">
+        <v>7.3816990790906738</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>96.424364793744232</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K11" t="s">
+        <v>263</v>
+      </c>
+      <c r="L11" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorHarvestDate</v>
+      </c>
+      <c r="M11" s="33">
+        <f>N11</f>
+        <v>44938</v>
+      </c>
+      <c r="N11" s="44">
+        <v>44938</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="28">
+        <v>44939</v>
+      </c>
+      <c r="B12" s="46">
+        <v>0</v>
+      </c>
+      <c r="C12" s="46">
+        <v>0</v>
+      </c>
+      <c r="E12" s="26">
+        <f t="shared" si="1"/>
+        <v>44938</v>
+      </c>
+      <c r="F12">
+        <v>13.932559604705048</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>110.35692439844928</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K12" t="s">
+        <v>264</v>
+      </c>
+      <c r="L12" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorHarvestStage</v>
+      </c>
+      <c r="M12" s="32" t="str">
+        <f>IF(N12="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I12,FALSE),N12)</f>
+        <v>EarlyReproductive</v>
+      </c>
+      <c r="N12" s="43"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="28">
+        <v>44940</v>
+      </c>
+      <c r="B13" s="46">
+        <v>0</v>
+      </c>
+      <c r="C13" s="46">
+        <v>0</v>
+      </c>
+      <c r="E13" s="26">
+        <f t="shared" si="1"/>
+        <v>44939</v>
+      </c>
+      <c r="F13">
+        <v>5.3540880739901002</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>115.71101247243938</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K13" t="s">
+        <v>265</v>
+      </c>
+      <c r="L13" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorResidueTreatment</v>
+      </c>
+      <c r="M13" s="32" t="str">
+        <f>IF(N13="",R2,N13)</f>
+        <v>None</v>
+      </c>
+      <c r="N13" s="43"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A14" s="28">
+        <v>44941</v>
+      </c>
+      <c r="B14" s="46">
+        <v>0</v>
+      </c>
+      <c r="C14" s="46">
+        <v>0</v>
+      </c>
+      <c r="E14" s="26">
+        <f t="shared" si="1"/>
+        <v>44940</v>
+      </c>
+      <c r="F14">
+        <v>13.363497784448709</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>129.07451025688809</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="2"/>
+        <v>Prior</v>
+      </c>
+      <c r="K14" t="s">
+        <v>266</v>
+      </c>
+      <c r="L14" s="34" t="str">
+        <f t="shared" si="0"/>
+        <v>PriorEstablishN</v>
+      </c>
+      <c r="M14" s="35">
+        <f>IF(N14="",0,N14)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="43"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A15" s="28">
+        <v>44942</v>
+      </c>
+      <c r="B15" s="46">
+        <v>1.3359956809311733</v>
+      </c>
+      <c r="C15" s="46">
+        <v>0</v>
+      </c>
+      <c r="E15" s="26">
+        <f t="shared" si="1"/>
+        <v>44941</v>
+      </c>
+      <c r="F15">
+        <v>6.6646938971593457</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>135.73920415404743</v>
+      </c>
+      <c r="J15" t="s">
+        <v>273</v>
+      </c>
+      <c r="K15" t="s">
+        <v>270</v>
+      </c>
+      <c r="L15" s="37" t="str">
+        <f>J15&amp;K15</f>
+        <v>CurrentCropName</v>
+      </c>
+      <c r="M15" s="38" t="str">
+        <f>N15</f>
+        <v>Potato Vegetable General</v>
+      </c>
+      <c r="N15" s="45" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="28">
+        <v>44943</v>
+      </c>
+      <c r="B16" s="46">
+        <v>0.78047365225292076</v>
+      </c>
+      <c r="C16" s="46">
+        <v>0</v>
+      </c>
+      <c r="E16" s="26">
+        <f t="shared" si="1"/>
+        <v>44942</v>
+      </c>
+      <c r="F16">
+        <v>15.119829112109056</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>150.85903326615647</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16" t="str">
+        <f>J15</f>
+        <v>Current</v>
+      </c>
+      <c r="K16" t="s">
+        <v>256</v>
+      </c>
+      <c r="L16" s="18" t="str">
+        <f t="shared" ref="L16:L26" si="4">J16&amp;K16</f>
+        <v>CurrentSaleableYield</v>
+      </c>
+      <c r="M16" s="19">
+        <f>IF(N16="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I16,FALSE),N16)</f>
         <v>50</v>
       </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A3" s="26">
-        <f>A2+1</f>
-        <v>44930</v>
-      </c>
-      <c r="B3">
-        <v>14.387874318606862</v>
-      </c>
-      <c r="C3">
-        <f>B3+B2</f>
-        <v>26.387874318606862</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>272</v>
-      </c>
-      <c r="I3" t="s">
-        <v>270</v>
-      </c>
-      <c r="J3" s="29" t="str">
-        <f>H3&amp;I3</f>
-        <v>PriorCropName</v>
-      </c>
-      <c r="K3" s="30" t="str">
-        <f>L3</f>
-        <v>Annual ryegrass Fodder General</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="N3" t="s">
-        <v>123</v>
-      </c>
-      <c r="O3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="26">
-        <f t="shared" ref="A4:A33" si="0">A3+1</f>
-        <v>44931</v>
-      </c>
-      <c r="B4">
-        <v>7.6885371447735746</v>
-      </c>
-      <c r="C4">
-        <f>B4+C3</f>
-        <v>34.076411463380438</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="G4">
+      <c r="N16" s="43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="28">
+        <v>44944</v>
+      </c>
+      <c r="B17" s="46">
+        <v>1.5414316932853449</v>
+      </c>
+      <c r="C17" s="46">
+        <v>0</v>
+      </c>
+      <c r="E17" s="26">
+        <f t="shared" si="1"/>
+        <v>44943</v>
+      </c>
+      <c r="F17">
+        <v>10.605844567907475</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>161.46487783406394</v>
+      </c>
+      <c r="I17">
         <v>8</v>
       </c>
-      <c r="H4" t="str">
-        <f>H3</f>
-        <v>Prior</v>
-      </c>
-      <c r="I4" t="s">
-        <v>256</v>
-      </c>
-      <c r="J4" s="31" t="str">
-        <f t="shared" ref="J4:J14" si="1">H4&amp;I4</f>
-        <v>PriorSaleableYield</v>
-      </c>
-      <c r="K4" s="32">
-        <f>IF(L4="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G3,FALSE),L4)</f>
-        <v>5</v>
-      </c>
-      <c r="L4" s="43"/>
-      <c r="O4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="26">
-        <f t="shared" si="0"/>
-        <v>44932</v>
-      </c>
-      <c r="B5">
-        <v>13.912023293050638</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C33" si="2">B5+C4</f>
-        <v>47.988434756431076</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ref="H5:H14" si="3">H4</f>
-        <v>Prior</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J17" t="str">
+        <f t="shared" ref="J17:J26" si="5">J16</f>
+        <v>Current</v>
+      </c>
+      <c r="K17" t="s">
         <v>257</v>
       </c>
-      <c r="J5" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorUnits</v>
-      </c>
-      <c r="K5" s="32" t="str">
-        <f>IF(L5="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G4,FALSE),L5)</f>
-        <v>t/ha</v>
-      </c>
-      <c r="L5" s="43"/>
-      <c r="O5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="26">
-        <f t="shared" si="0"/>
-        <v>44933</v>
-      </c>
-      <c r="B6">
-        <v>4.1491642970301701</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="2"/>
-        <v>52.137599053461244</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="G6">
-        <v>11</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I6" t="s">
-        <v>258</v>
-      </c>
-      <c r="J6" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorFieldLoss</v>
-      </c>
-      <c r="K6" s="32">
-        <f>IF(L6="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G5,FALSE),L6)</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="43"/>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="26">
-        <f t="shared" si="0"/>
-        <v>44934</v>
-      </c>
-      <c r="B7">
-        <v>11.680823993463974</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="2"/>
-        <v>63.818423046925219</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I7" t="s">
-        <v>259</v>
-      </c>
-      <c r="J7" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorDressingLoss</v>
-      </c>
-      <c r="K7" s="32">
-        <f>IF(L7="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G6,FALSE),L7)</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="43"/>
-      <c r="O7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A8" s="26">
-        <f t="shared" si="0"/>
-        <v>44935</v>
-      </c>
-      <c r="B8">
-        <v>11.289351844181724</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="2"/>
-        <v>75.107774891106942</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="H8" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I8" t="s">
-        <v>260</v>
-      </c>
-      <c r="J8" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorMoistureContent</v>
-      </c>
-      <c r="K8" s="32">
-        <f>IF(L8="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G7,FALSE),L8)</f>
-        <v>80</v>
-      </c>
-      <c r="L8" s="43"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A9" s="26">
-        <f t="shared" si="0"/>
-        <v>44936</v>
-      </c>
-      <c r="B9">
-        <v>13.934890823546613</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="2"/>
-        <v>89.042665714653552</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I9" t="s">
-        <v>261</v>
-      </c>
-      <c r="J9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorEstablishDate</v>
-      </c>
-      <c r="K9" s="33">
-        <f>L9</f>
-        <v>44929</v>
-      </c>
-      <c r="L9" s="44">
-        <v>44929</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A10" s="26">
-        <f t="shared" si="0"/>
-        <v>44937</v>
-      </c>
-      <c r="B10">
-        <v>7.3816990790906738</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="2"/>
-        <v>96.424364793744232</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="H10" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I10" t="s">
-        <v>262</v>
-      </c>
-      <c r="J10" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorEstablishStage</v>
-      </c>
-      <c r="K10" s="32" t="str">
-        <f>IF(L10="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G9,FALSE),L10)</f>
-        <v>Seed</v>
-      </c>
-      <c r="L10" s="43"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A11" s="26">
-        <f t="shared" si="0"/>
-        <v>44938</v>
-      </c>
-      <c r="B11">
-        <v>13.932559604705048</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="2"/>
-        <v>110.35692439844928</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I11" t="s">
-        <v>263</v>
-      </c>
-      <c r="J11" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorHarvestDate</v>
-      </c>
-      <c r="K11" s="33">
-        <f>L11</f>
-        <v>44938</v>
-      </c>
-      <c r="L11" s="44">
-        <v>44938</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="26">
-        <f t="shared" si="0"/>
-        <v>44939</v>
-      </c>
-      <c r="B12">
-        <v>5.3540880739901002</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
-        <v>115.71101247243938</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="H12" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I12" t="s">
-        <v>264</v>
-      </c>
-      <c r="J12" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorHarvestStage</v>
-      </c>
-      <c r="K12" s="32" t="str">
-        <f>IF(L12="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G11,FALSE),L12)</f>
-        <v>EarlyReproductive</v>
-      </c>
-      <c r="L12" s="43"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="26">
-        <f t="shared" si="0"/>
-        <v>44940</v>
-      </c>
-      <c r="B13">
-        <v>13.363497784448709</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
-        <v>129.07451025688809</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="H13" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I13" t="s">
-        <v>265</v>
-      </c>
-      <c r="J13" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorResidueTreatment</v>
-      </c>
-      <c r="K13" s="32" t="str">
-        <f>IF(L13="",P2,L13)</f>
-        <v>None</v>
-      </c>
-      <c r="L13" s="43"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="26">
-        <f t="shared" si="0"/>
-        <v>44941</v>
-      </c>
-      <c r="B14">
-        <v>6.6646938971593457</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
-        <v>135.73920415404743</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="H14" t="str">
-        <f t="shared" si="3"/>
-        <v>Prior</v>
-      </c>
-      <c r="I14" t="s">
-        <v>266</v>
-      </c>
-      <c r="J14" s="34" t="str">
-        <f t="shared" si="1"/>
-        <v>PriorEstablishN</v>
-      </c>
-      <c r="K14" s="35">
-        <f>IF(L14="",0,L14)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="43"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A15" s="26">
-        <f t="shared" si="0"/>
-        <v>44942</v>
-      </c>
-      <c r="B15">
-        <v>15.119829112109056</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>150.85903326615647</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="G15">
-        <v>7</v>
-      </c>
-      <c r="H15" t="s">
-        <v>273</v>
-      </c>
-      <c r="I15" t="s">
-        <v>270</v>
-      </c>
-      <c r="J15" s="37" t="str">
-        <f>H15&amp;I15</f>
-        <v>CurrentCropName</v>
-      </c>
-      <c r="K15" s="38" t="str">
-        <f>L15</f>
-        <v>Potato Vegetable General</v>
-      </c>
-      <c r="L15" s="45" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="26">
-        <f t="shared" si="0"/>
-        <v>44943</v>
-      </c>
-      <c r="B16">
-        <v>10.605844567907475</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="2"/>
-        <v>161.46487783406394</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16">
-        <v>8</v>
-      </c>
-      <c r="H16" t="str">
-        <f>H15</f>
-        <v>Current</v>
-      </c>
-      <c r="I16" t="s">
-        <v>256</v>
-      </c>
-      <c r="J16" s="18" t="str">
-        <f t="shared" ref="J16:J26" si="4">H16&amp;I16</f>
-        <v>CurrentSaleableYield</v>
-      </c>
-      <c r="K16" s="19">
-        <f>IF(L16="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G15,FALSE),L16)</f>
-        <v>10</v>
-      </c>
-      <c r="L16" s="43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="26">
-        <f t="shared" si="0"/>
-        <v>44944</v>
-      </c>
-      <c r="B17">
-        <v>11.901756295522578</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>173.36663412958652</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17">
-        <v>12</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" ref="H17:H26" si="5">H16</f>
-        <v>Current</v>
-      </c>
-      <c r="I17" t="s">
-        <v>257</v>
-      </c>
-      <c r="J17" s="18" t="str">
+      <c r="L17" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentUnits</v>
       </c>
-      <c r="K17" s="19" t="str">
-        <f>IF(L17="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G16,FALSE),L17)</f>
-        <v>kg/ha</v>
-      </c>
-      <c r="L17" s="43" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="26">
-        <f t="shared" si="0"/>
+      <c r="M17" s="19" t="str">
+        <f>IF(N17="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I17,FALSE),N17)</f>
+        <v>t/ha</v>
+      </c>
+      <c r="N17" s="43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="28">
         <v>44945</v>
       </c>
-      <c r="B18">
-        <v>3.8939814164824327</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="2"/>
-        <v>177.26061554606895</v>
-      </c>
-      <c r="E18" s="1"/>
+      <c r="B18" s="46">
+        <v>0.49411391691496576</v>
+      </c>
+      <c r="C18" s="46">
+        <v>0</v>
+      </c>
+      <c r="E18" s="26">
+        <f t="shared" si="1"/>
+        <v>44944</v>
+      </c>
+      <c r="F18">
+        <v>11.901756295522578</v>
+      </c>
       <c r="G18">
-        <v>11</v>
-      </c>
-      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>173.36663412958652</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>258</v>
       </c>
-      <c r="J18" s="18" t="str">
+      <c r="L18" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentFieldLoss</v>
       </c>
-      <c r="K18" s="19">
-        <f>IF(L18="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G17,FALSE),L18)</f>
-        <v>15</v>
-      </c>
-      <c r="L18" s="43">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="26">
-        <f t="shared" si="0"/>
+      <c r="M18" s="19">
+        <f>IF(N18="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I18,FALSE),N18)</f>
+        <v>5</v>
+      </c>
+      <c r="N18" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="28">
         <v>44946</v>
       </c>
-      <c r="B19">
-        <v>6.2562047514789443</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>183.51682029754789</v>
-      </c>
-      <c r="E19" s="1"/>
+      <c r="B19" s="46">
+        <v>1.4824885863887793</v>
+      </c>
+      <c r="C19" s="46">
+        <v>0</v>
+      </c>
+      <c r="E19" s="26">
+        <f t="shared" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="F19">
+        <v>3.8939814164824327</v>
+      </c>
       <c r="G19">
-        <v>15</v>
-      </c>
-      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>177.26061554606895</v>
+      </c>
+      <c r="I19">
+        <v>11</v>
+      </c>
+      <c r="J19" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>259</v>
       </c>
-      <c r="J19" s="18" t="str">
+      <c r="L19" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentDressingLoss</v>
       </c>
-      <c r="K19" s="19">
-        <f>IF(L19="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G18,FALSE),L19)</f>
-        <v>10</v>
-      </c>
-      <c r="L19" s="43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A20" s="26">
-        <f t="shared" si="0"/>
+      <c r="M19" s="19">
+        <f>IF(N19="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I19,FALSE),N19)</f>
+        <v>5</v>
+      </c>
+      <c r="N19" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A20" s="28">
         <v>44947</v>
       </c>
-      <c r="B20">
-        <v>5.2802002140493496</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>188.79702051159725</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="H20" t="str">
+      <c r="B20" s="46">
+        <v>0</v>
+      </c>
+      <c r="C20" s="46">
+        <v>0</v>
+      </c>
+      <c r="E20" s="26">
+        <f t="shared" si="1"/>
+        <v>44946</v>
+      </c>
+      <c r="F20">
+        <v>6.2562047514789443</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>183.51682029754789</v>
+      </c>
+      <c r="I20">
+        <v>15</v>
+      </c>
+      <c r="J20" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>260</v>
       </c>
-      <c r="J20" s="18" t="str">
+      <c r="L20" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentMoistureContent</v>
       </c>
-      <c r="K20" s="19">
-        <f>IF(L20="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G19,FALSE),L20)</f>
-        <v>72</v>
-      </c>
-      <c r="L20" s="43">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A21" s="26">
-        <f t="shared" si="0"/>
+      <c r="M20" s="19">
+        <f>IF(N20="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I20,FALSE),N20)</f>
+        <v>77.7</v>
+      </c>
+      <c r="N20" s="43"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A21" s="28">
         <v>44948</v>
       </c>
-      <c r="B21">
-        <v>14.049139077238873</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>202.84615958883612</v>
-      </c>
-      <c r="E21" s="1"/>
+      <c r="B21" s="46">
+        <v>0</v>
+      </c>
+      <c r="C21" s="46">
+        <v>0</v>
+      </c>
+      <c r="E21" s="26">
+        <f t="shared" si="1"/>
+        <v>44947</v>
+      </c>
+      <c r="F21">
+        <v>5.2802002140493496</v>
+      </c>
       <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>188.79702051159725</v>
+      </c>
+      <c r="J21" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>261</v>
       </c>
-      <c r="J21" s="18" t="str">
+      <c r="L21" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishDate</v>
       </c>
-      <c r="K21" s="39">
-        <f>L21</f>
+      <c r="M21" s="39">
+        <f>N21</f>
         <v>44941</v>
       </c>
-      <c r="L21" s="44">
+      <c r="N21" s="44">
         <v>44941</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A22" s="26">
-        <f t="shared" si="0"/>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A22" s="28">
         <v>44949</v>
       </c>
-      <c r="B22">
-        <v>13.012433227854736</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
-        <v>215.85859281669084</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="H22" t="str">
+      <c r="B22" s="46">
+        <v>0</v>
+      </c>
+      <c r="C22" s="46">
+        <v>0</v>
+      </c>
+      <c r="E22" s="26">
+        <f t="shared" si="1"/>
+        <v>44948</v>
+      </c>
+      <c r="F22">
+        <v>14.049139077238873</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>202.84615958883612</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>262</v>
       </c>
-      <c r="J22" s="18" t="str">
+      <c r="L22" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishStage</v>
       </c>
-      <c r="K22" s="19" t="str">
-        <f>IF(L22="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G21,FALSE),L22)</f>
+      <c r="M22" s="19" t="str">
+        <f>IF(N22="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I22,FALSE),N22)</f>
         <v>Seedling</v>
       </c>
-      <c r="L22" s="43" t="s">
+      <c r="N22" s="43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A23" s="26">
-        <f t="shared" si="0"/>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A23" s="28">
         <v>44950</v>
       </c>
-      <c r="B23">
-        <v>18.45901588220935</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>234.31760869890019</v>
-      </c>
-      <c r="E23" s="1"/>
+      <c r="B23" s="46">
+        <v>0</v>
+      </c>
+      <c r="C23" s="46">
+        <v>0</v>
+      </c>
+      <c r="E23" s="26">
+        <f t="shared" si="1"/>
+        <v>44949</v>
+      </c>
+      <c r="F23">
+        <v>13.012433227854736</v>
+      </c>
       <c r="G23">
-        <v>5</v>
-      </c>
-      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>215.85859281669084</v>
+      </c>
+      <c r="J23" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>263</v>
       </c>
-      <c r="J23" s="18" t="str">
+      <c r="L23" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentHarvestDate</v>
       </c>
-      <c r="K23" s="39">
-        <f>L23</f>
+      <c r="M23" s="39">
+        <f>N23</f>
         <v>44947</v>
       </c>
-      <c r="L23" s="44">
+      <c r="N23" s="44">
         <v>44947</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="26">
-        <f t="shared" si="0"/>
+    <row r="24" spans="1:14">
+      <c r="A24" s="28">
         <v>44951</v>
       </c>
-      <c r="B24">
-        <v>11.995492344501493</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="2"/>
-        <v>246.31310104340167</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="H24" t="str">
+      <c r="B24" s="46">
+        <v>0</v>
+      </c>
+      <c r="C24" s="46">
+        <v>0</v>
+      </c>
+      <c r="E24" s="26">
+        <f t="shared" si="1"/>
+        <v>44950</v>
+      </c>
+      <c r="F24">
+        <v>18.45901588220935</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>234.31760869890019</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>264</v>
       </c>
-      <c r="J24" s="18" t="str">
+      <c r="L24" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentHarvestStage</v>
       </c>
-      <c r="K24" s="19" t="str">
-        <f>IF(L24="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G23,FALSE),L24)</f>
+      <c r="M24" s="19" t="str">
+        <f>IF(N24="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I24,FALSE),N24)</f>
         <v>Vegetative</v>
       </c>
-      <c r="L24" s="43" t="s">
+      <c r="N24" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="26">
-        <f t="shared" si="0"/>
+    <row r="25" spans="1:14">
+      <c r="A25" s="28">
         <v>44952</v>
       </c>
-      <c r="B25">
-        <v>14.89124712931573</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="2"/>
-        <v>261.2043481727174</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="H25" t="str">
+      <c r="B25" s="46">
+        <v>0.70799810604867464</v>
+      </c>
+      <c r="C25" s="46">
+        <v>0</v>
+      </c>
+      <c r="E25" s="26">
+        <f t="shared" si="1"/>
+        <v>44951</v>
+      </c>
+      <c r="F25">
+        <v>11.995492344501493</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>246.31310104340167</v>
+      </c>
+      <c r="J25" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>265</v>
       </c>
-      <c r="J25" s="18" t="str">
+      <c r="L25" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentResidueTreatment</v>
       </c>
-      <c r="K25" s="19" t="str">
-        <f>IF(L25="",P2,L25)</f>
+      <c r="M25" s="19" t="str">
+        <f>IF(N25="",R2,N25)</f>
         <v>Incorporated</v>
       </c>
-      <c r="L25" s="43" t="s">
+      <c r="N25" s="43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="26">
-        <f t="shared" si="0"/>
+    <row r="26" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A26" s="28">
         <v>44953</v>
       </c>
-      <c r="B26">
-        <v>10.598117463308858</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="2"/>
-        <v>271.80246563602628</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="H26" t="str">
+      <c r="B26" s="46">
+        <v>0.43617634163370145</v>
+      </c>
+      <c r="C26" s="46">
+        <v>0</v>
+      </c>
+      <c r="E26" s="26">
+        <f t="shared" si="1"/>
+        <v>44952</v>
+      </c>
+      <c r="F26">
+        <v>14.89124712931573</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>261.2043481727174</v>
+      </c>
+      <c r="J26" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>266</v>
       </c>
-      <c r="J26" s="23" t="str">
+      <c r="L26" s="23" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishN</v>
       </c>
-      <c r="K26" s="24">
-        <f>IF(L26="",0,L26)</f>
+      <c r="M26" s="24">
+        <f>IF(N26="",0,N26)</f>
         <v>10</v>
       </c>
-      <c r="L26" s="43">
+      <c r="N26" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A27" s="26">
-        <f t="shared" si="0"/>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A27" s="28">
         <v>44954</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="46">
+        <v>0.90771934575078106</v>
+      </c>
+      <c r="C27" s="46">
+        <v>0</v>
+      </c>
+      <c r="E27" s="26">
+        <f t="shared" si="1"/>
+        <v>44953</v>
+      </c>
+      <c r="F27">
+        <v>10.598117463308858</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>271.80246563602628</v>
+      </c>
+      <c r="J27" t="s">
+        <v>274</v>
+      </c>
+      <c r="K27" t="s">
+        <v>270</v>
+      </c>
+      <c r="L27" s="29" t="str">
+        <f>J27&amp;K27</f>
+        <v>FollowingCropName</v>
+      </c>
+      <c r="M27" s="30" t="str">
+        <f>N27</f>
+        <v>Oat Grain General</v>
+      </c>
+      <c r="N27" s="45" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="28">
+        <v>44955</v>
+      </c>
+      <c r="B28" s="46">
+        <v>0.30344580387295927</v>
+      </c>
+      <c r="C28" s="46">
+        <v>0</v>
+      </c>
+      <c r="E28" s="26">
+        <f t="shared" si="1"/>
+        <v>44954</v>
+      </c>
+      <c r="F28">
         <v>18.08459347173163</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="2"/>
+      <c r="G28">
+        <f t="shared" si="3"/>
         <v>289.88705910775792</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="G27">
+      <c r="I28">
         <v>7</v>
       </c>
-      <c r="H27" t="s">
-        <v>274</v>
-      </c>
-      <c r="I27" t="s">
-        <v>270</v>
-      </c>
-      <c r="J27" s="29" t="str">
-        <f>H27&amp;I27</f>
-        <v>FollowingCropName</v>
-      </c>
-      <c r="K27" s="30" t="str">
-        <f>L27</f>
-        <v>Oat Grain General</v>
-      </c>
-      <c r="L27" s="45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="26">
-        <f t="shared" si="0"/>
+      <c r="J28" t="str">
+        <f>J27</f>
+        <v>Following</v>
+      </c>
+      <c r="K28" t="s">
+        <v>256</v>
+      </c>
+      <c r="L28" s="31" t="str">
+        <f t="shared" ref="L28:L38" si="6">J28&amp;K28</f>
+        <v>FollowingSaleableYield</v>
+      </c>
+      <c r="M28" s="32">
+        <f>IF(N28="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I28,FALSE),N28)</f>
+        <v>6</v>
+      </c>
+      <c r="N28" s="43"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="28">
+        <v>44956</v>
+      </c>
+      <c r="B29" s="46">
+        <v>0.94494045740038679</v>
+      </c>
+      <c r="C29" s="46">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26">
+        <f t="shared" si="1"/>
         <v>44955</v>
       </c>
-      <c r="B28">
+      <c r="F29">
         <v>14.79161849090584</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="2"/>
+      <c r="G29">
+        <f t="shared" si="3"/>
         <v>304.67867759866374</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="G28">
+      <c r="I29">
         <v>8</v>
       </c>
-      <c r="H28" t="str">
-        <f>H27</f>
+      <c r="J29" t="str">
+        <f t="shared" ref="J29:J38" si="7">J28</f>
         <v>Following</v>
       </c>
-      <c r="I28" t="s">
-        <v>256</v>
-      </c>
-      <c r="J28" s="31" t="str">
-        <f t="shared" ref="J28:J38" si="6">H28&amp;I28</f>
-        <v>FollowingSaleableYield</v>
-      </c>
-      <c r="K28" s="32">
-        <f>IF(L28="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G27,FALSE),L28)</f>
-        <v>5</v>
-      </c>
-      <c r="L28" s="43"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="26">
-        <f t="shared" si="0"/>
-        <v>44956</v>
-      </c>
-      <c r="B29">
-        <v>17.933505589637022</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="2"/>
-        <v>322.61218318830078</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="G29">
-        <v>12</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" ref="H29:H38" si="7">H28</f>
-        <v>Following</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>257</v>
       </c>
-      <c r="J29" s="31" t="str">
+      <c r="L29" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingUnits</v>
       </c>
-      <c r="K29" s="32" t="str">
-        <f>IF(L29="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G28,FALSE),L29)</f>
+      <c r="M29" s="32" t="str">
+        <f>IF(N29="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I29,FALSE),N29)</f>
         <v>t/ha</v>
       </c>
-      <c r="L29" s="43"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="26">
-        <f t="shared" si="0"/>
+      <c r="N29" s="43"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="28">
         <v>44957</v>
       </c>
-      <c r="B30">
-        <v>16.082282662694066</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="2"/>
-        <v>338.69446585099485</v>
-      </c>
-      <c r="E30" s="1"/>
+      <c r="B30" s="46">
+        <v>1.0543760030125071</v>
+      </c>
+      <c r="C30" s="46">
+        <v>0</v>
+      </c>
+      <c r="E30" s="26">
+        <f t="shared" si="1"/>
+        <v>44956</v>
+      </c>
+      <c r="F30">
+        <v>17.933505589637022</v>
+      </c>
       <c r="G30">
-        <v>11</v>
-      </c>
-      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>322.61218318830078</v>
+      </c>
+      <c r="I30">
+        <v>12</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>258</v>
       </c>
-      <c r="J30" s="31" t="str">
+      <c r="L30" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingFieldLoss</v>
       </c>
-      <c r="K30" s="32">
-        <f>IF(L30="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G29,FALSE),L30)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="43"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="26">
-        <f t="shared" si="0"/>
+      <c r="M30" s="32">
+        <f>IF(N30="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I30,FALSE),N30)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="43"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="28">
         <v>44958</v>
       </c>
-      <c r="B31">
-        <v>20.828587685127982</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="2"/>
-        <v>359.5230535361228</v>
-      </c>
-      <c r="E31" s="1"/>
+      <c r="B31" s="46">
+        <v>1.5207555114147002</v>
+      </c>
+      <c r="C31" s="46">
+        <v>0</v>
+      </c>
+      <c r="E31" s="26">
+        <f t="shared" si="1"/>
+        <v>44957</v>
+      </c>
+      <c r="F31">
+        <v>16.082282662694066</v>
+      </c>
       <c r="G31">
-        <v>15</v>
-      </c>
-      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>338.69446585099485</v>
+      </c>
+      <c r="I31">
+        <v>11</v>
+      </c>
+      <c r="J31" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>259</v>
       </c>
-      <c r="J31" s="31" t="str">
+      <c r="L31" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingDressingLoss</v>
       </c>
-      <c r="K31" s="32">
-        <f>IF(L31="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G30,FALSE),L31)</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="43"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A32" s="26">
-        <f t="shared" si="0"/>
-        <v>44959</v>
-      </c>
-      <c r="B32">
-        <v>13.76912650928467</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="2"/>
-        <v>373.29218004540746</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="H32" t="str">
+      <c r="M31" s="32">
+        <f>IF(N31="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I31,FALSE),N31)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="43"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A32" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E32" s="26">
+        <f t="shared" si="1"/>
+        <v>44958</v>
+      </c>
+      <c r="F32">
+        <v>20.828587685127982</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>359.5230535361228</v>
+      </c>
+      <c r="I32">
+        <v>15</v>
+      </c>
+      <c r="J32" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>260</v>
       </c>
-      <c r="J32" s="31" t="str">
+      <c r="L32" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingMoistureContent</v>
       </c>
-      <c r="K32" s="32">
-        <f>IF(L32="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G31,FALSE),L32)</f>
-        <v>80</v>
-      </c>
-      <c r="L32" s="43"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="26">
-        <f t="shared" si="0"/>
-        <v>44960</v>
-      </c>
-      <c r="B33">
-        <v>23.549644512826927</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="2"/>
-        <v>396.84182455823441</v>
-      </c>
-      <c r="E33" s="1"/>
+      <c r="M32" s="32">
+        <f>IF(N32="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I32,FALSE),N32)</f>
+        <v>13</v>
+      </c>
+      <c r="N32" s="43"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A33" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B33" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C33" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E33" s="26">
+        <f t="shared" si="1"/>
+        <v>44959</v>
+      </c>
+      <c r="F33">
+        <v>13.76912650928467</v>
+      </c>
       <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>373.29218004540746</v>
+      </c>
+      <c r="J33" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>261</v>
       </c>
-      <c r="J33" s="31" t="str">
+      <c r="L33" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishDate</v>
       </c>
-      <c r="K33" s="33">
-        <f>L33</f>
+      <c r="M33" s="33">
+        <f>N33</f>
         <v>44951</v>
       </c>
-      <c r="L33" s="44">
+      <c r="N33" s="44">
         <v>44951</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A34" s="26"/>
-      <c r="E34" s="1"/>
-      <c r="H34" t="str">
+    <row r="34" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A34" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B34" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C34" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" si="1"/>
+        <v>44960</v>
+      </c>
+      <c r="F34">
+        <v>23.549644512826927</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>396.84182455823441</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>262</v>
       </c>
-      <c r="J34" s="31" t="str">
+      <c r="L34" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishStage</v>
       </c>
-      <c r="K34" s="32" t="str">
-        <f>IF(L34="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G33,FALSE),L34)</f>
+      <c r="M34" s="32" t="str">
+        <f>IF(N34="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I34,FALSE),N34)</f>
         <v>Seed</v>
       </c>
-      <c r="L34" s="43"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A35" s="26"/>
-      <c r="E35" s="1"/>
-      <c r="G35">
-        <v>5</v>
-      </c>
-      <c r="H35" t="str">
+      <c r="N34" s="43"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A35" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B35" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C35" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="J35" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>263</v>
       </c>
-      <c r="J35" s="31" t="str">
+      <c r="L35" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingHarvestDate</v>
       </c>
-      <c r="K35" s="33">
-        <f>L35</f>
+      <c r="M35" s="33">
+        <f>N35</f>
         <v>44959</v>
       </c>
-      <c r="L35" s="44">
-        <f>A32</f>
+      <c r="N35" s="44">
+        <f>E33</f>
         <v>44959</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="26"/>
-      <c r="E36" s="1"/>
-      <c r="H36" t="str">
+    <row r="36" spans="1:14">
+      <c r="A36" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B36" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C36" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="I36">
+        <v>5</v>
+      </c>
+      <c r="J36" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>264</v>
       </c>
-      <c r="J36" s="31" t="str">
+      <c r="L36" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingHarvestStage</v>
       </c>
-      <c r="K36" s="32" t="str">
-        <f>IF(L36="",VLOOKUP(K$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$G35,FALSE),L36)</f>
+      <c r="M36" s="32" t="str">
+        <f>IF(N36="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I36,FALSE),N36)</f>
         <v>EarlyReproductive</v>
       </c>
-      <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="26"/>
-      <c r="E37" s="1"/>
-      <c r="H37" t="str">
+      <c r="N36" s="43"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B37" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C37" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="J37" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I37" t="s">
+      <c r="K37" t="s">
         <v>265</v>
       </c>
-      <c r="J37" s="31" t="str">
+      <c r="L37" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingResidueTreatment</v>
       </c>
-      <c r="K37" s="32" t="str">
-        <f>IF(L37="",P2,L37)</f>
+      <c r="M37" s="32" t="str">
+        <f>IF(N37="",R2,N37)</f>
         <v>None</v>
       </c>
-      <c r="L37" s="43"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1">
-      <c r="E38" s="1"/>
-      <c r="H38" t="str">
+      <c r="N37" s="43"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A38" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B38" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C38" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="J38" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="I38" t="s">
+      <c r="K38" t="s">
         <v>266</v>
       </c>
-      <c r="J38" s="34" t="str">
+      <c r="L38" s="34" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishN</v>
       </c>
-      <c r="K38" s="35">
-        <f>IF(L38="",0,L38)</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="43"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" t="e">
-        <f t="array" ref="A39">_xll.GetDailyNBalance(C2:C33,J2:K38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B39" s="27"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="B40" s="28"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="B41" s="28"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="B42" s="28"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="B43" s="28"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="B44" s="28"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="B45" s="28"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="B46" s="28"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="B47" s="28"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="B48" s="28"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="28"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="28"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="28"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="28"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="28"/>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="28"/>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" s="28"/>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" s="28"/>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="28"/>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="28"/>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="28"/>
-    </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="28"/>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="28"/>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="28"/>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="28"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="28"/>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="28"/>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="28"/>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="28"/>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="28"/>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" s="28"/>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" s="28"/>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" s="28"/>
+      <c r="M38" s="35">
+        <f>IF(N38="",0,N38)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="43"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B39" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C39" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B40" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C40" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B41" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C41" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B42" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C42" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B43" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C43" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B44" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C44" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B45" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C45" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B46" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C46" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B47" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C47" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B48" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C48" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B49" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C49" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B50" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C50" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B51" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C51" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B52" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C52" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B53" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C53" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B54" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C54" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B55" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C55" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B56" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C56" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B57" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C57" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B58" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C58" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B59" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C59" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B60" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C60" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B61" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C61" s="46" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:L13 K25:L25 K37:L37" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
-      <formula1>$P$2:$P$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:N13 M37:N37 M25:N25" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
+      <formula1>$R$2:$R$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L12 L24 L36" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
-      <formula1>$O$2:$O$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N12 N36 N24" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
+      <formula1>$Q$2:$Q$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10 L22 L34" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
-      <formula1>$N$2:$N$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N10 N34 N22" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
+      <formula1>$P$2:$P$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5 L17 L29" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
-      <formula1>$Q$2:$Q$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5 N29 N17" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
+      <formula1>$S$2:$S$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L8 L18:L20 L30:L32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N8 N18:N20 N30:N32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -3943,19 +5667,19 @@
           <x14:formula1>
             <xm:f>CropCoefficients!$F$3:$F$78</xm:f>
           </x14:formula1>
-          <xm:sqref>F1</xm:sqref>
+          <xm:sqref>H1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3A6DE27-0EE4-4266-A7F4-377B95F78D99}">
           <x14:formula1>
             <xm:f>CropCoefficients!$B$3:$B$78</xm:f>
           </x14:formula1>
-          <xm:sqref>G2 G14 G26</xm:sqref>
+          <xm:sqref>I3 I15 I27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFFB7881-7C85-4FD9-826D-70611F88B0E7}">
           <x14:formula1>
             <xm:f>CropCoefficients!$K$3:$K$78</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:L3 K15:L15 K27:L27</xm:sqref>
+          <xm:sqref>M3:N3 M15:N15 M27:N27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Basic residue model integrated
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED30C2C5-A6B9-4444-A77A-5A548BEB4F21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33310ED4-C0FA-4F1C-B84D-32973EE3ED25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
@@ -1461,94 +1461,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>50.014400000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15783182418578878</c:v>
+                  <c:v>49.730021815420564</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7235440432093423E-2</c:v>
+                  <c:v>49.574885831650356</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20235506135482084</c:v>
+                  <c:v>49.223681836607085</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.764623288907412E-2</c:v>
+                  <c:v>49.143732051174652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2106526484524287</c:v>
+                  <c:v>48.786636437289609</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23504877557079729</c:v>
+                  <c:v>48.387284487703333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33901731439190108</c:v>
+                  <c:v>47.786821651887692</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20415816274163623</c:v>
+                  <c:v>47.455028064239237</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>47.534162919679019</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>47.836685203083078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>48.13509795558236</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>48.40841278279408</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.3359956809311733</c:v>
+                  <c:v>47.334944133214066</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.78047365225292076</c:v>
+                  <c:v>46.793065058549367</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5414316932853449</c:v>
+                  <c:v>45.466450676534137</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.49411391691496576</c:v>
+                  <c:v>45.153900425572616</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.4824885863887793</c:v>
+                  <c:v>43.826063594329923</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>43.955967244912515</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>44.261763809315561</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>44.521168184266507</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>44.741972353269638</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>44.919693257413641</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.70799810604867464</c:v>
+                  <c:v>44.353738980233899</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.43617634163370145</c:v>
+                  <c:v>44.026761897523151</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.90771934575078106</c:v>
+                  <c:v>43.203852018310926</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30344580387295927</c:v>
+                  <c:v>42.96370348630699</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.94494045740038679</c:v>
+                  <c:v>42.065365531775008</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.0543760030125071</c:v>
+                  <c:v>41.044131166019824</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.5207555114147002</c:v>
+                  <c:v>39.546640210142314</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>#N/A</c:v>
@@ -3465,15 +3465,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3839,1312 +3839,1407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1">
       <c r="A1" t="str">
-        <f t="array" ref="A1:C61">_xll.GetDailyNBalance(G3:G34,L2:M38)</f>
+        <f t="array" ref="A1:D61">_xll.GetDailyNBalance(H3:H34,M2:N38)</f>
         <v>Date</v>
       </c>
       <c r="B1" s="28" t="str">
-        <v>RootN</v>
+        <v>SoilMineralN</v>
       </c>
       <c r="C1" t="str">
         <v>UptakeN</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="D1" t="str">
+        <v>ResidueN</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" t="s">
         <v>277</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>276</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="R1" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1">
+    <row r="2" spans="1:20" ht="15.75" thickBot="1">
       <c r="A2" s="28">
         <v>44929</v>
       </c>
       <c r="B2" s="46">
-        <v>0</v>
+        <v>50.014400000000002</v>
       </c>
       <c r="C2" s="46">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" s="46">
+        <v>1.44E-2</v>
+      </c>
+      <c r="G2" t="s">
         <v>255</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="M2" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="M2" s="41">
-        <f>IF(N2="",50,N2)</f>
+      <c r="N2" s="41">
+        <f>IF(O2="",50,O2)</f>
         <v>50</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>63</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>253</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1">
       <c r="A3" s="28">
         <v>44930</v>
       </c>
       <c r="B3" s="46">
-        <v>0.15783182418578878</v>
+        <v>49.730021815420564</v>
       </c>
       <c r="C3" s="46">
-        <v>0</v>
-      </c>
-      <c r="E3" s="26">
-        <f>M9</f>
+        <v>0.31566364837157701</v>
+      </c>
+      <c r="D3" s="46">
+        <v>3.1285463792140297E-2</v>
+      </c>
+      <c r="F3" s="26">
+        <f>N9</f>
         <v>44929</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
       </c>
       <c r="G3">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
         <v>272</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>270</v>
       </c>
-      <c r="L3" s="29" t="str">
-        <f>J3&amp;K3</f>
+      <c r="M3" s="29" t="str">
+        <f>K3&amp;L3</f>
         <v>PriorCropName</v>
       </c>
-      <c r="M3" s="30" t="str">
-        <f>N3</f>
+      <c r="N3" s="30" t="str">
+        <f>O3</f>
         <v>Annual ryegrass Fodder General</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="O3" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>123</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>49</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>249</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" s="28">
         <v>44931</v>
       </c>
       <c r="B4" s="46">
-        <v>9.7235440432093423E-2</v>
+        <v>49.574885831650356</v>
       </c>
       <c r="C4" s="46">
-        <v>0</v>
-      </c>
-      <c r="E4" s="26">
-        <f>E3+1</f>
+        <v>0.19447088086418701</v>
+      </c>
+      <c r="D4" s="46">
+        <v>3.9334897093980185E-2</v>
+      </c>
+      <c r="F4" s="26">
+        <f>F3+1</f>
         <v>44930</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>14.387874318606862</v>
       </c>
-      <c r="G4">
-        <f>F4+F3</f>
+      <c r="H4">
+        <f>G4+G3</f>
         <v>26.387874318606862</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>7</v>
       </c>
-      <c r="J4" t="str">
-        <f>J3</f>
+      <c r="K4" t="str">
+        <f>K3</f>
         <v>Prior</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>256</v>
       </c>
-      <c r="L4" s="31" t="str">
-        <f t="shared" ref="L4:L14" si="0">J4&amp;K4</f>
+      <c r="M4" s="31" t="str">
+        <f t="shared" ref="M4:M14" si="0">K4&amp;L4</f>
         <v>PriorSaleableYield</v>
       </c>
-      <c r="M4" s="32">
-        <f>IF(N4="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I4,FALSE),N4)</f>
+      <c r="N4" s="32">
+        <f>IF(O4="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J4,FALSE),O4)</f>
         <v>5</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="Q4" t="s">
+      <c r="O4" s="43"/>
+      <c r="R4" t="s">
         <v>43</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="28">
         <v>44932</v>
       </c>
       <c r="B5" s="46">
-        <v>0.20235506135482084</v>
+        <v>49.223681836607085</v>
       </c>
       <c r="C5" s="46">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26">
-        <f t="shared" ref="E5:E34" si="1">E4+1</f>
+        <v>0.40471012270964102</v>
+      </c>
+      <c r="D5" s="46">
+        <v>5.350612766636547E-2</v>
+      </c>
+      <c r="F5" s="26">
+        <f t="shared" ref="F5:F34" si="1">F4+1</f>
         <v>44931</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7.6885371447735746</v>
       </c>
-      <c r="G5">
-        <f>F5+G4</f>
+      <c r="H5">
+        <f>G5+H4</f>
         <v>34.076411463380438</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>8</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" ref="J5:J14" si="2">J4</f>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K14" si="2">K4</f>
         <v>Prior</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="31" t="str">
+      <c r="M5" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorUnits</v>
       </c>
-      <c r="M5" s="32" t="str">
-        <f>IF(N5="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I5,FALSE),N5)</f>
+      <c r="N5" s="32" t="str">
+        <f>IF(O5="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J5,FALSE),O5)</f>
         <v>t/ha</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="Q5" t="s">
+      <c r="O5" s="43"/>
+      <c r="R5" t="s">
         <v>55</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="28">
         <v>44933</v>
       </c>
       <c r="B6" s="46">
-        <v>6.764623288907412E-2</v>
+        <v>49.143732051174652</v>
       </c>
       <c r="C6" s="46">
-        <v>0</v>
-      </c>
-      <c r="E6" s="26">
+        <v>0.13529246577814799</v>
+      </c>
+      <c r="D6" s="46">
+        <v>5.534268034572009E-2</v>
+      </c>
+      <c r="F6" s="26">
         <f t="shared" si="1"/>
         <v>44932</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>13.912023293050638</v>
       </c>
-      <c r="G6">
-        <f t="shared" ref="G6:G34" si="3">F6+G5</f>
+      <c r="H6">
+        <f t="shared" ref="H6:H34" si="3">G6+H5</f>
         <v>47.988434756431076</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>12</v>
       </c>
-      <c r="J6" t="str">
+      <c r="K6" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>258</v>
       </c>
-      <c r="L6" s="31" t="str">
+      <c r="M6" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorFieldLoss</v>
       </c>
-      <c r="M6" s="32">
-        <f>IF(N6="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I6,FALSE),N6)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="43"/>
-      <c r="Q6" t="s">
+      <c r="N6" s="32">
+        <v>50</v>
+      </c>
+      <c r="O6" s="43"/>
+      <c r="R6" t="s">
         <v>34</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="28">
         <v>44934</v>
       </c>
       <c r="B7" s="46">
-        <v>0.2106526484524287</v>
+        <v>48.786636437289609</v>
       </c>
       <c r="C7" s="46">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
+        <v>0.42130529690485702</v>
+      </c>
+      <c r="D7" s="46">
+        <v>6.4209683019808755E-2</v>
+      </c>
+      <c r="F7" s="26">
         <f t="shared" si="1"/>
         <v>44933</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4.1491642970301701</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="3"/>
         <v>52.137599053461244</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>11</v>
       </c>
-      <c r="J7" t="str">
+      <c r="K7" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>259</v>
       </c>
-      <c r="L7" s="31" t="str">
+      <c r="M7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorDressingLoss</v>
       </c>
-      <c r="M7" s="32">
-        <f>IF(N7="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I7,FALSE),N7)</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="43"/>
-      <c r="Q7" t="s">
+      <c r="N7" s="32">
+        <f>IF(O7="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J7,FALSE),O7)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="43"/>
+      <c r="R7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1">
       <c r="A8" s="28">
         <v>44935</v>
       </c>
       <c r="B8" s="46">
-        <v>0.23504877557079729</v>
+        <v>48.387284487703333</v>
       </c>
       <c r="C8" s="46">
-        <v>0</v>
-      </c>
-      <c r="E8" s="26">
+        <v>0.47009755114159502</v>
+      </c>
+      <c r="D8" s="46">
+        <v>7.0745601555314758E-2</v>
+      </c>
+      <c r="F8" s="26">
         <f t="shared" si="1"/>
         <v>44934</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>11.680823993463974</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="3"/>
         <v>63.818423046925219</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>15</v>
       </c>
-      <c r="J8" t="str">
+      <c r="K8" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>260</v>
       </c>
-      <c r="L8" s="31" t="str">
+      <c r="M8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorMoistureContent</v>
       </c>
-      <c r="M8" s="32">
-        <f>IF(N8="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I8,FALSE),N8)</f>
+      <c r="N8" s="32">
+        <f>IF(O8="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J8,FALSE),O8)</f>
         <v>80</v>
       </c>
-      <c r="N8" s="43"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1">
+      <c r="O8" s="43"/>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" thickBot="1">
       <c r="A9" s="28">
         <v>44936</v>
       </c>
       <c r="B9" s="46">
-        <v>0.33901731439190108</v>
+        <v>47.786821651887692</v>
       </c>
       <c r="C9" s="46">
-        <v>0</v>
-      </c>
-      <c r="E9" s="26">
+        <v>0.67803462878380205</v>
+      </c>
+      <c r="D9" s="46">
+        <v>7.7571792968154946E-2</v>
+      </c>
+      <c r="F9" s="26">
         <f t="shared" si="1"/>
         <v>44935</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>11.289351844181724</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="3"/>
         <v>75.107774891106942</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>261</v>
       </c>
-      <c r="L9" s="31" t="str">
+      <c r="M9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishDate</v>
       </c>
-      <c r="M9" s="33">
-        <f>N9</f>
+      <c r="N9" s="33">
+        <f>O9</f>
         <v>44929</v>
       </c>
-      <c r="N9" s="44">
+      <c r="O9" s="44">
         <v>44929</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1">
+    <row r="10" spans="1:20" ht="15.75" thickBot="1">
       <c r="A10" s="28">
         <v>44937</v>
       </c>
       <c r="B10" s="46">
-        <v>0.20415816274163623</v>
+        <v>47.455028064239237</v>
       </c>
       <c r="C10" s="46">
-        <v>0</v>
-      </c>
-      <c r="E10" s="26">
+        <v>0.40831632548327201</v>
+      </c>
+      <c r="D10" s="46">
+        <v>7.6522737834811005E-2</v>
+      </c>
+      <c r="F10" s="26">
         <f t="shared" si="1"/>
         <v>44936</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>13.934890823546613</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="3"/>
         <v>89.042665714653552</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>262</v>
       </c>
-      <c r="L10" s="31" t="str">
+      <c r="M10" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishStage</v>
       </c>
-      <c r="M10" s="32" t="str">
-        <f>IF(N10="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I10,FALSE),N10)</f>
+      <c r="N10" s="32" t="str">
+        <f>IF(O10="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J10,FALSE),O10)</f>
         <v>Seed</v>
       </c>
-      <c r="N10" s="43"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1">
+      <c r="O10" s="43"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" thickBot="1">
       <c r="A11" s="28">
         <v>44938</v>
       </c>
       <c r="B11" s="46">
-        <v>0</v>
+        <v>47.534162919679019</v>
       </c>
       <c r="C11" s="46">
         <v>0</v>
       </c>
-      <c r="E11" s="26">
+      <c r="D11" s="46">
+        <v>7.9134855439784074E-2</v>
+      </c>
+      <c r="F11" s="26">
         <f t="shared" si="1"/>
         <v>44937</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>7.3816990790906738</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="3"/>
         <v>96.424364793744232</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>263</v>
       </c>
-      <c r="L11" s="31" t="str">
+      <c r="M11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorHarvestDate</v>
       </c>
-      <c r="M11" s="33">
-        <f>N11</f>
+      <c r="N11" s="33">
+        <f>O11</f>
         <v>44938</v>
       </c>
-      <c r="N11" s="44">
+      <c r="O11" s="44">
         <v>44938</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" s="28">
         <v>44939</v>
       </c>
       <c r="B12" s="46">
-        <v>0</v>
+        <v>47.836685203083078</v>
       </c>
       <c r="C12" s="46">
         <v>0</v>
       </c>
-      <c r="E12" s="26">
+      <c r="D12" s="46">
+        <v>0.30252228340405707</v>
+      </c>
+      <c r="F12" s="26">
         <f t="shared" si="1"/>
         <v>44938</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>13.932559604705048</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="3"/>
         <v>110.35692439844928</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>5</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>264</v>
       </c>
-      <c r="L12" s="31" t="str">
+      <c r="M12" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorHarvestStage</v>
       </c>
-      <c r="M12" s="32" t="str">
-        <f>IF(N12="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I12,FALSE),N12)</f>
+      <c r="N12" s="32" t="str">
+        <f>IF(O12="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J12,FALSE),O12)</f>
         <v>EarlyReproductive</v>
       </c>
-      <c r="N12" s="43"/>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="O12" s="43"/>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="28">
         <v>44940</v>
       </c>
       <c r="B13" s="46">
-        <v>0</v>
+        <v>48.13509795558236</v>
       </c>
       <c r="C13" s="46">
         <v>0</v>
       </c>
-      <c r="E13" s="26">
+      <c r="D13" s="46">
+        <v>0.29841275249928356</v>
+      </c>
+      <c r="F13" s="26">
         <f t="shared" si="1"/>
         <v>44939</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>5.3540880739901002</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="3"/>
         <v>115.71101247243938</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>265</v>
       </c>
-      <c r="L13" s="31" t="str">
+      <c r="M13" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorResidueTreatment</v>
       </c>
-      <c r="M13" s="32" t="str">
-        <f>IF(N13="",R2,N13)</f>
+      <c r="N13" s="32" t="str">
+        <f>IF(O13="",S2,O13)</f>
         <v>None</v>
       </c>
-      <c r="N13" s="43"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1">
+      <c r="O13" s="43"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1">
       <c r="A14" s="28">
         <v>44941</v>
       </c>
       <c r="B14" s="46">
-        <v>0</v>
+        <v>48.40841278279408</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
       </c>
-      <c r="E14" s="26">
+      <c r="D14" s="46">
+        <v>0.27331482721172123</v>
+      </c>
+      <c r="F14" s="26">
         <f t="shared" si="1"/>
         <v>44940</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>13.363497784448709</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="3"/>
         <v>129.07451025688809</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>266</v>
       </c>
-      <c r="L14" s="34" t="str">
+      <c r="M14" s="34" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishN</v>
       </c>
-      <c r="M14" s="35">
-        <f>IF(N14="",0,N14)</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="43"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1">
+      <c r="N14" s="35">
+        <f>IF(O14="",0,O14)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="43"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" thickBot="1">
       <c r="A15" s="28">
         <v>44942</v>
       </c>
       <c r="B15" s="46">
-        <v>1.3359956809311733</v>
+        <v>47.334944133214066</v>
       </c>
       <c r="C15" s="46">
-        <v>0</v>
-      </c>
-      <c r="E15" s="26">
+        <v>1.3359956809311699</v>
+      </c>
+      <c r="D15" s="46">
+        <v>0.26252703135115807</v>
+      </c>
+      <c r="F15" s="26">
         <f t="shared" si="1"/>
         <v>44941</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>6.6646938971593457</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="3"/>
         <v>135.73920415404743</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>273</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>270</v>
       </c>
-      <c r="L15" s="37" t="str">
-        <f>J15&amp;K15</f>
+      <c r="M15" s="37" t="str">
+        <f>K15&amp;L15</f>
         <v>CurrentCropName</v>
       </c>
-      <c r="M15" s="38" t="str">
-        <f>N15</f>
+      <c r="N15" s="38" t="str">
+        <f>O15</f>
         <v>Potato Vegetable General</v>
       </c>
-      <c r="N15" s="45" t="s">
+      <c r="O15" s="45" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="28">
         <v>44943</v>
       </c>
       <c r="B16" s="46">
-        <v>0.78047365225292076</v>
+        <v>46.793065058549367</v>
       </c>
       <c r="C16" s="46">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26">
+        <v>0.78047365225292098</v>
+      </c>
+      <c r="D16" s="46">
+        <v>0.23859457758822508</v>
+      </c>
+      <c r="F16" s="26">
         <f t="shared" si="1"/>
         <v>44942</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>15.119829112109056</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="3"/>
         <v>150.85903326615647</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>7</v>
       </c>
-      <c r="J16" t="str">
-        <f>J15</f>
+      <c r="K16" t="str">
+        <f>K15</f>
         <v>Current</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>256</v>
       </c>
-      <c r="L16" s="18" t="str">
-        <f t="shared" ref="L16:L26" si="4">J16&amp;K16</f>
+      <c r="M16" s="18" t="str">
+        <f t="shared" ref="M16:M26" si="4">K16&amp;L16</f>
         <v>CurrentSaleableYield</v>
       </c>
-      <c r="M16" s="19">
-        <f>IF(N16="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I16,FALSE),N16)</f>
+      <c r="N16" s="19">
+        <f>IF(O16="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J16,FALSE),O16)</f>
         <v>50</v>
       </c>
-      <c r="N16" s="43">
+      <c r="O16" s="43">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="28">
         <v>44944</v>
       </c>
       <c r="B17" s="46">
-        <v>1.5414316932853449</v>
+        <v>45.466450676534137</v>
       </c>
       <c r="C17" s="46">
-        <v>0</v>
-      </c>
-      <c r="E17" s="26">
+        <v>1.54143169328534</v>
+      </c>
+      <c r="D17" s="46">
+        <v>0.21481731127010711</v>
+      </c>
+      <c r="F17" s="26">
         <f t="shared" si="1"/>
         <v>44943</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>10.605844567907475</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="3"/>
         <v>161.46487783406394</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>8</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" ref="J17:J26" si="5">J16</f>
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K26" si="5">K16</f>
         <v>Current</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>257</v>
       </c>
-      <c r="L17" s="18" t="str">
+      <c r="M17" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentUnits</v>
       </c>
-      <c r="M17" s="19" t="str">
-        <f>IF(N17="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I17,FALSE),N17)</f>
+      <c r="N17" s="19" t="str">
+        <f>IF(O17="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J17,FALSE),O17)</f>
         <v>t/ha</v>
       </c>
-      <c r="N17" s="43" t="s">
+      <c r="O17" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="28">
         <v>44945</v>
       </c>
       <c r="B18" s="46">
-        <v>0.49411391691496576</v>
+        <v>45.153900425572616</v>
       </c>
       <c r="C18" s="46">
-        <v>0</v>
-      </c>
-      <c r="E18" s="26">
+        <v>0.49411391691496598</v>
+      </c>
+      <c r="D18" s="46">
+        <v>0.18156366595344955</v>
+      </c>
+      <c r="F18" s="26">
         <f t="shared" si="1"/>
         <v>44944</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>11.901756295522578</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="3"/>
         <v>173.36663412958652</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>12</v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>258</v>
       </c>
-      <c r="L18" s="18" t="str">
+      <c r="M18" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentFieldLoss</v>
       </c>
-      <c r="M18" s="19">
-        <f>IF(N18="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I18,FALSE),N18)</f>
+      <c r="N18" s="19">
+        <f>IF(O18="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J18,FALSE),O18)</f>
         <v>5</v>
       </c>
-      <c r="N18" s="43">
+      <c r="O18" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="28">
         <v>44946</v>
       </c>
       <c r="B19" s="46">
-        <v>1.4824885863887793</v>
+        <v>43.826063594329923</v>
       </c>
       <c r="C19" s="46">
-        <v>0</v>
-      </c>
-      <c r="E19" s="26">
+        <v>1.48248858638878</v>
+      </c>
+      <c r="D19" s="46">
+        <v>0.15465175514608945</v>
+      </c>
+      <c r="F19" s="26">
         <f t="shared" si="1"/>
         <v>44945</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>3.8939814164824327</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="3"/>
         <v>177.26061554606895</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>11</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>259</v>
       </c>
-      <c r="L19" s="18" t="str">
+      <c r="M19" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentDressingLoss</v>
       </c>
-      <c r="M19" s="19">
-        <f>IF(N19="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I19,FALSE),N19)</f>
+      <c r="N19" s="19">
+        <f>IF(O19="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J19,FALSE),O19)</f>
         <v>5</v>
       </c>
-      <c r="N19" s="43">
+      <c r="O19" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1">
+    <row r="20" spans="1:15" ht="15.75" thickBot="1">
       <c r="A20" s="28">
         <v>44947</v>
       </c>
       <c r="B20" s="46">
-        <v>0</v>
+        <v>43.955967244912515</v>
       </c>
       <c r="C20" s="46">
         <v>0</v>
       </c>
-      <c r="E20" s="26">
+      <c r="D20" s="46">
+        <v>0.12990365058259176</v>
+      </c>
+      <c r="F20" s="26">
         <f t="shared" si="1"/>
         <v>44946</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>6.2562047514789443</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="3"/>
         <v>183.51682029754789</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>15</v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>260</v>
       </c>
-      <c r="L20" s="18" t="str">
+      <c r="M20" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentMoistureContent</v>
       </c>
-      <c r="M20" s="19">
-        <f>IF(N20="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I20,FALSE),N20)</f>
+      <c r="N20" s="19">
+        <f>IF(O20="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J20,FALSE),O20)</f>
         <v>77.7</v>
       </c>
-      <c r="N20" s="43"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O20" s="43"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1">
       <c r="A21" s="28">
         <v>44948</v>
       </c>
       <c r="B21" s="46">
-        <v>0</v>
+        <v>44.261763809315561</v>
       </c>
       <c r="C21" s="46">
         <v>0</v>
       </c>
-      <c r="E21" s="26">
+      <c r="D21" s="46">
+        <v>0.30579656440304448</v>
+      </c>
+      <c r="F21" s="26">
         <f t="shared" si="1"/>
         <v>44947</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>5.2802002140493496</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="3"/>
         <v>188.79702051159725</v>
       </c>
-      <c r="J21" t="str">
+      <c r="K21" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>261</v>
       </c>
-      <c r="L21" s="18" t="str">
+      <c r="M21" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishDate</v>
       </c>
-      <c r="M21" s="39">
-        <f>N21</f>
+      <c r="N21" s="39">
+        <f>O21</f>
         <v>44941</v>
       </c>
-      <c r="N21" s="44">
+      <c r="O21" s="44">
         <v>44941</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1">
+    <row r="22" spans="1:15" ht="15.75" thickBot="1">
       <c r="A22" s="28">
         <v>44949</v>
       </c>
       <c r="B22" s="46">
-        <v>0</v>
+        <v>44.521168184266507</v>
       </c>
       <c r="C22" s="46">
         <v>0</v>
       </c>
-      <c r="E22" s="26">
+      <c r="D22" s="46">
+        <v>0.25940437495094348</v>
+      </c>
+      <c r="F22" s="26">
         <f t="shared" si="1"/>
         <v>44948</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>14.049139077238873</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="3"/>
         <v>202.84615958883612</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="J22" t="str">
+      <c r="K22" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>262</v>
       </c>
-      <c r="L22" s="18" t="str">
+      <c r="M22" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishStage</v>
       </c>
-      <c r="M22" s="19" t="str">
-        <f>IF(N22="",VLOOKUP(M$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I22,FALSE),N22)</f>
+      <c r="N22" s="19" t="str">
+        <f>IF(O22="",VLOOKUP(N$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J22,FALSE),O22)</f>
         <v>Seedling</v>
       </c>
-      <c r="N22" s="43" t="s">
+      <c r="O22" s="43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1">
+    <row r="23" spans="1:15" ht="15.75" thickBot="1">
       <c r="A23" s="28">
         <v>44950</v>
       </c>
       <c r="B23" s="46">
-        <v>0</v>
+        <v>44.741972353269638</v>
       </c>
       <c r="C23" s="46">
         <v>0</v>
       </c>
-      <c r="E23" s="26">
+      <c r="D23" s="46">
+        <v>0.22080416900312955</v>
+      </c>
+      <c r="F23" s="26">
         <f t="shared" si="1"/>
         <v>44949</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>13.012433227854736</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="3"/>
         <v>215.85859281669084</v>
       </c>
-      <c r="J23" t="str">
+      <c r="K23" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>263</v>
       </c>
-      <c r="L23" s="18" t="str">
+      <c r="M23" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentHarvestDate</v>
       </c>
-      <c r="M23" s="39">
-        <f>N23</f>
+      <c r="N23" s="39">
+        <f>O23</f>
         <v>44947</v>
       </c>
-      <c r="N23" s="44">
+      <c r="O23" s="44">
         <v>44947</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" s="28">
         <v>44951</v>
       </c>
       <c r="B24" s="46">
-        <v>0</v>
+        <v>44.919693257413641</v>
       </c>
       <c r="C24" s="46">
         <v>0</v>
       </c>
-      <c r="E24" s="26">
+      <c r="D24" s="46">
+        <v>0.17772090414400205</v>
+      </c>
+      <c r="F24" s="26">
         <f t="shared" si="1"/>
         <v>44950</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>18.45901588220935</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="3"/>
         <v>234.31760869890019</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>5</v>
       </c>
-      <c r="J24" t="str">
+      <c r="K24" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>264</v>
       </c>
-      <c r="L24" s="18" t="str">
+      <c r="M24" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentHarvestStage</v>
       </c>
-      <c r="M24" s="19" t="str">
-        <f>IF(N24="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I24,FALSE),N24)</f>
+      <c r="N24" s="19" t="str">
+        <f>IF(O24="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J24,FALSE),O24)</f>
         <v>Vegetative</v>
       </c>
-      <c r="N24" s="43" t="s">
+      <c r="O24" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="28">
         <v>44952</v>
       </c>
       <c r="B25" s="46">
-        <v>0.70799810604867464</v>
+        <v>44.353738980233899</v>
       </c>
       <c r="C25" s="46">
-        <v>0</v>
-      </c>
-      <c r="E25" s="26">
+        <v>0.70799810604867497</v>
+      </c>
+      <c r="D25" s="46">
+        <v>0.14204382886893566</v>
+      </c>
+      <c r="F25" s="26">
         <f t="shared" si="1"/>
         <v>44951</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>11.995492344501493</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="3"/>
         <v>246.31310104340167</v>
       </c>
-      <c r="J25" t="str">
+      <c r="K25" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>265</v>
       </c>
-      <c r="L25" s="18" t="str">
+      <c r="M25" s="18" t="str">
         <f t="shared" si="4"/>
         <v>CurrentResidueTreatment</v>
       </c>
-      <c r="M25" s="19" t="str">
-        <f>IF(N25="",R2,N25)</f>
+      <c r="N25" s="19" t="str">
+        <f>IF(O25="",S2,O25)</f>
         <v>Incorporated</v>
       </c>
-      <c r="N25" s="43" t="s">
+      <c r="O25" s="43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1">
+    <row r="26" spans="1:15" ht="15.75" thickBot="1">
       <c r="A26" s="28">
         <v>44953</v>
       </c>
       <c r="B26" s="46">
-        <v>0.43617634163370145</v>
+        <v>44.026761897523151</v>
       </c>
       <c r="C26" s="46">
-        <v>0</v>
-      </c>
-      <c r="E26" s="26">
+        <v>0.436176341633701</v>
+      </c>
+      <c r="D26" s="46">
+        <v>0.10919925892295834</v>
+      </c>
+      <c r="F26" s="26">
         <f t="shared" si="1"/>
         <v>44952</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>14.89124712931573</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="3"/>
         <v>261.2043481727174</v>
       </c>
-      <c r="J26" t="str">
+      <c r="K26" t="str">
         <f t="shared" si="5"/>
         <v>Current</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>266</v>
       </c>
-      <c r="L26" s="23" t="str">
+      <c r="M26" s="23" t="str">
         <f t="shared" si="4"/>
         <v>CurrentEstablishN</v>
       </c>
-      <c r="M26" s="24">
-        <f>IF(N26="",0,N26)</f>
+      <c r="N26" s="24">
+        <f>IF(O26="",0,O26)</f>
         <v>10</v>
       </c>
-      <c r="N26" s="43">
+      <c r="O26" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1">
       <c r="A27" s="28">
         <v>44954</v>
       </c>
       <c r="B27" s="46">
-        <v>0.90771934575078106</v>
+        <v>43.203852018310926</v>
       </c>
       <c r="C27" s="46">
-        <v>0</v>
-      </c>
-      <c r="E27" s="26">
+        <v>0.90771934575078095</v>
+      </c>
+      <c r="D27" s="46">
+        <v>8.4809466538550801E-2</v>
+      </c>
+      <c r="F27" s="26">
         <f t="shared" si="1"/>
         <v>44953</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>10.598117463308858</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="3"/>
         <v>271.80246563602628</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>274</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>270</v>
       </c>
-      <c r="L27" s="29" t="str">
-        <f>J27&amp;K27</f>
+      <c r="M27" s="29" t="str">
+        <f>K27&amp;L27</f>
         <v>FollowingCropName</v>
       </c>
-      <c r="M27" s="30" t="str">
-        <f>N27</f>
+      <c r="N27" s="30" t="str">
+        <f>O27</f>
         <v>Oat Grain General</v>
       </c>
-      <c r="N27" s="45" t="s">
+      <c r="O27" s="45" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" s="28">
         <v>44955</v>
       </c>
       <c r="B28" s="46">
-        <v>0.30344580387295927</v>
+        <v>42.96370348630699</v>
       </c>
       <c r="C28" s="46">
-        <v>0</v>
-      </c>
-      <c r="E28" s="26">
+        <v>0.303445803872959</v>
+      </c>
+      <c r="D28" s="46">
+        <v>6.3297271869023966E-2</v>
+      </c>
+      <c r="F28" s="26">
         <f t="shared" si="1"/>
         <v>44954</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>18.08459347173163</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="3"/>
         <v>289.88705910775792</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>7</v>
       </c>
-      <c r="J28" t="str">
-        <f>J27</f>
+      <c r="K28" t="str">
+        <f>K27</f>
         <v>Following</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>256</v>
       </c>
-      <c r="L28" s="31" t="str">
-        <f t="shared" ref="L28:L38" si="6">J28&amp;K28</f>
+      <c r="M28" s="31" t="str">
+        <f t="shared" ref="M28:M38" si="6">K28&amp;L28</f>
         <v>FollowingSaleableYield</v>
       </c>
-      <c r="M28" s="32">
-        <f>IF(N28="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I28,FALSE),N28)</f>
+      <c r="N28" s="32">
+        <f>IF(O28="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J28,FALSE),O28)</f>
         <v>6</v>
       </c>
-      <c r="N28" s="43"/>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28" s="43"/>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="28">
         <v>44956</v>
       </c>
       <c r="B29" s="46">
-        <v>0.94494045740038679</v>
+        <v>42.065365531775008</v>
       </c>
       <c r="C29" s="46">
-        <v>0</v>
-      </c>
-      <c r="E29" s="26">
+        <v>0.94494045740038701</v>
+      </c>
+      <c r="D29" s="46">
+        <v>4.6602502868402E-2</v>
+      </c>
+      <c r="F29" s="26">
         <f t="shared" si="1"/>
         <v>44955</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>14.79161849090584</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="3"/>
         <v>304.67867759866374</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>8</v>
       </c>
-      <c r="J29" t="str">
-        <f t="shared" ref="J29:J38" si="7">J28</f>
+      <c r="K29" t="str">
+        <f t="shared" ref="K29:K38" si="7">K28</f>
         <v>Following</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>257</v>
       </c>
-      <c r="L29" s="31" t="str">
+      <c r="M29" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingUnits</v>
       </c>
-      <c r="M29" s="32" t="str">
-        <f>IF(N29="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I29,FALSE),N29)</f>
+      <c r="N29" s="32" t="str">
+        <f>IF(O29="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J29,FALSE),O29)</f>
         <v>t/ha</v>
       </c>
-      <c r="N29" s="43"/>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" s="43"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="28">
         <v>44957</v>
       </c>
       <c r="B30" s="46">
-        <v>1.0543760030125071</v>
+        <v>41.044131166019824</v>
       </c>
       <c r="C30" s="46">
-        <v>0</v>
-      </c>
-      <c r="E30" s="26">
+        <v>1.05437600301251</v>
+      </c>
+      <c r="D30" s="46">
+        <v>3.3141637257324399E-2</v>
+      </c>
+      <c r="F30" s="26">
         <f t="shared" si="1"/>
         <v>44956</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>17.933505589637022</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="3"/>
         <v>322.61218318830078</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>12</v>
       </c>
-      <c r="J30" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>258</v>
       </c>
-      <c r="L30" s="31" t="str">
+      <c r="M30" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingFieldLoss</v>
       </c>
-      <c r="M30" s="32">
-        <f>IF(N30="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I30,FALSE),N30)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="43"/>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="N30" s="32">
+        <f>IF(O30="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J30,FALSE),O30)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="43"/>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="28">
         <v>44958</v>
       </c>
       <c r="B31" s="46">
-        <v>1.5207555114147002</v>
+        <v>39.546640210142314</v>
       </c>
       <c r="C31" s="46">
-        <v>0</v>
-      </c>
-      <c r="E31" s="26">
+        <v>1.5207555114147</v>
+      </c>
+      <c r="D31" s="46">
+        <v>2.3264555537192054E-2</v>
+      </c>
+      <c r="F31" s="26">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>16.082282662694066</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="3"/>
         <v>338.69446585099485</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>11</v>
       </c>
-      <c r="J31" t="str">
+      <c r="K31" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>259</v>
       </c>
-      <c r="L31" s="31" t="str">
+      <c r="M31" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingDressingLoss</v>
       </c>
-      <c r="M31" s="32">
-        <f>IF(N31="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I31,FALSE),N31)</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="43"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1">
+      <c r="N31" s="32">
+        <f>IF(O31="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J31,FALSE),O31)</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="43"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1">
       <c r="A32" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5154,38 +5249,41 @@
       <c r="C32" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E32" s="26">
+      <c r="D32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F32" s="26">
         <f t="shared" si="1"/>
         <v>44958</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>20.828587685127982</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="3"/>
         <v>359.5230535361228</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>15</v>
       </c>
-      <c r="J32" t="str">
+      <c r="K32" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>260</v>
       </c>
-      <c r="L32" s="31" t="str">
+      <c r="M32" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingMoistureContent</v>
       </c>
-      <c r="M32" s="32">
-        <f>IF(N32="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I32,FALSE),N32)</f>
+      <c r="N32" s="32">
+        <f>IF(O32="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J32,FALSE),O32)</f>
         <v>13</v>
       </c>
-      <c r="N32" s="43"/>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O32" s="43"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1">
       <c r="A33" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5195,37 +5293,40 @@
       <c r="C33" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E33" s="26">
+      <c r="D33" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F33" s="26">
         <f t="shared" si="1"/>
         <v>44959</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>13.76912650928467</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="3"/>
         <v>373.29218004540746</v>
       </c>
-      <c r="J33" t="str">
+      <c r="K33" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>261</v>
       </c>
-      <c r="L33" s="31" t="str">
+      <c r="M33" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishDate</v>
       </c>
-      <c r="M33" s="33">
-        <f>N33</f>
+      <c r="N33" s="33">
+        <f>O33</f>
         <v>44951</v>
       </c>
-      <c r="N33" s="44">
+      <c r="O33" s="44">
         <v>44951</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1">
+    <row r="34" spans="1:15" ht="15.75" thickBot="1">
       <c r="A34" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5235,38 +5336,41 @@
       <c r="C34" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E34" s="26">
+      <c r="D34" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F34" s="26">
         <f t="shared" si="1"/>
         <v>44960</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>23.549644512826927</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="3"/>
         <v>396.84182455823441</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>3</v>
       </c>
-      <c r="J34" t="str">
+      <c r="K34" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>262</v>
       </c>
-      <c r="L34" s="31" t="str">
+      <c r="M34" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishStage</v>
       </c>
-      <c r="M34" s="32" t="str">
-        <f>IF(N34="",VLOOKUP(M$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I34,FALSE),N34)</f>
+      <c r="N34" s="32" t="str">
+        <f>IF(O34="",VLOOKUP(N$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J34,FALSE),O34)</f>
         <v>Seed</v>
       </c>
-      <c r="N34" s="43"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O34" s="43"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" thickBot="1">
       <c r="A35" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5276,28 +5380,31 @@
       <c r="C35" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G35" s="1"/>
-      <c r="J35" t="str">
+      <c r="D35" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="K35" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>263</v>
       </c>
-      <c r="L35" s="31" t="str">
+      <c r="M35" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingHarvestDate</v>
       </c>
-      <c r="M35" s="33">
-        <f>N35</f>
+      <c r="N35" s="33">
+        <f>O35</f>
         <v>44959</v>
       </c>
-      <c r="N35" s="44">
-        <f>E33</f>
+      <c r="O35" s="44">
+        <f>F33</f>
         <v>44959</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5307,28 +5414,31 @@
       <c r="C36" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G36" s="1"/>
-      <c r="I36">
+      <c r="D36" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="J36">
         <v>5</v>
       </c>
-      <c r="J36" t="str">
+      <c r="K36" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>264</v>
       </c>
-      <c r="L36" s="31" t="str">
+      <c r="M36" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingHarvestStage</v>
       </c>
-      <c r="M36" s="32" t="str">
-        <f>IF(N36="",VLOOKUP(M$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$I36,FALSE),N36)</f>
+      <c r="N36" s="32" t="str">
+        <f>IF(O36="",VLOOKUP(N$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$J36,FALSE),O36)</f>
         <v>EarlyReproductive</v>
       </c>
-      <c r="N36" s="43"/>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36" s="43"/>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5338,25 +5448,28 @@
       <c r="C37" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="J37" t="str">
+      <c r="D37" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="K37" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>265</v>
       </c>
-      <c r="L37" s="31" t="str">
+      <c r="M37" s="31" t="str">
         <f t="shared" si="6"/>
         <v>FollowingResidueTreatment</v>
       </c>
-      <c r="M37" s="32" t="str">
-        <f>IF(N37="",R2,N37)</f>
+      <c r="N37" s="32" t="str">
+        <f>IF(O37="",S2,O37)</f>
         <v>None</v>
       </c>
-      <c r="N37" s="43"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1">
+      <c r="O37" s="43"/>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickBot="1">
       <c r="A38" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5366,25 +5479,28 @@
       <c r="C38" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="J38" t="str">
+      <c r="D38" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="K38" t="str">
         <f t="shared" si="7"/>
         <v>Following</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>266</v>
       </c>
-      <c r="L38" s="34" t="str">
+      <c r="M38" s="34" t="str">
         <f t="shared" si="6"/>
         <v>FollowingEstablishN</v>
       </c>
-      <c r="M38" s="35">
-        <f>IF(N38="",0,N38)</f>
-        <v>0</v>
-      </c>
-      <c r="N38" s="43"/>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="N38" s="35">
+        <f>IF(O38="",0,O38)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="43"/>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5394,10 +5510,13 @@
       <c r="C39" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="D39" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5407,8 +5526,11 @@
       <c r="C40" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="D40" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5418,8 +5540,11 @@
       <c r="C41" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="D41" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5429,8 +5554,11 @@
       <c r="C42" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="D42" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5440,8 +5568,11 @@
       <c r="C43" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="D43" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5451,8 +5582,11 @@
       <c r="C44" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="D44" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5462,8 +5596,11 @@
       <c r="C45" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="D45" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5473,8 +5610,11 @@
       <c r="C46" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="D46" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5484,8 +5624,11 @@
       <c r="C47" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="D47" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5495,8 +5638,11 @@
       <c r="C48" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5506,8 +5652,11 @@
       <c r="C49" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5517,8 +5666,11 @@
       <c r="C50" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5528,8 +5680,11 @@
       <c r="C51" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5539,8 +5694,11 @@
       <c r="C52" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5550,8 +5708,11 @@
       <c r="C53" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5561,8 +5722,11 @@
       <c r="C54" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5572,8 +5736,11 @@
       <c r="C55" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5583,8 +5750,11 @@
       <c r="C56" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5594,8 +5764,11 @@
       <c r="C57" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5605,8 +5778,11 @@
       <c r="C58" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5616,8 +5792,11 @@
       <c r="C59" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5627,8 +5806,11 @@
       <c r="C60" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5638,22 +5820,25 @@
       <c r="C61" s="46" t="e">
         <v>#N/A</v>
       </c>
+      <c r="D61" s="46" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:N13 M37:N37 M25:N25" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
-      <formula1>$R$2:$R$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N13:O13 N25:O25 N37:O37" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
+      <formula1>$S$2:$S$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N12 N36 N24" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
-      <formula1>$Q$2:$Q$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O12 O24 O36" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
+      <formula1>$R$2:$R$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N10 N34 N22" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
-      <formula1>$P$2:$P$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O10 O22 O34" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
+      <formula1>$Q$2:$Q$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5 N29 N17" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
-      <formula1>$S$2:$S$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5 O17 O29" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
+      <formula1>$T$2:$T$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N8 N18:N20 N30:N32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O8 O18:O20 O30:O32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>
@@ -5667,19 +5852,19 @@
           <x14:formula1>
             <xm:f>CropCoefficients!$F$3:$F$78</xm:f>
           </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
+          <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3A6DE27-0EE4-4266-A7F4-377B95F78D99}">
           <x14:formula1>
             <xm:f>CropCoefficients!$B$3:$B$78</xm:f>
           </x14:formula1>
-          <xm:sqref>I3 I15 I27</xm:sqref>
+          <xm:sqref>J3 J15 J27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFFB7881-7C85-4FD9-826D-70611F88B0E7}">
           <x14:formula1>
             <xm:f>CropCoefficients!$K$3:$K$78</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:N3 M15:N15 M27:N27</xm:sqref>
+          <xm:sqref>N3:O3 N15:O15 N27:O27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
refactor config to tidy up type handling
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578196F2-5DB4-404B-AE3A-5F20E10CB3C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8C9DBD-1890-470A-AD8F-03365C47CAC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
   <sheets>
     <sheet name="NBalance Test" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="298">
   <si>
     <t>EndUse</t>
   </si>
@@ -899,6 +899,45 @@
   </si>
   <si>
     <t>Splits</t>
+  </si>
+  <si>
+    <t>SoilN</t>
+  </si>
+  <si>
+    <t>CurrentCropName</t>
+  </si>
+  <si>
+    <t>CurrentSaleableYield</t>
+  </si>
+  <si>
+    <t>CurrentUnits</t>
+  </si>
+  <si>
+    <t>CurrentFieldLoss</t>
+  </si>
+  <si>
+    <t>CurrentDressingLoss</t>
+  </si>
+  <si>
+    <t>CurrentMoistureContent</t>
+  </si>
+  <si>
+    <t>CurrentEstablishDate</t>
+  </si>
+  <si>
+    <t>CurrentEstablishStage</t>
+  </si>
+  <si>
+    <t>CurrentHarvestDate</t>
+  </si>
+  <si>
+    <t>CurrentHarvestStage</t>
+  </si>
+  <si>
+    <t>CurrentResidueTreatment</t>
+  </si>
+  <si>
+    <t>CurrentEstablishN</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1417,7 @@
                   <c:v>44958</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44959</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>#N/A</c:v>
@@ -1480,31 +1519,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1741427976479302</c:v>
+                  <c:v>2.8251545523323598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8529731258417499</c:v>
+                  <c:v>2.53780388154575</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1644957578447004</c:v>
+                  <c:v>7.2880049100407502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0923271496150999</c:v>
+                  <c:v>2.9535621917708701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3855521678958498</c:v>
+                  <c:v>10.084322113807501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.9491167415605197</c:v>
+                  <c:v>11.0872670773593</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.9640838852432</c:v>
+                  <c:v>12.481960896135</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.91768974534161</c:v>
+                  <c:v>5.1697011973906903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.1211458679747004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1516,22 +1555,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.416845524679601</c:v>
+                  <c:v>20.603856240089101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.905369773059999</c:v>
+                  <c:v>28.447151406630699</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42.2979047986043</c:v>
+                  <c:v>53.649641873682597</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.5262812186348</c:v>
+                  <c:v>23.405551076727701</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34.8524175601178</c:v>
+                  <c:v>43.311922091425899</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33.916105544638199</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1546,28 +1585,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.36853385461654</c:v>
+                  <c:v>4.0467494560163999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.7338784334915398</c:v>
+                  <c:v>4.67751589013925</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.2509561270017</c:v>
+                  <c:v>13.288745453302001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.2783033628279</c:v>
+                  <c:v>17.323396019436199</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22.612540590591902</c:v>
+                  <c:v>28.1443776785114</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.289568708651998</c:v>
+                  <c:v>27.099564152401101</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30.0492178787513</c:v>
+                  <c:v>28.2621717874101</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15.4900614607009</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>#N/A</c:v>
@@ -2060,112 +2099,112 @@
                   <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44978</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Crop Test'!$J$36:$J$67</c:f>
+              <c:f>'Crop Test'!$C$36:$C$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>5.3835246346392154E-2</c:v>
+                  <c:v>0.33522855275841695</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42349796341566553</c:v>
+                  <c:v>0.51082902926001172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74241051060908547</c:v>
+                  <c:v>0.6380181044769937</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97158441773664173</c:v>
+                  <c:v>0.94753996287915065</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98620667777240589</c:v>
+                  <c:v>1.063902167143687</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99825010121612701</c:v>
+                  <c:v>1.4641520076038363</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9997645107001577</c:v>
+                  <c:v>1.9701271928745332</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.99998022615321358</c:v>
+                  <c:v>2.7828050302780944</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.99999467739480674</c:v>
+                  <c:v>3.3028993915675144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99999955297412213</c:v>
+                  <c:v>4.4449302938747888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999982744788474</c:v>
+                  <c:v>4.9313574074792328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99999998396509482</c:v>
+                  <c:v>6.2185302216902407</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.99999999509706305</c:v>
+                  <c:v>6.8764219213981645</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.99999999966658248</c:v>
+                  <c:v>8.3236359770049315</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.99999999994941002</c:v>
+                  <c:v>9.2445077455772076</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.99999999999390354</c:v>
+                  <c:v>10.141371478468965</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.99999999999694933</c:v>
+                  <c:v>10.400099866147247</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99999999999899702</c:v>
+                  <c:v>10.779416313943202</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99999999999960765</c:v>
+                  <c:v>11.065390171261214</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.9999999999999678</c:v>
+                  <c:v>11.685163262837966</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.99738015904888566</c:v>
+                  <c:v>12.101695800803148</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.80681764407083278</c:v>
+                  <c:v>12.49690247240852</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.68298161704994975</c:v>
+                  <c:v>12.665233887387556</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.52925112988692158</c:v>
+                  <c:v>12.808284813701666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.41984096789733027</c:v>
+                  <c:v>12.878405504849862</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2331438202097158</c:v>
+                  <c:v>12.957499478723086</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.0441853961365939E-2</c:v>
+                  <c:v>12.997050336896374</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>13.026556156235843</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>13.042393735799077</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>13.054235569720101</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>13.058838051481922</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3857,8 +3896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3965,10 +4004,10 @@
         <v>44930</v>
       </c>
       <c r="B3" s="46">
-        <v>49.836406040039719</v>
+        <v>49.185394285355294</v>
       </c>
       <c r="C3" s="46">
-        <v>2.1741427976479302</v>
+        <v>2.8251545523323598</v>
       </c>
       <c r="D3" s="46">
         <v>1.7058263792140295E-2</v>
@@ -4019,10 +4058,10 @@
         <v>44931</v>
       </c>
       <c r="B4" s="46">
-        <v>48.569057576600038</v>
+        <v>47.233215066211613</v>
       </c>
       <c r="C4" s="46">
-        <v>1.8529731258417499</v>
+        <v>2.53780388154575</v>
       </c>
       <c r="D4" s="46">
         <v>8.9843765440523332E-3</v>
@@ -4069,10 +4108,10 @@
         <v>44932</v>
       </c>
       <c r="B5" s="46">
-        <v>44.464095354731406</v>
+        <v>41.004743692146931</v>
       </c>
       <c r="C5" s="46">
-        <v>5.1644957578447004</v>
+        <v>7.2880049100407502</v>
       </c>
       <c r="D5" s="46">
         <v>1.6131788997271183E-2</v>
@@ -4119,10 +4158,10 @@
         <v>44933</v>
       </c>
       <c r="B6" s="46">
-        <v>42.687699787947686</v>
+        <v>38.367113083207443</v>
       </c>
       <c r="C6" s="46">
-        <v>2.0923271496150999</v>
+        <v>2.9535621917708701</v>
       </c>
       <c r="D6" s="46">
         <v>4.7442605541209385E-3</v>
@@ -4168,10 +4207,10 @@
         <v>44934</v>
       </c>
       <c r="B7" s="46">
-        <v>36.191510155529706</v>
+        <v>29.172153504877812</v>
       </c>
       <c r="C7" s="46">
-        <v>7.3855521678958498</v>
+        <v>10.084322113807501</v>
       </c>
       <c r="D7" s="46">
         <v>1.3300735968070092E-2</v>
@@ -4215,10 +4254,10 @@
         <v>44935</v>
       </c>
       <c r="B8" s="46">
-        <v>28.101799619542934</v>
+        <v>18.944292633092264</v>
       </c>
       <c r="C8" s="46">
-        <v>8.9491167415605197</v>
+        <v>11.0872670773593</v>
       </c>
       <c r="D8" s="46">
         <v>1.2704817260122748E-2</v>
@@ -4259,10 +4298,10 @@
         <v>44936</v>
       </c>
       <c r="B9" s="46">
-        <v>17.198337561259919</v>
+        <v>7.5229535639174507</v>
       </c>
       <c r="C9" s="46">
-        <v>11.9640838852432</v>
+        <v>12.481960896135</v>
       </c>
       <c r="D9" s="46">
         <v>1.5505015194188732E-2</v>
@@ -4302,10 +4341,10 @@
         <v>44937</v>
       </c>
       <c r="B10" s="46">
-        <v>11.84237423110365</v>
+        <v>2.9149787817120991</v>
       </c>
       <c r="C10" s="46">
-        <v>5.91768974534161</v>
+        <v>5.1697011973906903</v>
       </c>
       <c r="D10" s="46">
         <v>8.098984253538553E-3</v>
@@ -4346,10 +4385,10 @@
         <v>44938</v>
       </c>
       <c r="B11" s="46">
-        <v>3.7813438906561121</v>
+        <v>3.9750943092392625</v>
       </c>
       <c r="C11" s="46">
-        <v>9.1211458679747004</v>
+        <v>0</v>
       </c>
       <c r="D11" s="46">
         <v>1.5173557174284849E-2</v>
@@ -4389,13 +4428,13 @@
         <v>44939</v>
       </c>
       <c r="B12" s="46">
-        <v>4.3404637388442202</v>
+        <v>4.664182341383623</v>
       </c>
       <c r="C12" s="46">
         <v>0</v>
       </c>
       <c r="D12" s="46">
-        <v>0.15756324263885091</v>
+        <v>0.28753142659510328</v>
       </c>
       <c r="E12" s="47">
         <v>0.40155660554925754</v>
@@ -4433,13 +4472,13 @@
         <v>44940</v>
       </c>
       <c r="B13" s="46">
-        <v>5.7338893236937825</v>
+        <v>6.3802642546605481</v>
       </c>
       <c r="C13" s="46">
         <v>0</v>
       </c>
       <c r="D13" s="46">
-        <v>0.39116325101590882</v>
+        <v>0.71381957944327168</v>
       </c>
       <c r="E13" s="47">
         <v>1.0022623338336534</v>
@@ -4474,13 +4513,13 @@
         <v>44941</v>
       </c>
       <c r="B14" s="46">
-        <v>6.4262167910040269</v>
+        <v>7.2313576944623819</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
       </c>
       <c r="D14" s="46">
-        <v>0.19247542502329423</v>
+        <v>0.35124139751488304</v>
       </c>
       <c r="E14" s="47">
         <v>0.49985204228695096</v>
@@ -4515,13 +4554,13 @@
         <v>44942</v>
       </c>
       <c r="B15" s="46">
-        <v>-9.4228932016079483</v>
+        <v>-11.446979788073536</v>
       </c>
       <c r="C15" s="46">
-        <v>17.416845524679601</v>
+        <v>20.603856240089101</v>
       </c>
       <c r="D15" s="46">
-        <v>0.433748348659447</v>
+        <v>0.79153157414500463</v>
       </c>
       <c r="E15" s="47">
         <v>1.1339871834081792</v>
@@ -4557,13 +4596,13 @@
         <v>44943</v>
       </c>
       <c r="B16" s="46">
-        <v>-31.233170960437157</v>
+        <v>-38.551865773361953</v>
       </c>
       <c r="C16" s="46">
-        <v>22.905369773059999</v>
+        <v>28.447151406630699</v>
       </c>
       <c r="D16" s="46">
-        <v>0.29965367163773077</v>
+        <v>0.54682707874921987</v>
       </c>
       <c r="E16" s="47">
         <v>0.79543834259306068</v>
@@ -4603,13 +4642,13 @@
         <v>44944</v>
       </c>
       <c r="B17" s="46">
-        <v>-72.305742552003593</v>
+        <v>-90.701741094612231</v>
       </c>
       <c r="C17" s="46">
-        <v>42.2979047986043</v>
+        <v>53.649641873682597</v>
       </c>
       <c r="D17" s="46">
-        <v>0.33270148487366635</v>
+        <v>0.60713483026812676</v>
       </c>
       <c r="E17" s="47">
         <v>0.8926317221641934</v>
@@ -4649,13 +4688,13 @@
         <v>44945</v>
       </c>
       <c r="B18" s="46">
-        <v>-90.432418410192412</v>
+        <v>-113.61896715913532</v>
       </c>
       <c r="C18" s="46">
-        <v>18.5262812186348</v>
+        <v>23.405551076727701</v>
       </c>
       <c r="D18" s="46">
-        <v>0.10755675420981019</v>
+        <v>0.19627640596843149</v>
       </c>
       <c r="E18" s="47">
         <v>0.29204860623618245</v>
@@ -4695,13 +4734,13 @@
         <v>44946</v>
       </c>
       <c r="B19" s="46">
-        <v>-124.64348912272237</v>
+        <v>-156.14755740100361</v>
       </c>
       <c r="C19" s="46">
-        <v>34.8524175601178</v>
+        <v>43.311922091425899</v>
       </c>
       <c r="D19" s="46">
-        <v>0.17213149122691923</v>
+        <v>0.31411649319671242</v>
       </c>
       <c r="E19" s="47">
         <v>0.46921535636092082</v>
@@ -4741,13 +4780,13 @@
         <v>44947</v>
       </c>
       <c r="B20" s="46">
-        <v>-158.0192105683459</v>
+        <v>-155.4880885001175</v>
       </c>
       <c r="C20" s="46">
-        <v>33.916105544638199</v>
+        <v>0</v>
       </c>
       <c r="D20" s="46">
-        <v>0.144369082960981</v>
+        <v>0.26345388483241483</v>
       </c>
       <c r="E20" s="47">
         <v>0.39601501605370126</v>
@@ -4785,13 +4824,13 @@
         <v>44948</v>
       </c>
       <c r="B21" s="46">
-        <v>-156.72870572467272</v>
+        <v>-153.90584814345007</v>
       </c>
       <c r="C21" s="46">
         <v>0</v>
       </c>
       <c r="D21" s="46">
-        <v>0.23681941288025557</v>
+        <v>0.52855492587450303</v>
       </c>
       <c r="E21" s="47">
         <v>1.0536854307929155</v>
@@ -4828,13 +4867,13 @@
         <v>44949</v>
       </c>
       <c r="B22" s="46">
-        <v>-155.53651065603165</v>
+        <v>-152.4472413269522</v>
       </c>
       <c r="C22" s="46">
         <v>0</v>
       </c>
       <c r="D22" s="46">
-        <v>0.21626257655197786</v>
+        <v>0.48267432440877311</v>
       </c>
       <c r="E22" s="47">
         <v>0.97593249208910526</v>
@@ -4874,13 +4913,13 @@
         <v>44950</v>
       </c>
       <c r="B23" s="46">
-        <v>-153.84929337986486</v>
+        <v>-150.38701868167936</v>
       </c>
       <c r="C23" s="46">
         <v>0</v>
       </c>
       <c r="D23" s="46">
-        <v>0.30279108500109236</v>
+        <v>0.67579645410714551</v>
       </c>
       <c r="E23" s="47">
         <v>1.3844261911657012</v>
@@ -4917,13 +4956,13 @@
         <v>44951</v>
       </c>
       <c r="B24" s="46">
-        <v>-152.75649642159638</v>
+        <v>-149.05630057041878</v>
       </c>
       <c r="C24" s="46">
         <v>0</v>
       </c>
       <c r="D24" s="46">
-        <v>0.19313503243086771</v>
+        <v>0.43105618542295604</v>
       </c>
       <c r="E24" s="47">
         <v>0.89966192583761195</v>
@@ -4963,13 +5002,13 @@
         <v>44952</v>
       </c>
       <c r="B25" s="46">
-        <v>-154.77130424250569</v>
+        <v>-151.4575107645507</v>
       </c>
       <c r="C25" s="46">
-        <v>3.36853385461654</v>
+        <v>4.0467494560163999</v>
       </c>
       <c r="D25" s="46">
-        <v>0.23688249900855446</v>
+        <v>0.52869572718576885</v>
       </c>
       <c r="E25" s="47">
         <v>1.1168435346986798</v>
@@ -5006,13 +5045,13 @@
         <v>44953</v>
       </c>
       <c r="B26" s="46">
-        <v>-157.54424483171368</v>
+        <v>-154.96949767596993</v>
       </c>
       <c r="C26" s="46">
-        <v>3.7338784334915398</v>
+        <v>4.67751589013925</v>
       </c>
       <c r="D26" s="46">
-        <v>0.1660790345353472</v>
+        <v>0.37067016897185362</v>
       </c>
       <c r="E26" s="47">
         <v>0.79485880974816436</v>
@@ -5049,13 +5088,13 @@
         <v>44954</v>
       </c>
       <c r="B27" s="46">
-        <v>-166.15846319105643</v>
+        <v>-166.27609165689356</v>
       </c>
       <c r="C27" s="46">
-        <v>10.2509561270017</v>
+        <v>13.288745453302001</v>
       </c>
       <c r="D27" s="46">
-        <v>0.28039325727909187</v>
+        <v>0.6258069619984985</v>
       </c>
       <c r="E27" s="47">
         <v>1.3563445103798721</v>
@@ -5091,13 +5130,13 @@
         <v>44955</v>
       </c>
       <c r="B28" s="46">
-        <v>-178.10220543388476</v>
+        <v>-181.9875175317415</v>
       </c>
       <c r="C28" s="46">
-        <v>13.2783033628279</v>
+        <v>17.323396019436199</v>
       </c>
       <c r="D28" s="46">
-        <v>0.22518973318161864</v>
+        <v>0.5025987577703056</v>
       </c>
       <c r="E28" s="47">
         <v>1.109371386817938</v>
@@ -5135,13 +5174,13 @@
         <v>44956</v>
       </c>
       <c r="B29" s="46">
-        <v>-199.10074927109085</v>
+        <v>-208.1865399086285</v>
       </c>
       <c r="C29" s="46">
-        <v>22.612540590591902</v>
+        <v>28.1443776785114</v>
       </c>
       <c r="D29" s="46">
-        <v>0.268983834163046</v>
+        <v>0.60034238240163218</v>
       </c>
       <c r="E29" s="47">
         <v>1.3450129192227767</v>
@@ -5179,13 +5218,13 @@
         <v>44957</v>
       </c>
       <c r="B30" s="46">
-        <v>-221.94725522836023</v>
+        <v>-233.55121692957186</v>
       </c>
       <c r="C30" s="46">
-        <v>24.289568708651998</v>
+        <v>27.099564152401101</v>
       </c>
       <c r="D30" s="46">
-        <v>0.23689155168055803</v>
+        <v>0.52871593175566278</v>
       </c>
       <c r="E30" s="47">
         <v>1.206171199702055</v>
@@ -5223,13 +5262,13 @@
         <v>44958</v>
       </c>
       <c r="B31" s="46">
-        <v>-250.13245866180415</v>
+        <v>-259.57750312367887</v>
       </c>
       <c r="C31" s="46">
-        <v>30.0492178787513</v>
+        <v>28.2621717874101</v>
       </c>
       <c r="D31" s="46">
-        <v>0.3018703689227728</v>
+        <v>0.67374151691847128</v>
       </c>
       <c r="E31" s="47">
         <v>1.5621440763845988</v>
@@ -5263,20 +5302,20 @@
       <c r="P31" s="43"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A32" s="28">
-        <v>44959</v>
-      </c>
-      <c r="B32" s="46">
-        <v>-264.39443508593058</v>
-      </c>
-      <c r="C32" s="46">
-        <v>15.4900614607009</v>
-      </c>
-      <c r="D32" s="46">
-        <v>0.19540054837814444</v>
-      </c>
-      <c r="E32" s="46">
-        <v>1.0326844881963502</v>
+      <c r="A32" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D32" s="46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E32" s="46" t="e">
+        <v>#N/A</v>
       </c>
       <c r="F32" s="46"/>
       <c r="H32" s="26">
@@ -5649,6 +5688,12 @@
         <v>#N/A</v>
       </c>
       <c r="F43" s="46"/>
+      <c r="N43" t="s">
+        <v>266</v>
+      </c>
+      <c r="O43">
+        <v>37</v>
+      </c>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="28" t="e">
@@ -5667,6 +5712,12 @@
         <v>#N/A</v>
       </c>
       <c r="F44" s="46"/>
+      <c r="N44" t="s">
+        <v>285</v>
+      </c>
+      <c r="O44">
+        <v>23</v>
+      </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="28" t="e">
@@ -6026,8 +6077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6871C5-A1CC-4FCE-AC7A-C84D2E0677C6}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B35:B36"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6076,7 +6127,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="I2" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="J2" t="s">
         <v>271</v>
@@ -6107,7 +6158,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
       <c r="J3">
         <v>12</v>
@@ -6141,7 +6192,7 @@
         <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="J4" t="s">
         <v>36</v>
@@ -6163,7 +6214,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="J5">
         <v>10</v>
@@ -6185,7 +6236,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="J6">
         <f>F20</f>
@@ -6208,7 +6259,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>260</v>
+        <v>291</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -6227,7 +6278,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="J8" s="26">
         <v>44947</v>
@@ -6243,7 +6294,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
@@ -6259,7 +6310,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="J10" s="26">
         <f>A33</f>
@@ -6276,7 +6327,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="J11" t="s">
         <v>269</v>
@@ -6292,7 +6343,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="J12" t="s">
         <v>252</v>
@@ -6308,7 +6359,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="J13">
         <v>10</v>
@@ -6556,31 +6607,31 @@
         <v>44947</v>
       </c>
       <c r="C36">
-        <v>0.32826590267958394</v>
+        <v>0.33522855275841695</v>
       </c>
       <c r="D36">
-        <v>0.45136561618442778</v>
+        <v>0.46093926004282321</v>
       </c>
       <c r="E36">
-        <v>7.5398574521716917</v>
+        <v>7.699780821169889</v>
       </c>
       <c r="F36">
-        <v>0.83776193913018815</v>
+        <v>0.85553120235221003</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>9.1572509101658923</v>
+        <v>9.3514798363233407</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>5.3835246346392154E-2</v>
+        <v>6.1117457438044233E-2</v>
       </c>
       <c r="K36">
-        <v>7.5548054211533114E-2</v>
+        <v>8.0314105887464238E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6588,31 +6639,31 @@
         <v>44948</v>
       </c>
       <c r="C37">
-        <v>0.48808460900452805</v>
+        <v>0.51082902926001172</v>
       </c>
       <c r="D37">
-        <v>0.67111633738122589</v>
+        <v>0.70238991523251593</v>
       </c>
       <c r="E37">
-        <v>11.210693363072751</v>
+        <v>11.733104265815891</v>
       </c>
       <c r="F37">
-        <v>1.2456325958969727</v>
+        <v>1.3036782517573218</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>13.61552690535548</v>
+        <v>14.250001462065743</v>
       </c>
       <c r="I37">
-        <v>4.4582759951895881</v>
+        <v>4.8985216257424025</v>
       </c>
       <c r="J37">
-        <v>0.42349796341566553</v>
+        <v>0.49688601323733578</v>
       </c>
       <c r="K37">
-        <v>0.16612937996243612</v>
+        <v>0.17660987768080746</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6620,31 +6671,31 @@
         <v>44949</v>
       </c>
       <c r="C38">
-        <v>0.60191329863549692</v>
+        <v>0.6380181044769937</v>
       </c>
       <c r="D38">
-        <v>0.82763078562380821</v>
+        <v>0.87727489365586608</v>
       </c>
       <c r="E38">
-        <v>13.82519607803407</v>
+        <v>14.654478337205948</v>
       </c>
       <c r="F38">
-        <v>1.5361328975593416</v>
+        <v>1.6282753708006612</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>16.790873059852718</v>
+        <v>17.798046706139466</v>
       </c>
       <c r="I38">
-        <v>3.1753461544972374</v>
+        <v>3.5480452440737231</v>
       </c>
       <c r="J38">
-        <v>0.74241051060908547</v>
+        <v>0.80857015829254442</v>
       </c>
       <c r="K38">
-        <v>0.21453388171416449</v>
+        <v>0.22806804321122803</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6652,31 +6703,31 @@
         <v>44950</v>
       </c>
       <c r="C39">
-        <v>0.87458541209486573</v>
+        <v>0.94753996287915065</v>
       </c>
       <c r="D39">
-        <v>1.2025549416304402</v>
+        <v>1.3028674489588317</v>
       </c>
       <c r="E39">
-        <v>20.088133684053943</v>
+        <v>21.763808522380486</v>
       </c>
       <c r="F39">
-        <v>2.2320148537837725</v>
+        <v>2.4182009469311661</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>24.397288891563026</v>
+        <v>26.432416881149638</v>
       </c>
       <c r="I39">
-        <v>7.6064158317103079</v>
+        <v>8.6343701750101722</v>
       </c>
       <c r="J39">
-        <v>0.97158441773664173</v>
+        <v>0.98321335826309841</v>
       </c>
       <c r="K39">
-        <v>0.30211940587545627</v>
+        <v>0.32117901920013953</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -6684,31 +6735,31 @@
         <v>44951</v>
       </c>
       <c r="C40">
-        <v>0.97596911896507899</v>
+        <v>1.063902167143687</v>
       </c>
       <c r="D40">
-        <v>1.3419575385769831</v>
+        <v>1.4628654798225691</v>
       </c>
       <c r="E40">
-        <v>22.416790701229154</v>
+        <v>24.436502901581555</v>
       </c>
       <c r="F40">
-        <v>2.4907545223587957</v>
+        <v>2.7151669890646177</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>27.225471881130012</v>
+        <v>29.678437537612432</v>
       </c>
       <c r="I40">
-        <v>2.8281829895669865</v>
+        <v>3.2460206564627931</v>
       </c>
       <c r="J40">
-        <v>0.98620667777240589</v>
+        <v>0.99226681948646744</v>
       </c>
       <c r="K40">
-        <v>0.32824117997917229</v>
+        <v>0.3489487209248201</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -6716,31 +6767,31 @@
         <v>44952</v>
       </c>
       <c r="C41">
-        <v>1.3217359777221946</v>
+        <v>1.4641520076038363</v>
       </c>
       <c r="D41">
-        <v>1.8173869693680174</v>
+        <v>2.0132090104552747</v>
       </c>
       <c r="E41">
-        <v>30.358623238306656</v>
+        <v>33.629741424650618</v>
       </c>
       <c r="F41">
-        <v>3.3731803598118515</v>
+        <v>3.7366379360722912</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>36.870926545208718</v>
+        <v>40.843740378782016</v>
       </c>
       <c r="I41">
-        <v>9.6454546640787058</v>
+        <v>11.165302841169584</v>
       </c>
       <c r="J41">
-        <v>0.99825010121612701</v>
+        <v>0.99914388713482938</v>
       </c>
       <c r="K41">
-        <v>0.40177980700363841</v>
+        <v>0.42712663218014496</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -6748,31 +6799,31 @@
         <v>44953</v>
       </c>
       <c r="C42">
-        <v>1.7550605016760175</v>
+        <v>1.9701271928745332</v>
       </c>
       <c r="D42">
-        <v>2.4132081898045237</v>
+        <v>2.7089248902024825</v>
       </c>
       <c r="E42">
-        <v>40.311545897871021</v>
+        <v>45.251358961336926</v>
       </c>
       <c r="F42">
-        <v>4.4790606553190031</v>
+        <v>5.0279287734818814</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>48.958875244670566</v>
+        <v>54.958339817895826</v>
       </c>
       <c r="I42">
-        <v>12.087948699461847</v>
+        <v>14.11459943911381</v>
       </c>
       <c r="J42">
-        <v>0.9997645107001577</v>
+        <v>0.99989856999543736</v>
       </c>
       <c r="K42">
-        <v>0.47285385409841441</v>
+        <v>0.5026844821313492</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -6780,31 +6831,31 @@
         <v>44954</v>
       </c>
       <c r="C43">
-        <v>2.4488471902102389</v>
+        <v>2.7828050302780944</v>
       </c>
       <c r="D43">
-        <v>3.3671648865390775</v>
+        <v>3.826356916632379</v>
       </c>
       <c r="E43">
-        <v>56.246958900141408</v>
+        <v>63.917553039199966</v>
       </c>
       <c r="F43">
-        <v>6.2496621000157146</v>
+        <v>7.1019503376888879</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>68.312633076906451</v>
+        <v>77.628665323799339</v>
       </c>
       <c r="I43">
-        <v>19.353757832235885</v>
+        <v>22.670325505903513</v>
       </c>
       <c r="J43">
-        <v>0.99998022615321358</v>
+        <v>0.99999271626123865</v>
       </c>
       <c r="K43">
-        <v>0.56058334471250559</v>
+        <v>0.5959485068923972</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -6812,31 +6863,31 @@
         <v>44955</v>
       </c>
       <c r="C44">
-        <v>2.8943128418798212</v>
+        <v>3.3028993915675144</v>
       </c>
       <c r="D44">
-        <v>3.9796801575847534</v>
+        <v>4.5414866634053324</v>
       </c>
       <c r="E44">
-        <v>66.478748086927126</v>
+        <v>75.863470400066333</v>
       </c>
       <c r="F44">
-        <v>7.3865275652141271</v>
+        <v>8.4292744888962634</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>80.739268651605826</v>
+        <v>92.13713094393546</v>
       </c>
       <c r="I44">
-        <v>12.426635574699375</v>
+        <v>14.508465620136121</v>
       </c>
       <c r="J44">
-        <v>0.99999467739480674</v>
+        <v>0.99999819521272737</v>
       </c>
       <c r="K44">
-        <v>0.60705609489586954</v>
+        <v>0.64535305368135432</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -6844,31 +6895,31 @@
         <v>44956</v>
       </c>
       <c r="C45">
-        <v>3.883658272780584</v>
+        <v>4.4449302938747888</v>
       </c>
       <c r="D45">
-        <v>5.3400301250733015</v>
+        <v>6.1117791540778326</v>
       </c>
       <c r="E45">
-        <v>89.202775952929031</v>
+        <v>102.09449268743653</v>
       </c>
       <c r="F45">
-        <v>9.9114195503254496</v>
+        <v>11.343832520826284</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>108.33788390110836</v>
+        <v>123.99503465621545</v>
       </c>
       <c r="I45">
-        <v>27.598615249502529</v>
+        <v>31.857903712279992</v>
       </c>
       <c r="J45">
-        <v>0.99999955297412213</v>
+        <v>0.99999987035220539</v>
       </c>
       <c r="K45">
-        <v>0.69477090892267568</v>
+        <v>0.73860147596266168</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -6876,31 +6927,31 @@
         <v>44957</v>
       </c>
       <c r="C46">
-        <v>4.3117699299026784</v>
+        <v>4.9313574074792328</v>
       </c>
       <c r="D46">
-        <v>5.928683653616182</v>
+        <v>6.7806164352839451</v>
       </c>
       <c r="E46">
-        <v>99.035965577452146</v>
+        <v>113.26711545303863</v>
       </c>
       <c r="F46">
-        <v>11.003996175272464</v>
+        <v>12.58523505033763</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>120.28041533624346</v>
+        <v>137.56432434613944</v>
       </c>
       <c r="I46">
-        <v>11.942531435135109</v>
+        <v>13.569289689923991</v>
       </c>
       <c r="J46">
-        <v>0.99999982744788474</v>
+        <v>0.99999995287276255</v>
       </c>
       <c r="K46">
-        <v>0.72847848692826955</v>
+        <v>0.7744355423380993</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -6908,31 +6959,31 @@
         <v>44958</v>
       </c>
       <c r="C47">
-        <v>5.4710632139814965</v>
+        <v>6.2185302216902407</v>
       </c>
       <c r="D47">
-        <v>7.5227119192245553</v>
+        <v>8.5504790548240788</v>
       </c>
       <c r="E47">
-        <v>125.66348319613746</v>
+        <v>142.83186602944767</v>
       </c>
       <c r="F47">
-        <v>13.962609244015278</v>
+        <v>15.870207336605302</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>152.61986757335882</v>
+        <v>173.4710826425673</v>
       </c>
       <c r="I47">
-        <v>32.339452237115353</v>
+        <v>35.906758296427853</v>
       </c>
       <c r="J47">
-        <v>0.99999998396509482</v>
+        <v>0.99999999623016689</v>
       </c>
       <c r="K47">
-        <v>0.81261067485120564</v>
+        <v>0.86387532367869146</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -6940,31 +6991,31 @@
         <v>44959</v>
       </c>
       <c r="C48">
-        <v>6.0816390949054302</v>
+        <v>6.8764219213981645</v>
       </c>
       <c r="D48">
-        <v>8.3622537554949652</v>
+        <v>9.4550801419224744</v>
       </c>
       <c r="E48">
-        <v>139.68764796110906</v>
+        <v>157.94281600711406</v>
       </c>
       <c r="F48">
-        <v>15.520849773456568</v>
+        <v>17.549201778568236</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>169.65239058496607</v>
+        <v>191.82351984900293</v>
       </c>
       <c r="I48">
-        <v>17.032523011607253</v>
+        <v>18.352437206435638</v>
       </c>
       <c r="J48">
-        <v>0.99999999509706305</v>
+        <v>0.99999999893033653</v>
       </c>
       <c r="K48">
-        <v>0.85456939617169458</v>
+        <v>0.90848106795902406</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -6972,31 +7023,31 @@
         <v>44960</v>
       </c>
       <c r="C49">
-        <v>7.4793779856040734</v>
+        <v>8.3236359770049315</v>
       </c>
       <c r="D49">
-        <v>10.284144730205599</v>
+        <v>11.444999468381779</v>
       </c>
       <c r="E49">
-        <v>171.79196310684353</v>
+        <v>191.183513846832</v>
       </c>
       <c r="F49">
-        <v>19.087995900760397</v>
+        <v>21.242612649648006</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>208.64348172341363</v>
+        <v>232.19476194186674</v>
       </c>
       <c r="I49">
-        <v>38.991091138447558</v>
+        <v>40.37124209286381</v>
       </c>
       <c r="J49">
-        <v>0.99999999966658248</v>
+        <v>0.99999999993860578</v>
       </c>
       <c r="K49">
-        <v>0.94975886862425551</v>
+        <v>1.0096756976515484</v>
       </c>
     </row>
     <row r="50" spans="2:11">
@@ -7004,31 +7055,31 @@
         <v>44961</v>
       </c>
       <c r="C50">
-        <v>8.4168188368175141</v>
+        <v>9.2445077455772076</v>
       </c>
       <c r="D50">
-        <v>11.573125900624081</v>
+        <v>12.711198150168658</v>
       </c>
       <c r="E50">
-        <v>193.32380765815228</v>
+        <v>212.33478728122648</v>
       </c>
       <c r="F50">
-        <v>21.480423073128037</v>
+        <v>23.592754142358501</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>234.79417546872193</v>
+        <v>257.88324731933085</v>
       </c>
       <c r="I50">
-        <v>26.150693745308303</v>
+        <v>25.688485377464104</v>
       </c>
       <c r="J50">
-        <v>0.99999999994941002</v>
+        <v>0.99999999999172928</v>
       </c>
       <c r="K50">
-        <v>1.0165297786555361</v>
+        <v>1.0806589412892906</v>
       </c>
     </row>
     <row r="51" spans="2:11">
@@ -7036,31 +7087,31 @@
         <v>44962</v>
       </c>
       <c r="C51">
-        <v>9.3751509436163669</v>
+        <v>10.141371478468965</v>
       </c>
       <c r="D51">
-        <v>12.890832547472501</v>
+        <v>13.944385782894825</v>
       </c>
       <c r="E51">
-        <v>215.33549823618836</v>
+        <v>232.93462614608401</v>
       </c>
       <c r="F51">
-        <v>23.926166470687601</v>
+        <v>25.881625127342673</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>261.52764819796488</v>
+        <v>282.90200853479053</v>
       </c>
       <c r="I51">
-        <v>26.733472729242948</v>
+        <v>25.018761215459676</v>
       </c>
       <c r="J51">
-        <v>0.99999999999390354</v>
+        <v>0.99999999999912781</v>
       </c>
       <c r="K51">
-        <v>1.0914593228077525</v>
+        <v>1.1603155175697402</v>
       </c>
     </row>
     <row r="52" spans="2:11">
@@ -7068,31 +7119,31 @@
         <v>44963</v>
       </c>
       <c r="C52">
-        <v>9.6614162956291114</v>
+        <v>10.400099866147247</v>
       </c>
       <c r="D52">
-        <v>13.284447406490028</v>
+        <v>14.300137315952462</v>
       </c>
       <c r="E52">
-        <v>221.91065554023115</v>
+        <v>238.87729380056956</v>
       </c>
       <c r="F52">
-        <v>24.656739504470135</v>
+        <v>26.541921533396625</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>269.51325874682044</v>
+        <v>290.11945251606591</v>
       </c>
       <c r="I52">
-        <v>7.9856105488555613</v>
+        <v>7.2174439812753803</v>
       </c>
       <c r="J52">
-        <v>0.99999999999694933</v>
+        <v>0.99999999999958233</v>
       </c>
       <c r="K52">
-        <v>1.115974549403679</v>
+        <v>1.1863773205536725</v>
       </c>
     </row>
     <row r="53" spans="2:11">
@@ -7100,31 +7151,31 @@
         <v>44964</v>
       </c>
       <c r="C53">
-        <v>10.090221512713546</v>
+        <v>10.779416313943202</v>
       </c>
       <c r="D53">
-        <v>13.874054579981122</v>
+        <v>14.821697431671897</v>
       </c>
       <c r="E53">
-        <v>231.75977537013921</v>
+        <v>247.58971846088284</v>
       </c>
       <c r="F53">
-        <v>25.751086152237701</v>
+        <v>27.509968717875878</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>281.47513761507156</v>
+        <v>300.70080092437382</v>
       </c>
       <c r="I53">
-        <v>11.961878868251119</v>
+        <v>10.581348408307917</v>
       </c>
       <c r="J53">
-        <v>0.99999999999899702</v>
+        <v>0.99999999999987188</v>
       </c>
       <c r="K53">
-        <v>1.1553615573806109</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -7132,31 +7183,31 @@
         <v>44965</v>
       </c>
       <c r="C54">
-        <v>10.421396655229284</v>
+        <v>11.065390171261214</v>
       </c>
       <c r="D54">
-        <v>14.329420400940263</v>
+        <v>15.214911485484166</v>
       </c>
       <c r="E54">
-        <v>239.36645442479758</v>
+        <v>254.15818049615598</v>
       </c>
       <c r="F54">
-        <v>26.596272713866409</v>
+        <v>28.239797832906227</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>290.71354419483356</v>
+        <v>308.67827998580765</v>
       </c>
       <c r="I54">
-        <v>9.2384065797619996</v>
+        <v>7.9774790614338258</v>
       </c>
       <c r="J54">
-        <v>0.99999999999960765</v>
+        <v>0.9999999999999527</v>
       </c>
       <c r="K54">
-        <v>1.1886039617155066</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="55" spans="2:11">
@@ -7164,28 +7215,28 @@
         <v>44966</v>
       </c>
       <c r="C55">
-        <v>11.166380440125588</v>
+        <v>11.685163262837966</v>
       </c>
       <c r="D55">
-        <v>15.35377310517268</v>
+        <v>16.067099486402199</v>
       </c>
       <c r="E55">
-        <v>256.47780073413452</v>
+        <v>268.39359369330947</v>
       </c>
       <c r="F55">
-        <v>28.497533414903845</v>
+        <v>29.821510410367726</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>311.4954876943367</v>
+        <v>325.96736685291739</v>
       </c>
       <c r="I55">
-        <v>20.781943499503143</v>
+        <v>17.289086867109745</v>
       </c>
       <c r="J55">
-        <v>0.9999999999999678</v>
+        <v>0.99960599385063065</v>
       </c>
       <c r="K55">
         <v>1.2</v>
@@ -7196,28 +7247,28 @@
         <v>44967</v>
       </c>
       <c r="C56">
-        <v>11.692727695360439</v>
+        <v>12.101695800803148</v>
       </c>
       <c r="D56">
-        <v>16.077500581120599</v>
+        <v>16.639831726104326</v>
       </c>
       <c r="E56">
-        <v>268.56733925281003</v>
+        <v>277.96082542469725</v>
       </c>
       <c r="F56">
-        <v>29.840815472534455</v>
+        <v>30.884536158299703</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>326.17838300182558</v>
+        <v>337.58688910990446</v>
       </c>
       <c r="I56">
-        <v>14.682895307488877</v>
+        <v>11.619522256987068</v>
       </c>
       <c r="J56">
-        <v>0.99738015904888566</v>
+        <v>0.85679685776854186</v>
       </c>
       <c r="K56">
         <v>1.2</v>
@@ -7228,28 +7279,28 @@
         <v>44968</v>
       </c>
       <c r="C57">
-        <v>12.217902966359345</v>
+        <v>12.49690247240852</v>
       </c>
       <c r="D57">
-        <v>16.799616578744097</v>
+        <v>17.183240899561714</v>
       </c>
       <c r="E57">
-        <v>280.6299587585662</v>
+        <v>287.03822866313317</v>
       </c>
       <c r="F57">
-        <v>31.181106528729583</v>
+        <v>31.893136518125917</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>340.8285848323992</v>
+        <v>348.61150855322938</v>
       </c>
       <c r="I57">
-        <v>14.650201830573621</v>
+        <v>11.024619443324923</v>
       </c>
       <c r="J57">
-        <v>0.80681764407083278</v>
+        <v>0.65421244754302488</v>
       </c>
       <c r="K57">
         <v>1.2</v>
@@ -7260,28 +7311,28 @@
         <v>44969</v>
       </c>
       <c r="C58">
-        <v>12.452025304349887</v>
+        <v>12.665233887387556</v>
       </c>
       <c r="D58">
-        <v>17.121534793481093</v>
+        <v>17.414696595157888</v>
       </c>
       <c r="E58">
-        <v>286.00745620928643</v>
+        <v>290.90459085093289</v>
       </c>
       <c r="F58">
-        <v>31.778606245476279</v>
+        <v>32.322732316770328</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>347.35962255259375</v>
+        <v>353.30725365024875</v>
       </c>
       <c r="I58">
-        <v>6.5310377201945471</v>
+        <v>4.695745097019369</v>
       </c>
       <c r="J58">
-        <v>0.68298161704994975</v>
+        <v>0.52256405645422088</v>
       </c>
       <c r="K58">
         <v>1.2</v>
@@ -7292,28 +7343,28 @@
         <v>44970</v>
       </c>
       <c r="C59">
-        <v>12.657982785372736</v>
+        <v>12.808284813701666</v>
       </c>
       <c r="D59">
-        <v>17.404726329887506</v>
+        <v>17.611391618839786</v>
       </c>
       <c r="E59">
-        <v>290.73804210152997</v>
+        <v>294.19029181471012</v>
       </c>
       <c r="F59">
-        <v>32.304226900170008</v>
+        <v>32.687810201634463</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>353.10497811696024</v>
+        <v>357.29777844888605</v>
       </c>
       <c r="I59">
-        <v>5.7453555643664913</v>
+        <v>3.9905247986372956</v>
       </c>
       <c r="J59">
-        <v>0.52925112988692158</v>
+        <v>0.3591352725761835</v>
       </c>
       <c r="K59">
         <v>1.2</v>
@@ -7324,28 +7375,28 @@
         <v>44971</v>
       </c>
       <c r="C60">
-        <v>12.762144586383007</v>
+        <v>12.878405504849862</v>
       </c>
       <c r="D60">
-        <v>17.547948806276633</v>
+        <v>17.707807569168558</v>
       </c>
       <c r="E60">
-        <v>293.13050846848466</v>
+        <v>295.80087643952021</v>
       </c>
       <c r="F60">
-        <v>32.570056496498303</v>
+        <v>32.866764048835584</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>356.01065835764263</v>
+        <v>359.25385356237422</v>
       </c>
       <c r="I60">
-        <v>2.9056802406823863</v>
+        <v>1.9560751134881684</v>
       </c>
       <c r="J60">
-        <v>0.41984096789733027</v>
+        <v>0.24282282182010295</v>
       </c>
       <c r="K60">
         <v>1.2</v>
@@ -7356,28 +7407,28 @@
         <v>44972</v>
       </c>
       <c r="C61">
-        <v>12.883318601532229</v>
+        <v>12.957499478723086</v>
       </c>
       <c r="D61">
-        <v>17.71456307710681</v>
+        <v>17.816561783244239</v>
       </c>
       <c r="E61">
-        <v>295.91372412894333</v>
+        <v>297.61756615192081</v>
       </c>
       <c r="F61">
-        <v>32.879302680993717</v>
+        <v>33.068618461324547</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>359.39090848857614</v>
+        <v>361.46024587521276</v>
       </c>
       <c r="I61">
-        <v>3.3802501309335184</v>
+        <v>2.2063923128385454</v>
       </c>
       <c r="J61">
-        <v>0.2331438202097158</v>
+        <v>4.4347630833892593E-2</v>
       </c>
       <c r="K61">
         <v>1.2</v>
@@ -7388,28 +7439,28 @@
         <v>44973</v>
       </c>
       <c r="C62">
-        <v>12.946076762605795</v>
+        <v>12.997050336896374</v>
       </c>
       <c r="D62">
-        <v>17.800855548582966</v>
+        <v>17.870944213232512</v>
       </c>
       <c r="E62">
-        <v>297.35520064110182</v>
+        <v>298.52599992558856</v>
       </c>
       <c r="F62">
-        <v>33.039466737900213</v>
+        <v>33.169555547287622</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>361.14159969019079</v>
+        <v>362.56355002300506</v>
       </c>
       <c r="I62">
-        <v>1.750691201614643</v>
+        <v>1.1033041477923007</v>
       </c>
       <c r="J62">
-        <v>8.0441853961365939E-2</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>1.2</v>
@@ -7420,25 +7471,25 @@
         <v>44974</v>
       </c>
       <c r="C63">
-        <v>12.994427297901929</v>
+        <v>13.026556156235843</v>
       </c>
       <c r="D63">
-        <v>17.86733753461515</v>
+        <v>17.911514714824282</v>
       </c>
       <c r="E63">
-        <v>298.46575199868488</v>
+        <v>299.20371171354196</v>
       </c>
       <c r="F63">
-        <v>33.162861333187223</v>
+        <v>33.244856857060235</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>362.4903781643892</v>
+        <v>363.38663944166234</v>
       </c>
       <c r="I63">
-        <v>1.3487784741984115</v>
+        <v>0.82308941865727547</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -7452,25 +7503,25 @@
         <v>44975</v>
       </c>
       <c r="C64">
-        <v>13.021253506266081</v>
+        <v>13.042393735799077</v>
       </c>
       <c r="D64">
-        <v>17.904223571115857</v>
+        <v>17.933291386723727</v>
       </c>
       <c r="E64">
-        <v>299.08191647204899</v>
+        <v>299.56748111913504</v>
       </c>
       <c r="F64">
-        <v>33.231324052449892</v>
+        <v>33.285275679903897</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>363.23871760188086</v>
+        <v>363.82844192156176</v>
       </c>
       <c r="I64">
-        <v>0.74833943749166565</v>
+        <v>0.44180247989942245</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -7484,25 +7535,25 @@
         <v>44976</v>
       </c>
       <c r="C65">
-        <v>13.042003028798327</v>
+        <v>13.054235569720101</v>
       </c>
       <c r="D65">
-        <v>17.932754164597693</v>
+        <v>17.949573908365135</v>
       </c>
       <c r="E65">
-        <v>299.55850706771156</v>
+        <v>299.83947324200852</v>
       </c>
       <c r="F65">
-        <v>33.28427856307907</v>
+        <v>33.315497026889844</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>363.81754282418666</v>
+        <v>364.15877974698361</v>
       </c>
       <c r="I65">
-        <v>0.57882522230579525</v>
+        <v>0.33033782542185008</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -7516,25 +7567,25 @@
         <v>44977</v>
       </c>
       <c r="C66">
-        <v>13.050338820683718</v>
+        <v>13.058838051481922</v>
       </c>
       <c r="D66">
-        <v>17.944215878440108</v>
+        <v>17.95590232078764</v>
       </c>
       <c r="E66">
-        <v>299.74996978757912</v>
+        <v>299.94518649497542</v>
       </c>
       <c r="F66">
-        <v>33.305552198619907</v>
+        <v>33.327242943886155</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>364.05007668532284</v>
+        <v>364.28716981113115</v>
       </c>
       <c r="I66">
-        <v>0.2325338611361758</v>
+        <v>0.1283900641475384</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -7544,35 +7595,35 @@
       </c>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="28">
-        <v>44978</v>
-      </c>
-      <c r="C67">
-        <v>13.058838051481922</v>
-      </c>
-      <c r="D67">
-        <v>17.95590232078764</v>
-      </c>
-      <c r="E67">
-        <v>299.94518649497542</v>
-      </c>
-      <c r="F67">
-        <v>33.327242943886155</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>364.28716981113115</v>
-      </c>
-      <c r="I67">
-        <v>0.23709312580831465</v>
-      </c>
-      <c r="J67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <v>1.2</v>
+      <c r="B67" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J67" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K67" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress with getting fert schedulling working
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8C9DBD-1890-470A-AD8F-03365C47CAC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8762DECC-52BB-4414-A7E9-201FF4FA4C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
   <sheets>
     <sheet name="NBalance Test" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="301">
   <si>
     <t>EndUse</t>
   </si>
@@ -938,6 +938,15 @@
   </si>
   <si>
     <t>CurrentEstablishN</t>
+  </si>
+  <si>
+    <t>Soil Mineral N Tests</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1238,6 +1247,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3519,16 +3531,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3894,10 +3906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B2"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3912,16 +3924,19 @@
     <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="str">
-        <f t="array" ref="A1:E61">_xll.GetDailyNBalance(I3:I34,N2:O39)</f>
+        <f t="array" ref="A1:E61">_xll.GetDailyNBalance(I3:I34,N2:O43,R2:S14)</f>
         <v>Date</v>
       </c>
       <c r="B1" s="28" t="str">
@@ -3946,20 +3961,24 @@
       <c r="P1" t="s">
         <v>276</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="S1" s="48"/>
+      <c r="U1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="V1" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1">
       <c r="A2" s="28">
         <v>44929</v>
       </c>
@@ -3987,19 +4006,25 @@
         <v>50</v>
       </c>
       <c r="R2" t="s">
+        <v>299</v>
+      </c>
+      <c r="S2" t="s">
+        <v>300</v>
+      </c>
+      <c r="U2" t="s">
         <v>32</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>63</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>253</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1">
       <c r="A3" s="28">
         <v>44930</v>
       </c>
@@ -4040,20 +4065,20 @@
       <c r="P3" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>123</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>49</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>249</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:24">
       <c r="A4" s="28">
         <v>44931</v>
       </c>
@@ -4096,14 +4121,14 @@
         <v>5</v>
       </c>
       <c r="P4" s="43"/>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>43</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:24">
       <c r="A5" s="28">
         <v>44932</v>
       </c>
@@ -4146,14 +4171,14 @@
         <v>t/ha</v>
       </c>
       <c r="P5" s="43"/>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>55</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:24">
       <c r="A6" s="28">
         <v>44933</v>
       </c>
@@ -4195,14 +4220,14 @@
         <v>50</v>
       </c>
       <c r="P6" s="43"/>
-      <c r="S6" t="s">
+      <c r="V6" t="s">
         <v>34</v>
       </c>
-      <c r="T6" t="s">
+      <c r="W6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:24">
       <c r="A7" s="28">
         <v>44934</v>
       </c>
@@ -4245,11 +4270,11 @@
         <v>0</v>
       </c>
       <c r="P7" s="43"/>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1">
+    <row r="8" spans="1:24" ht="15.75" thickBot="1">
       <c r="A8" s="28">
         <v>44935</v>
       </c>
@@ -4293,7 +4318,7 @@
       </c>
       <c r="P8" s="43"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1">
+    <row r="9" spans="1:24" ht="15.75" thickBot="1">
       <c r="A9" s="28">
         <v>44936</v>
       </c>
@@ -4336,7 +4361,7 @@
         <v>44929</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1">
       <c r="A10" s="28">
         <v>44937</v>
       </c>
@@ -4380,7 +4405,7 @@
       </c>
       <c r="P10" s="43"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1">
       <c r="A11" s="28">
         <v>44938</v>
       </c>
@@ -4423,7 +4448,7 @@
         <v>44938</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:24">
       <c r="A12" s="28">
         <v>44939</v>
       </c>
@@ -4467,7 +4492,7 @@
       </c>
       <c r="P12" s="43"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:24">
       <c r="A13" s="28">
         <v>44940</v>
       </c>
@@ -4503,17 +4528,17 @@
         <v>PriorResidueTreatment</v>
       </c>
       <c r="O13" s="32" t="str">
-        <f>IF(P13="",T2,P13)</f>
+        <f>IF(P13="",W2,P13)</f>
         <v>None</v>
       </c>
       <c r="P13" s="43"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1">
       <c r="A14" s="28">
         <v>44941</v>
       </c>
       <c r="B14" s="46">
-        <v>7.2313576944623819</v>
+        <v>44.231357694462382</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
@@ -4549,12 +4574,12 @@
       </c>
       <c r="P14" s="43"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1">
+    <row r="15" spans="1:24" ht="15.75" thickBot="1">
       <c r="A15" s="28">
         <v>44942</v>
       </c>
       <c r="B15" s="46">
-        <v>-11.446979788073536</v>
+        <v>25.553020211926466</v>
       </c>
       <c r="C15" s="46">
         <v>20.603856240089101</v>
@@ -4591,12 +4616,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:24">
       <c r="A16" s="28">
         <v>44943</v>
       </c>
       <c r="B16" s="46">
-        <v>-38.551865773361953</v>
+        <v>-1.5518657733619534</v>
       </c>
       <c r="C16" s="46">
         <v>28.447151406630699</v>
@@ -4642,7 +4667,7 @@
         <v>44944</v>
       </c>
       <c r="B17" s="46">
-        <v>-90.701741094612231</v>
+        <v>-53.701741094612231</v>
       </c>
       <c r="C17" s="46">
         <v>53.649641873682597</v>
@@ -4688,7 +4713,7 @@
         <v>44945</v>
       </c>
       <c r="B18" s="46">
-        <v>-113.61896715913532</v>
+        <v>-76.618967159135323</v>
       </c>
       <c r="C18" s="46">
         <v>23.405551076727701</v>
@@ -4734,7 +4759,7 @@
         <v>44946</v>
       </c>
       <c r="B19" s="46">
-        <v>-156.14755740100361</v>
+        <v>-119.14755740100361</v>
       </c>
       <c r="C19" s="46">
         <v>43.311922091425899</v>
@@ -4780,7 +4805,7 @@
         <v>44947</v>
       </c>
       <c r="B20" s="46">
-        <v>-155.4880885001175</v>
+        <v>-118.4880885001175</v>
       </c>
       <c r="C20" s="46">
         <v>0</v>
@@ -4824,7 +4849,7 @@
         <v>44948</v>
       </c>
       <c r="B21" s="46">
-        <v>-153.90584814345007</v>
+        <v>-116.90584814345007</v>
       </c>
       <c r="C21" s="46">
         <v>0</v>
@@ -4867,7 +4892,7 @@
         <v>44949</v>
       </c>
       <c r="B22" s="46">
-        <v>-152.4472413269522</v>
+        <v>-115.4472413269522</v>
       </c>
       <c r="C22" s="46">
         <v>0</v>
@@ -4913,7 +4938,7 @@
         <v>44950</v>
       </c>
       <c r="B23" s="46">
-        <v>-150.38701868167936</v>
+        <v>-113.38701868167936</v>
       </c>
       <c r="C23" s="46">
         <v>0</v>
@@ -4956,7 +4981,7 @@
         <v>44951</v>
       </c>
       <c r="B24" s="46">
-        <v>-149.05630057041878</v>
+        <v>-112.05630057041878</v>
       </c>
       <c r="C24" s="46">
         <v>0</v>
@@ -5002,7 +5027,7 @@
         <v>44952</v>
       </c>
       <c r="B25" s="46">
-        <v>-151.4575107645507</v>
+        <v>-114.4575107645507</v>
       </c>
       <c r="C25" s="46">
         <v>4.0467494560163999</v>
@@ -5033,7 +5058,7 @@
         <v>CurrentResidueTreatment</v>
       </c>
       <c r="O25" s="19" t="str">
-        <f>IF(P25="",T2,P25)</f>
+        <f>IF(P25="",W2,P25)</f>
         <v>Incorporated</v>
       </c>
       <c r="P25" s="43" t="s">
@@ -5045,7 +5070,7 @@
         <v>44953</v>
       </c>
       <c r="B26" s="46">
-        <v>-154.96949767596993</v>
+        <v>-117.96949767596993</v>
       </c>
       <c r="C26" s="46">
         <v>4.67751589013925</v>
@@ -5088,7 +5113,7 @@
         <v>44954</v>
       </c>
       <c r="B27" s="46">
-        <v>-166.27609165689356</v>
+        <v>-129.27609165689356</v>
       </c>
       <c r="C27" s="46">
         <v>13.288745453302001</v>
@@ -5130,7 +5155,7 @@
         <v>44955</v>
       </c>
       <c r="B28" s="46">
-        <v>-181.9875175317415</v>
+        <v>-144.9875175317415</v>
       </c>
       <c r="C28" s="46">
         <v>17.323396019436199</v>
@@ -5174,7 +5199,7 @@
         <v>44956</v>
       </c>
       <c r="B29" s="46">
-        <v>-208.1865399086285</v>
+        <v>-171.1865399086285</v>
       </c>
       <c r="C29" s="46">
         <v>28.1443776785114</v>
@@ -5218,7 +5243,7 @@
         <v>44957</v>
       </c>
       <c r="B30" s="46">
-        <v>-233.55121692957186</v>
+        <v>-196.55121692957186</v>
       </c>
       <c r="C30" s="46">
         <v>27.099564152401101</v>
@@ -5262,7 +5287,7 @@
         <v>44958</v>
       </c>
       <c r="B31" s="46">
-        <v>-259.57750312367887</v>
+        <v>-222.57750312367887</v>
       </c>
       <c r="C31" s="46">
         <v>28.2621717874101</v>
@@ -5535,7 +5560,7 @@
         <v>FollowingResidueTreatment</v>
       </c>
       <c r="O37" s="32" t="str">
-        <f>IF(P37="",T2,P37)</f>
+        <f>IF(P37="",W2,P37)</f>
         <v>None</v>
       </c>
       <c r="P37" s="43"/>
@@ -6026,20 +6051,23 @@
       <c r="F61" s="46"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R1:S1"/>
+  </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O13:P13 O37:P37 O25:P25" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
-      <formula1>$T$2:$T$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:P25 O37:P37 O13:P13" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
+      <formula1>$W$2:$W$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P12 P36 P24" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
-      <formula1>$S$2:$S$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P24 P36 P12" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
+      <formula1>$V$2:$V$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P10 P34 P22" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
-      <formula1>$R$2:$R$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P22 P34 P10" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
+      <formula1>$U$2:$U$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5 P29 P17" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
-      <formula1>$U$2:$U$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P17 P29 P5" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
+      <formula1>$X$2:$X$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P8 P18:P20 P30:P32" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P18:P20 P30:P32 P6:P8" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>
@@ -6065,7 +6093,7 @@
           <x14:formula1>
             <xm:f>CropCoefficients!$K$3:$K$78</xm:f>
           </x14:formula1>
-          <xm:sqref>O3:P3 O15:P15 O27:P27</xm:sqref>
+          <xm:sqref>O15:P15 O27:P27 O3:P3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
few code tidy ups and moving toward getting it working with the excel prototype
</commit_message>
<xml_diff>
--- a/modelCsharp/Test2.xlsx
+++ b/modelCsharp/Test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\SVS\modelCsharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972D9882-ECDE-4051-8ADC-8C09A939D8FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4154C7C-E217-4FE1-9070-2DC14978ABEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{1F14EB4F-D50B-4F9D-800C-255669009A65}"/>
   </bookViews>
   <sheets>
     <sheet name="NBalance Test" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="Type">CropCoefficients!$E$3:$E$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1564,64 +1563,64 @@
                   <c:v>4.4704319228004765</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-87.626972327845209</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.024121111956646</c:v>
+                  <c:v>137.85109343980184</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.332794344830148</c:v>
+                  <c:v>122.35976667267533</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>74.769689993112422</c:v>
+                  <c:v>100.79666232095761</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.971551746940349</c:v>
+                  <c:v>59.998524074785536</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96.73359554051018</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>62.664509829950077</c:v>
+                  <c:v>122.93091428943993</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.407873186198003</c:v>
+                  <c:v>89.674277645687852</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.990113542865458</c:v>
+                  <c:v>91.256518002355278</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.448720359363335</c:v>
+                  <c:v>92.715124818853155</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>34.508943004636137</c:v>
+                  <c:v>94.775347464125986</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35.839661115896718</c:v>
+                  <c:v>96.106065575386566</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34.116666523164668</c:v>
+                  <c:v>94.383070982654488</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31.548317068393146</c:v>
+                  <c:v>91.814721527882966</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.279512413769794</c:v>
+                  <c:v>83.545916873259642</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.613179195530222</c:v>
+                  <c:v>71.87958365502007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-9.0540060934372377</c:v>
+                  <c:v>51.212398366052582</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-31.608687670631639</c:v>
+                  <c:v>28.65771678885821</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-59.422019956079851</c:v>
+                  <c:v>0.84438450341001214</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-73.443284360329358</c:v>
+                  <c:v>-13.176879900839495</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>#N/A</c:v>
@@ -2114,7 +2113,7 @@
                   <c:v>44977</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>#N/A</c:v>
+                  <c:v>44978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2126,100 +2125,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.33522855275841695</c:v>
+                  <c:v>0.32826590267958394</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51082902926001172</c:v>
+                  <c:v>0.48808460900452805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6380181044769937</c:v>
+                  <c:v>0.60191329863549692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.94753996287915065</c:v>
+                  <c:v>0.87458541209486573</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.063902167143687</c:v>
+                  <c:v>0.97596911896507899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4641520076038363</c:v>
+                  <c:v>1.3217359777221946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9701271928745332</c:v>
+                  <c:v>1.7550605016760175</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7828050302780944</c:v>
+                  <c:v>2.4488471902102389</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.3028993915675144</c:v>
+                  <c:v>2.8943128418798212</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4449302938747888</c:v>
+                  <c:v>3.883658272780584</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9313574074792328</c:v>
+                  <c:v>4.3117699299026784</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.2185302216902407</c:v>
+                  <c:v>5.4710632139814965</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.8764219213981645</c:v>
+                  <c:v>6.0816390949054302</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.3236359770049315</c:v>
+                  <c:v>7.4793779856040734</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.2445077455772076</c:v>
+                  <c:v>8.4168188368175141</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.141371478468965</c:v>
+                  <c:v>9.3751509436163669</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.400099866147247</c:v>
+                  <c:v>9.6614162956291114</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.779416313943202</c:v>
+                  <c:v>10.090221512713546</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.065390171261214</c:v>
+                  <c:v>10.421396655229284</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.685163262837966</c:v>
+                  <c:v>11.166380440125588</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.101695800803148</c:v>
+                  <c:v>11.692727695360439</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.49690247240852</c:v>
+                  <c:v>12.217902966359345</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.665233887387556</c:v>
+                  <c:v>12.452025304349887</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.808284813701666</c:v>
+                  <c:v>12.657982785372736</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.878405504849862</c:v>
+                  <c:v>12.762144586383007</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.957499478723086</c:v>
+                  <c:v>12.883318601532229</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.997050336896374</c:v>
+                  <c:v>12.946076762605795</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.026556156235843</c:v>
+                  <c:v>12.994427297901929</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.042393735799077</c:v>
+                  <c:v>13.021253506266081</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.054235569720101</c:v>
+                  <c:v>13.042003028798327</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>13.050338820683718</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>13.058838051481922</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3534,16 +3533,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3909,10 +3908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7E2-E497-4AE2-9FEE-13422347FF1E}">
-  <dimension ref="A1:X61"/>
+  <dimension ref="A1:AD61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+      <selection activeCell="A61" sqref="A1:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3920,26 +3919,26 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" customWidth="1"/>
-    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+    <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:30" ht="15.75" thickBot="1">
       <c r="A1" t="str">
-        <f t="array" ref="A1:F61">_xll.GetDailyNBalance(H2:I34,N2:O43,R2:S14)</f>
+        <f t="array" ref="A1:F61">_xll.GetDailyNBalance(N2:O34,T2:U43,X2:Y14)</f>
         <v>Date</v>
       </c>
       <c r="B1" s="28" t="str">
@@ -3957,34 +3956,34 @@
       <c r="F1" t="str">
         <v>FertiliserN</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" t="s">
+      <c r="T1" s="3"/>
+      <c r="U1" t="s">
         <v>277</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>276</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="S1" s="48"/>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="48"/>
+      <c r="AA1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1">
+    <row r="2" spans="1:30" ht="15.75" thickBot="1">
       <c r="A2" s="28">
         <v>44929</v>
       </c>
@@ -4003,39 +4002,45 @@
       <c r="F2" s="46">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="N2" t="s">
         <v>299</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>301</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="T2" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="O2" s="41">
-        <f>IF(P2="",50,P2)</f>
+      <c r="U2" s="41">
+        <f>IF(V2="",50,V2)</f>
         <v>50</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>299</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>300</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>32</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>63</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AC2" t="s">
         <v>253</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AD2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1">
+    <row r="3" spans="1:30" ht="15.75" thickBot="1">
       <c r="A3" s="28">
         <v>44930</v>
       </c>
@@ -4054,51 +4059,57 @@
       <c r="F3" s="46">
         <v>0</v>
       </c>
-      <c r="H3" s="26">
-        <f>O9</f>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="N3" s="26">
+        <f>U9</f>
         <v>44929</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="R3" t="s">
         <v>272</v>
       </c>
-      <c r="M3" t="s">
+      <c r="S3" t="s">
         <v>270</v>
       </c>
-      <c r="N3" s="29" t="str">
-        <f>L3&amp;M3</f>
+      <c r="T3" s="29" t="str">
+        <f>R3&amp;S3</f>
         <v>PriorCropName</v>
       </c>
-      <c r="O3" s="30" t="str">
-        <f>P3</f>
+      <c r="U3" s="30" t="str">
+        <f>V3</f>
         <v>Annual ryegrass Fodder General</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="V3" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="R3" s="26">
-        <f>P21-1</f>
+      <c r="X3" s="26">
+        <f>V21-1</f>
         <v>44940</v>
       </c>
-      <c r="S3">
+      <c r="Y3">
         <v>100</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AA3" t="s">
         <v>123</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AB3" t="s">
         <v>49</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AC3" t="s">
         <v>249</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AD3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:30">
       <c r="A4" s="28">
         <v>44931</v>
       </c>
@@ -4117,40 +4128,52 @@
       <c r="F4" s="46">
         <v>0</v>
       </c>
-      <c r="H4" s="26">
-        <f>H3+1</f>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="N4" s="26">
+        <f>N3+1</f>
         <v>44930</v>
       </c>
-      <c r="I4">
+      <c r="O4">
         <v>14.387874318606862</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>7</v>
       </c>
-      <c r="L4" t="str">
-        <f>L3</f>
+      <c r="R4" t="str">
+        <f>R3</f>
         <v>Prior</v>
       </c>
-      <c r="M4" t="s">
+      <c r="S4" t="s">
         <v>256</v>
       </c>
-      <c r="N4" s="31" t="str">
-        <f t="shared" ref="N4:N14" si="0">L4&amp;M4</f>
+      <c r="T4" s="31" t="str">
+        <f t="shared" ref="T4:T14" si="0">R4&amp;S4</f>
         <v>PriorSaleableYield</v>
       </c>
-      <c r="O4" s="32">
-        <f>IF(P4="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K4,FALSE),P4)</f>
+      <c r="U4" s="32">
+        <f>IF(V4="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q4,FALSE),V4)</f>
         <v>5</v>
       </c>
-      <c r="P4" s="43"/>
-      <c r="V4" t="s">
+      <c r="V4" s="43"/>
+      <c r="X4" s="26">
+        <v>44945</v>
+      </c>
+      <c r="Y4">
+        <v>120</v>
+      </c>
+      <c r="AB4" t="s">
         <v>43</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AC4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:30">
       <c r="A5" s="28">
         <v>44932</v>
       </c>
@@ -4169,40 +4192,46 @@
       <c r="F5" s="46">
         <v>0</v>
       </c>
-      <c r="H5" s="26">
-        <f t="shared" ref="H5:H34" si="1">H4+1</f>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="N5" s="26">
+        <f t="shared" ref="N5:N34" si="1">N4+1</f>
         <v>44931</v>
       </c>
-      <c r="I5">
+      <c r="O5">
         <v>7.6885371447735746</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>8</v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" ref="L5:L14" si="2">L4</f>
+      <c r="R5" t="str">
+        <f t="shared" ref="R5:R14" si="2">R4</f>
         <v>Prior</v>
       </c>
-      <c r="M5" t="s">
+      <c r="S5" t="s">
         <v>257</v>
       </c>
-      <c r="N5" s="31" t="str">
+      <c r="T5" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorUnits</v>
       </c>
-      <c r="O5" s="32" t="str">
-        <f>IF(P5="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K5,FALSE),P5)</f>
+      <c r="U5" s="32" t="str">
+        <f>IF(V5="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q5,FALSE),V5)</f>
         <v>t/ha</v>
       </c>
-      <c r="P5" s="43"/>
-      <c r="V5" t="s">
+      <c r="V5" s="43"/>
+      <c r="AB5" t="s">
         <v>55</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AC5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:30">
       <c r="A6" s="28">
         <v>44933</v>
       </c>
@@ -4221,39 +4250,45 @@
       <c r="F6" s="46">
         <v>0</v>
       </c>
-      <c r="H6" s="26">
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="N6" s="26">
         <f t="shared" si="1"/>
         <v>44932</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>13.912023293050638</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>12</v>
       </c>
-      <c r="L6" t="str">
+      <c r="R6" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M6" t="s">
+      <c r="S6" t="s">
         <v>258</v>
       </c>
-      <c r="N6" s="31" t="str">
+      <c r="T6" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorFieldLoss</v>
       </c>
-      <c r="O6" s="32">
+      <c r="U6" s="32">
         <v>50</v>
       </c>
-      <c r="P6" s="43"/>
-      <c r="V6" t="s">
+      <c r="V6" s="43"/>
+      <c r="AB6" t="s">
         <v>34</v>
       </c>
-      <c r="W6" t="s">
+      <c r="AC6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:30">
       <c r="A7" s="28">
         <v>44934</v>
       </c>
@@ -4272,37 +4307,43 @@
       <c r="F7" s="46">
         <v>0</v>
       </c>
-      <c r="H7" s="26">
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="N7" s="26">
         <f t="shared" si="1"/>
         <v>44933</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>4.1491642970301701</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>11</v>
       </c>
-      <c r="L7" t="str">
+      <c r="R7" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M7" t="s">
+      <c r="S7" t="s">
         <v>259</v>
       </c>
-      <c r="N7" s="31" t="str">
+      <c r="T7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorDressingLoss</v>
       </c>
-      <c r="O7" s="32">
-        <f>IF(P7="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K7,FALSE),P7)</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="43"/>
-      <c r="V7" t="s">
+      <c r="U7" s="32">
+        <f>IF(V7="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q7,FALSE),V7)</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="43"/>
+      <c r="AB7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1">
+    <row r="8" spans="1:30" ht="15.75" thickBot="1">
       <c r="A8" s="28">
         <v>44935</v>
       </c>
@@ -4321,34 +4362,40 @@
       <c r="F8" s="46">
         <v>0</v>
       </c>
-      <c r="H8" s="26">
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="N8" s="26">
         <f t="shared" si="1"/>
         <v>44934</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>11.680823993463974</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>15</v>
       </c>
-      <c r="L8" t="str">
+      <c r="R8" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M8" t="s">
+      <c r="S8" t="s">
         <v>260</v>
       </c>
-      <c r="N8" s="31" t="str">
+      <c r="T8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorMoistureContent</v>
       </c>
-      <c r="O8" s="32">
-        <f>IF(P8="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K8,FALSE),P8)</f>
+      <c r="U8" s="32">
+        <f>IF(V8="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q8,FALSE),V8)</f>
         <v>80</v>
       </c>
-      <c r="P8" s="43"/>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" thickBot="1">
+      <c r="V8" s="43"/>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" thickBot="1">
       <c r="A9" s="28">
         <v>44936</v>
       </c>
@@ -4367,33 +4414,39 @@
       <c r="F9" s="46">
         <v>0</v>
       </c>
-      <c r="H9" s="26">
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="N9" s="26">
         <f t="shared" si="1"/>
         <v>44935</v>
       </c>
-      <c r="I9">
+      <c r="O9">
         <v>11.289351844181724</v>
       </c>
-      <c r="L9" t="str">
+      <c r="R9" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M9" t="s">
+      <c r="S9" t="s">
         <v>261</v>
       </c>
-      <c r="N9" s="31" t="str">
+      <c r="T9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishDate</v>
       </c>
-      <c r="O9" s="33">
-        <f>P9</f>
+      <c r="U9" s="33">
+        <f>V9</f>
         <v>44929</v>
       </c>
-      <c r="P9" s="44">
+      <c r="V9" s="44">
         <v>44929</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="28">
         <v>44937</v>
       </c>
@@ -4412,34 +4465,40 @@
       <c r="F10" s="46">
         <v>0</v>
       </c>
-      <c r="H10" s="26">
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="N10" s="26">
         <f t="shared" si="1"/>
         <v>44936</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>13.934890823546613</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
         <v>3</v>
       </c>
-      <c r="L10" t="str">
+      <c r="R10" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M10" t="s">
+      <c r="S10" t="s">
         <v>262</v>
       </c>
-      <c r="N10" s="31" t="str">
+      <c r="T10" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishStage</v>
       </c>
-      <c r="O10" s="32" t="str">
-        <f>IF(P10="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K10,FALSE),P10)</f>
+      <c r="U10" s="32" t="str">
+        <f>IF(V10="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q10,FALSE),V10)</f>
         <v>Seed</v>
       </c>
-      <c r="P10" s="43"/>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" thickBot="1">
+      <c r="V10" s="43"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" thickBot="1">
       <c r="A11" s="28">
         <v>44938</v>
       </c>
@@ -4458,33 +4517,39 @@
       <c r="F11" s="46">
         <v>0</v>
       </c>
-      <c r="H11" s="26">
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="N11" s="26">
         <f t="shared" si="1"/>
         <v>44937</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>7.3816990790906738</v>
       </c>
-      <c r="L11" t="str">
+      <c r="R11" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M11" t="s">
+      <c r="S11" t="s">
         <v>263</v>
       </c>
-      <c r="N11" s="31" t="str">
+      <c r="T11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorHarvestDate</v>
       </c>
-      <c r="O11" s="33">
-        <f>P11</f>
+      <c r="U11" s="33">
+        <f>V11</f>
         <v>44938</v>
       </c>
-      <c r="P11" s="44">
+      <c r="V11" s="44">
         <v>44938</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:30">
       <c r="A12" s="28">
         <v>44939</v>
       </c>
@@ -4503,39 +4568,45 @@
       <c r="F12" s="46">
         <v>0</v>
       </c>
-      <c r="H12" s="26">
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="N12" s="26">
         <f t="shared" si="1"/>
         <v>44938</v>
       </c>
-      <c r="I12">
+      <c r="O12">
         <v>13.932559604705048</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>5</v>
       </c>
-      <c r="L12" t="str">
+      <c r="R12" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M12" t="s">
+      <c r="S12" t="s">
         <v>264</v>
       </c>
-      <c r="N12" s="31" t="str">
+      <c r="T12" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorHarvestStage</v>
       </c>
-      <c r="O12" s="32" t="str">
-        <f>IF(P12="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K12,FALSE),P12)</f>
+      <c r="U12" s="32" t="str">
+        <f>IF(V12="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q12,FALSE),V12)</f>
         <v>EarlyReproductive</v>
       </c>
-      <c r="P12" s="43"/>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="V12" s="43"/>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13" s="28">
         <v>44940</v>
       </c>
       <c r="B13" s="46">
-        <v>-87.626972327845209</v>
+        <v>100</v>
       </c>
       <c r="C13" s="46">
         <v>0</v>
@@ -4549,36 +4620,42 @@
       <c r="F13" s="46">
         <v>0</v>
       </c>
-      <c r="H13" s="26">
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="N13" s="26">
         <f t="shared" si="1"/>
         <v>44939</v>
       </c>
-      <c r="I13">
+      <c r="O13">
         <v>5.3540880739901002</v>
       </c>
-      <c r="L13" t="str">
+      <c r="R13" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M13" t="s">
+      <c r="S13" t="s">
         <v>265</v>
       </c>
-      <c r="N13" s="31" t="str">
+      <c r="T13" s="31" t="str">
         <f t="shared" si="0"/>
         <v>PriorResidueTreatment</v>
       </c>
-      <c r="O13" s="32" t="str">
-        <f>IF(P13="",W2,P13)</f>
+      <c r="U13" s="32" t="str">
+        <f>IF(V13="",AC2,V13)</f>
         <v>None</v>
       </c>
-      <c r="P13" s="43"/>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" thickBot="1">
+      <c r="V13" s="43"/>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" thickBot="1">
       <c r="A14" s="28">
         <v>44941</v>
       </c>
       <c r="B14" s="46">
-        <v>31.024121111956646</v>
+        <v>137.85109343980184</v>
       </c>
       <c r="C14" s="46">
         <v>0</v>
@@ -4590,38 +4667,44 @@
         <v>0.49985204228695124</v>
       </c>
       <c r="F14" s="46">
-        <v>101</v>
-      </c>
-      <c r="H14" s="26">
+        <v>37</v>
+      </c>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="N14" s="26">
         <f t="shared" si="1"/>
         <v>44940</v>
       </c>
-      <c r="I14">
+      <c r="O14">
         <v>13.363497784448709</v>
       </c>
-      <c r="L14" t="str">
+      <c r="R14" t="str">
         <f t="shared" si="2"/>
         <v>Prior</v>
       </c>
-      <c r="M14" t="s">
+      <c r="S14" t="s">
         <v>266</v>
       </c>
-      <c r="N14" s="34" t="str">
+      <c r="T14" s="34" t="str">
         <f t="shared" si="0"/>
         <v>PriorEstablishN</v>
       </c>
-      <c r="O14" s="35">
-        <f>IF(P14="",0,P14)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="43"/>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1">
+      <c r="U14" s="35">
+        <f>IF(V14="",0,V14)</f>
+        <v>0</v>
+      </c>
+      <c r="V14" s="43"/>
+    </row>
+    <row r="15" spans="1:30" ht="15.75" thickBot="1">
       <c r="A15" s="28">
         <v>44942</v>
       </c>
       <c r="B15" s="46">
-        <v>96.332794344830148</v>
+        <v>122.35976667267533</v>
       </c>
       <c r="C15" s="46">
         <v>17.416845524679701</v>
@@ -4633,39 +4716,45 @@
         <v>1.1339871834081825</v>
       </c>
       <c r="F15" s="46">
-        <v>101</v>
-      </c>
-      <c r="H15" s="26">
+        <v>0</v>
+      </c>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="26">
         <f t="shared" si="1"/>
         <v>44941</v>
       </c>
-      <c r="I15">
+      <c r="O15">
         <v>6.6646938971593457</v>
       </c>
-      <c r="L15" t="s">
+      <c r="R15" t="s">
         <v>273</v>
       </c>
-      <c r="M15" t="s">
+      <c r="S15" t="s">
         <v>270</v>
       </c>
-      <c r="N15" s="37" t="str">
-        <f>L15&amp;M15</f>
+      <c r="T15" s="37" t="str">
+        <f>R15&amp;S15</f>
         <v>CurrentCropName</v>
       </c>
-      <c r="O15" s="38" t="str">
-        <f>P15</f>
+      <c r="U15" s="38" t="str">
+        <f>V15</f>
         <v>Potato Vegetable General</v>
       </c>
-      <c r="P15" s="45" t="s">
+      <c r="V15" s="45" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:30">
       <c r="A16" s="28">
         <v>44943</v>
       </c>
       <c r="B16" s="46">
-        <v>74.769689993112422</v>
+        <v>100.79666232095761</v>
       </c>
       <c r="C16" s="46">
         <v>22.905369773059999</v>
@@ -4679,41 +4768,47 @@
       <c r="F16" s="46">
         <v>0</v>
       </c>
-      <c r="H16" s="26">
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="26">
         <f t="shared" si="1"/>
         <v>44942</v>
       </c>
-      <c r="I16">
+      <c r="O16">
         <v>15.119829112109056</v>
       </c>
-      <c r="K16">
+      <c r="Q16">
         <v>7</v>
       </c>
-      <c r="L16" t="str">
-        <f>L15</f>
+      <c r="R16" t="str">
+        <f>R15</f>
         <v>Current</v>
       </c>
-      <c r="M16" t="s">
+      <c r="S16" t="s">
         <v>256</v>
       </c>
-      <c r="N16" s="18" t="str">
-        <f t="shared" ref="N16:N26" si="3">L16&amp;M16</f>
+      <c r="T16" s="18" t="str">
+        <f t="shared" ref="T16:T26" si="3">R16&amp;S16</f>
         <v>CurrentSaleableYield</v>
       </c>
-      <c r="O16" s="19">
-        <f>IF(P16="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K16,FALSE),P16)</f>
+      <c r="U16" s="19">
+        <f>IF(V16="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q16,FALSE),V16)</f>
         <v>50</v>
       </c>
-      <c r="P16" s="43">
+      <c r="V16" s="43">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:22">
       <c r="A17" s="28">
         <v>44944</v>
       </c>
       <c r="B17" s="46">
-        <v>33.971551746940349</v>
+        <v>59.998524074785536</v>
       </c>
       <c r="C17" s="46">
         <v>42.297904798604399</v>
@@ -4727,41 +4822,47 @@
       <c r="F17" s="46">
         <v>0</v>
       </c>
-      <c r="H17" s="26">
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="26">
         <f t="shared" si="1"/>
         <v>44943</v>
       </c>
-      <c r="I17">
+      <c r="O17">
         <v>10.605844567907475</v>
       </c>
-      <c r="K17">
+      <c r="Q17">
         <v>8</v>
       </c>
-      <c r="L17" t="str">
-        <f t="shared" ref="L17:L26" si="4">L16</f>
+      <c r="R17" t="str">
+        <f t="shared" ref="R17:R26" si="4">R16</f>
         <v>Current</v>
       </c>
-      <c r="M17" t="s">
+      <c r="S17" t="s">
         <v>257</v>
       </c>
-      <c r="N17" s="18" t="str">
+      <c r="T17" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentUnits</v>
       </c>
-      <c r="O17" s="19" t="str">
-        <f>IF(P17="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K17,FALSE),P17)</f>
+      <c r="U17" s="19" t="str">
+        <f>IF(V17="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q17,FALSE),V17)</f>
         <v>t/ha</v>
       </c>
-      <c r="P17" s="43" t="s">
+      <c r="V17" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:22">
       <c r="A18" s="28">
         <v>44945</v>
       </c>
       <c r="B18" s="46">
-        <v>96.73359554051018</v>
+        <v>157</v>
       </c>
       <c r="C18" s="46">
         <v>18.5262812186348</v>
@@ -4773,43 +4874,49 @@
         <v>0.29204860623618223</v>
       </c>
       <c r="F18" s="46">
-        <v>101</v>
-      </c>
-      <c r="H18" s="26">
+        <v>0</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="N18" s="26">
         <f t="shared" si="1"/>
         <v>44944</v>
       </c>
-      <c r="I18">
+      <c r="O18">
         <v>11.901756295522578</v>
       </c>
-      <c r="K18">
+      <c r="Q18">
         <v>12</v>
       </c>
-      <c r="L18" t="str">
+      <c r="R18" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M18" t="s">
+      <c r="S18" t="s">
         <v>258</v>
       </c>
-      <c r="N18" s="18" t="str">
+      <c r="T18" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentFieldLoss</v>
       </c>
-      <c r="O18" s="19">
-        <f>IF(P18="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K18,FALSE),P18)</f>
+      <c r="U18" s="19">
+        <f>IF(V18="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q18,FALSE),V18)</f>
         <v>5</v>
       </c>
-      <c r="P18" s="43">
+      <c r="V18" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:22">
       <c r="A19" s="28">
         <v>44946</v>
       </c>
       <c r="B19" s="46">
-        <v>62.664509829950077</v>
+        <v>122.93091428943993</v>
       </c>
       <c r="C19" s="46">
         <v>34.852417560117701</v>
@@ -4823,41 +4930,47 @@
       <c r="F19" s="46">
         <v>0</v>
       </c>
-      <c r="H19" s="26">
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="N19" s="26">
         <f t="shared" si="1"/>
         <v>44945</v>
       </c>
-      <c r="I19">
+      <c r="O19">
         <v>3.8939814164824327</v>
       </c>
-      <c r="K19">
+      <c r="Q19">
         <v>11</v>
       </c>
-      <c r="L19" t="str">
+      <c r="R19" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M19" t="s">
+      <c r="S19" t="s">
         <v>259</v>
       </c>
-      <c r="N19" s="18" t="str">
+      <c r="T19" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentDressingLoss</v>
       </c>
-      <c r="O19" s="19">
-        <f>IF(P19="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K19,FALSE),P19)</f>
+      <c r="U19" s="19">
+        <f>IF(V19="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q19,FALSE),V19)</f>
         <v>5</v>
       </c>
-      <c r="P19" s="43">
+      <c r="V19" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1">
+    <row r="20" spans="1:22" ht="15.75" thickBot="1">
       <c r="A20" s="28">
         <v>44947</v>
       </c>
       <c r="B20" s="46">
-        <v>29.407873186198003</v>
+        <v>89.674277645687852</v>
       </c>
       <c r="C20" s="46">
         <v>33.916105544638199</v>
@@ -4871,39 +4984,45 @@
       <c r="F20" s="46">
         <v>0</v>
       </c>
-      <c r="H20" s="26">
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="N20" s="26">
         <f t="shared" si="1"/>
         <v>44946</v>
       </c>
-      <c r="I20">
+      <c r="O20">
         <v>6.2562047514789443</v>
       </c>
-      <c r="K20">
+      <c r="Q20">
         <v>15</v>
       </c>
-      <c r="L20" t="str">
+      <c r="R20" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M20" t="s">
+      <c r="S20" t="s">
         <v>260</v>
       </c>
-      <c r="N20" s="18" t="str">
+      <c r="T20" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentMoistureContent</v>
       </c>
-      <c r="O20" s="19">
-        <f>IF(P20="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K20,FALSE),P20)</f>
+      <c r="U20" s="19">
+        <f>IF(V20="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q20,FALSE),V20)</f>
         <v>77.7</v>
       </c>
-      <c r="P20" s="43"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1">
+      <c r="V20" s="43"/>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" thickBot="1">
       <c r="A21" s="28">
         <v>44948</v>
       </c>
       <c r="B21" s="46">
-        <v>30.990113542865458</v>
+        <v>91.256518002355278</v>
       </c>
       <c r="C21" s="46">
         <v>0</v>
@@ -4917,38 +5036,44 @@
       <c r="F21" s="46">
         <v>0</v>
       </c>
-      <c r="H21" s="26">
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="N21" s="26">
         <f t="shared" si="1"/>
         <v>44947</v>
       </c>
-      <c r="I21">
+      <c r="O21">
         <v>5.2802002140493496</v>
       </c>
-      <c r="L21" t="str">
+      <c r="R21" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M21" t="s">
+      <c r="S21" t="s">
         <v>261</v>
       </c>
-      <c r="N21" s="18" t="str">
+      <c r="T21" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentEstablishDate</v>
       </c>
-      <c r="O21" s="39">
-        <f>P21</f>
+      <c r="U21" s="39">
+        <f>V21</f>
         <v>44941</v>
       </c>
-      <c r="P21" s="44">
+      <c r="V21" s="44">
         <v>44941</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" thickBot="1">
+    <row r="22" spans="1:22" ht="15.75" thickBot="1">
       <c r="A22" s="28">
         <v>44949</v>
       </c>
       <c r="B22" s="46">
-        <v>32.448720359363335</v>
+        <v>92.715124818853155</v>
       </c>
       <c r="C22" s="46">
         <v>0</v>
@@ -4962,41 +5087,47 @@
       <c r="F22" s="46">
         <v>0</v>
       </c>
-      <c r="H22" s="26">
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="N22" s="26">
         <f t="shared" si="1"/>
         <v>44948</v>
       </c>
-      <c r="I22">
+      <c r="O22">
         <v>14.049139077238873</v>
       </c>
-      <c r="K22">
+      <c r="Q22">
         <v>3</v>
       </c>
-      <c r="L22" t="str">
+      <c r="R22" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M22" t="s">
+      <c r="S22" t="s">
         <v>262</v>
       </c>
-      <c r="N22" s="18" t="str">
+      <c r="T22" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentEstablishStage</v>
       </c>
-      <c r="O22" s="19" t="str">
-        <f>IF(P22="",VLOOKUP(O$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K22,FALSE),P22)</f>
+      <c r="U22" s="19" t="str">
+        <f>IF(V22="",VLOOKUP(U$15,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q22,FALSE),V22)</f>
         <v>Seedling</v>
       </c>
-      <c r="P22" s="43" t="s">
+      <c r="V22" s="43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1">
+    <row r="23" spans="1:22" ht="15.75" thickBot="1">
       <c r="A23" s="28">
         <v>44950</v>
       </c>
       <c r="B23" s="46">
-        <v>34.508943004636137</v>
+        <v>94.775347464125986</v>
       </c>
       <c r="C23" s="46">
         <v>0</v>
@@ -5010,38 +5141,44 @@
       <c r="F23" s="46">
         <v>0</v>
       </c>
-      <c r="H23" s="26">
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="N23" s="26">
         <f t="shared" si="1"/>
         <v>44949</v>
       </c>
-      <c r="I23">
+      <c r="O23">
         <v>13.012433227854736</v>
       </c>
-      <c r="L23" t="str">
+      <c r="R23" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M23" t="s">
+      <c r="S23" t="s">
         <v>263</v>
       </c>
-      <c r="N23" s="18" t="str">
+      <c r="T23" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentHarvestDate</v>
       </c>
-      <c r="O23" s="39">
-        <f>P23</f>
+      <c r="U23" s="39">
+        <f>V23</f>
         <v>44947</v>
       </c>
-      <c r="P23" s="44">
+      <c r="V23" s="44">
         <v>44947</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:22">
       <c r="A24" s="28">
         <v>44951</v>
       </c>
       <c r="B24" s="46">
-        <v>35.839661115896718</v>
+        <v>96.106065575386566</v>
       </c>
       <c r="C24" s="46">
         <v>0</v>
@@ -5055,41 +5192,47 @@
       <c r="F24" s="46">
         <v>0</v>
       </c>
-      <c r="H24" s="26">
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="N24" s="26">
         <f t="shared" si="1"/>
         <v>44950</v>
       </c>
-      <c r="I24">
+      <c r="O24">
         <v>18.45901588220935</v>
       </c>
-      <c r="K24">
+      <c r="Q24">
         <v>5</v>
       </c>
-      <c r="L24" t="str">
+      <c r="R24" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M24" t="s">
+      <c r="S24" t="s">
         <v>264</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="T24" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentHarvestStage</v>
       </c>
-      <c r="O24" s="19" t="str">
-        <f>IF(P24="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K24,FALSE),P24)</f>
+      <c r="U24" s="19" t="str">
+        <f>IF(V24="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q24,FALSE),V24)</f>
         <v>Vegetative</v>
       </c>
-      <c r="P24" s="43" t="s">
+      <c r="V24" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:22">
       <c r="A25" s="28">
         <v>44952</v>
       </c>
       <c r="B25" s="46">
-        <v>34.116666523164668</v>
+        <v>94.383070982654488</v>
       </c>
       <c r="C25" s="46">
         <v>3.3685338546165302</v>
@@ -5103,38 +5246,44 @@
       <c r="F25" s="46">
         <v>0</v>
       </c>
-      <c r="H25" s="26">
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="N25" s="26">
         <f t="shared" si="1"/>
         <v>44951</v>
       </c>
-      <c r="I25">
+      <c r="O25">
         <v>11.995492344501493</v>
       </c>
-      <c r="L25" t="str">
+      <c r="R25" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M25" t="s">
+      <c r="S25" t="s">
         <v>265</v>
       </c>
-      <c r="N25" s="18" t="str">
+      <c r="T25" s="18" t="str">
         <f t="shared" si="3"/>
         <v>CurrentResidueTreatment</v>
       </c>
-      <c r="O25" s="19" t="str">
-        <f>IF(P25="",W2,P25)</f>
+      <c r="U25" s="19" t="str">
+        <f>IF(V25="",AC2,V25)</f>
         <v>Incorporated</v>
       </c>
-      <c r="P25" s="43" t="s">
+      <c r="V25" s="43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1">
+    <row r="26" spans="1:22" ht="15.75" thickBot="1">
       <c r="A26" s="28">
         <v>44953</v>
       </c>
       <c r="B26" s="46">
-        <v>31.548317068393146</v>
+        <v>91.814721527882966</v>
       </c>
       <c r="C26" s="46">
         <v>3.7338784334915598</v>
@@ -5148,38 +5297,44 @@
       <c r="F26" s="46">
         <v>0</v>
       </c>
-      <c r="H26" s="26">
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="N26" s="26">
         <f t="shared" si="1"/>
         <v>44952</v>
       </c>
-      <c r="I26">
+      <c r="O26">
         <v>14.89124712931573</v>
       </c>
-      <c r="L26" t="str">
+      <c r="R26" t="str">
         <f t="shared" si="4"/>
         <v>Current</v>
       </c>
-      <c r="M26" t="s">
+      <c r="S26" t="s">
         <v>266</v>
       </c>
-      <c r="N26" s="23" t="str">
+      <c r="T26" s="23" t="str">
         <f t="shared" si="3"/>
         <v>CurrentEstablishN</v>
       </c>
-      <c r="O26" s="24">
-        <f>IF(P26="",0,P26)</f>
+      <c r="U26" s="24">
+        <f>IF(V26="",0,V26)</f>
         <v>10</v>
       </c>
-      <c r="P26" s="43">
+      <c r="V26" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1">
+    <row r="27" spans="1:22" ht="15.75" thickBot="1">
       <c r="A27" s="28">
         <v>44954</v>
       </c>
       <c r="B27" s="46">
-        <v>23.279512413769794</v>
+        <v>83.545916873259642</v>
       </c>
       <c r="C27" s="46">
         <v>10.2509561270017</v>
@@ -5193,37 +5348,43 @@
       <c r="F27" s="46">
         <v>0</v>
       </c>
-      <c r="H27" s="26">
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="N27" s="26">
         <f t="shared" si="1"/>
         <v>44953</v>
       </c>
-      <c r="I27">
+      <c r="O27">
         <v>10.598117463308858</v>
       </c>
-      <c r="L27" t="s">
+      <c r="R27" t="s">
         <v>274</v>
       </c>
-      <c r="M27" t="s">
+      <c r="S27" t="s">
         <v>270</v>
       </c>
-      <c r="N27" s="29" t="str">
-        <f>L27&amp;M27</f>
+      <c r="T27" s="29" t="str">
+        <f>R27&amp;S27</f>
         <v>FollowingCropName</v>
       </c>
-      <c r="O27" s="30" t="str">
-        <f>P27</f>
+      <c r="U27" s="30" t="str">
+        <f>V27</f>
         <v>Oat Grain General</v>
       </c>
-      <c r="P27" s="45" t="s">
+      <c r="V27" s="45" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:22">
       <c r="A28" s="28">
         <v>44955</v>
       </c>
       <c r="B28" s="46">
-        <v>11.613179195530222</v>
+        <v>71.87958365502007</v>
       </c>
       <c r="C28" s="46">
         <v>13.278303362827801</v>
@@ -5237,39 +5398,45 @@
       <c r="F28" s="46">
         <v>0</v>
       </c>
-      <c r="H28" s="26">
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="N28" s="26">
         <f t="shared" si="1"/>
         <v>44954</v>
       </c>
-      <c r="I28">
+      <c r="O28">
         <v>18.08459347173163</v>
       </c>
-      <c r="K28">
+      <c r="Q28">
         <v>7</v>
       </c>
-      <c r="L28" t="str">
-        <f>L27</f>
+      <c r="R28" t="str">
+        <f>R27</f>
         <v>Following</v>
       </c>
-      <c r="M28" t="s">
+      <c r="S28" t="s">
         <v>256</v>
       </c>
-      <c r="N28" s="31" t="str">
-        <f t="shared" ref="N28:N38" si="5">L28&amp;M28</f>
+      <c r="T28" s="31" t="str">
+        <f t="shared" ref="T28:T38" si="5">R28&amp;S28</f>
         <v>FollowingSaleableYield</v>
       </c>
-      <c r="O28" s="32">
-        <f>IF(P28="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K28,FALSE),P28)</f>
+      <c r="U28" s="32">
+        <f>IF(V28="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q28,FALSE),V28)</f>
         <v>6</v>
       </c>
-      <c r="P28" s="43"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="V28" s="43"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="28">
         <v>44956</v>
       </c>
       <c r="B29" s="46">
-        <v>-9.0540060934372377</v>
+        <v>51.212398366052582</v>
       </c>
       <c r="C29" s="46">
         <v>22.612540590591902</v>
@@ -5283,39 +5450,45 @@
       <c r="F29" s="46">
         <v>0</v>
       </c>
-      <c r="H29" s="26">
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="N29" s="26">
         <f t="shared" si="1"/>
         <v>44955</v>
       </c>
-      <c r="I29">
+      <c r="O29">
         <v>14.79161849090584</v>
       </c>
-      <c r="K29">
+      <c r="Q29">
         <v>8</v>
       </c>
-      <c r="L29" t="str">
-        <f t="shared" ref="L29:L38" si="6">L28</f>
+      <c r="R29" t="str">
+        <f t="shared" ref="R29:R38" si="6">R28</f>
         <v>Following</v>
       </c>
-      <c r="M29" t="s">
+      <c r="S29" t="s">
         <v>257</v>
       </c>
-      <c r="N29" s="31" t="str">
+      <c r="T29" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingUnits</v>
       </c>
-      <c r="O29" s="32" t="str">
-        <f>IF(P29="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K29,FALSE),P29)</f>
+      <c r="U29" s="32" t="str">
+        <f>IF(V29="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q29,FALSE),V29)</f>
         <v>t/ha</v>
       </c>
-      <c r="P29" s="43"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="V29" s="43"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="28">
         <v>44957</v>
       </c>
       <c r="B30" s="46">
-        <v>-31.608687670631639</v>
+        <v>28.65771678885821</v>
       </c>
       <c r="C30" s="46">
         <v>24.289568708652101</v>
@@ -5329,39 +5502,45 @@
       <c r="F30" s="46">
         <v>0</v>
       </c>
-      <c r="H30" s="26">
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="N30" s="26">
         <f t="shared" si="1"/>
         <v>44956</v>
       </c>
-      <c r="I30">
+      <c r="O30">
         <v>17.933505589637022</v>
       </c>
-      <c r="K30">
+      <c r="Q30">
         <v>12</v>
       </c>
-      <c r="L30" t="str">
+      <c r="R30" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M30" t="s">
+      <c r="S30" t="s">
         <v>258</v>
       </c>
-      <c r="N30" s="31" t="str">
+      <c r="T30" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingFieldLoss</v>
       </c>
-      <c r="O30" s="32">
-        <f>IF(P30="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K30,FALSE),P30)</f>
-        <v>0</v>
-      </c>
-      <c r="P30" s="43"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="U30" s="32">
+        <f>IF(V30="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q30,FALSE),V30)</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="43"/>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="28">
         <v>44958</v>
       </c>
       <c r="B31" s="46">
-        <v>-59.422019956079851</v>
+        <v>0.84438450341001214</v>
       </c>
       <c r="C31" s="46">
         <v>30.0492178787513</v>
@@ -5375,39 +5554,45 @@
       <c r="F31" s="46">
         <v>0</v>
       </c>
-      <c r="H31" s="26">
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="N31" s="26">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="I31">
+      <c r="O31">
         <v>16.082282662694066</v>
       </c>
-      <c r="K31">
+      <c r="Q31">
         <v>11</v>
       </c>
-      <c r="L31" t="str">
+      <c r="R31" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M31" t="s">
+      <c r="S31" t="s">
         <v>259</v>
       </c>
-      <c r="N31" s="31" t="str">
+      <c r="T31" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingDressingLoss</v>
       </c>
-      <c r="O31" s="32">
-        <f>IF(P31="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K31,FALSE),P31)</f>
-        <v>0</v>
-      </c>
-      <c r="P31" s="43"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1">
+      <c r="U31" s="32">
+        <f>IF(V31="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q31,FALSE),V31)</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="43"/>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" thickBot="1">
       <c r="A32" s="28">
         <v>44959</v>
       </c>
       <c r="B32" s="46">
-        <v>-73.443284360329358</v>
+        <v>-13.176879900839495</v>
       </c>
       <c r="C32" s="46">
         <v>15.4900614607009</v>
@@ -5421,34 +5606,40 @@
       <c r="F32" s="46">
         <v>0</v>
       </c>
-      <c r="H32" s="26">
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="N32" s="26">
         <f t="shared" si="1"/>
         <v>44958</v>
       </c>
-      <c r="I32">
+      <c r="O32">
         <v>20.828587685127982</v>
       </c>
-      <c r="K32">
+      <c r="Q32">
         <v>15</v>
       </c>
-      <c r="L32" t="str">
+      <c r="R32" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M32" t="s">
+      <c r="S32" t="s">
         <v>260</v>
       </c>
-      <c r="N32" s="31" t="str">
+      <c r="T32" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingMoistureContent</v>
       </c>
-      <c r="O32" s="32">
-        <f>IF(P32="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K32,FALSE),P32)</f>
+      <c r="U32" s="32">
+        <f>IF(V32="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q32,FALSE),V32)</f>
         <v>13</v>
       </c>
-      <c r="P32" s="43"/>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" thickBot="1">
+      <c r="V32" s="43"/>
+    </row>
+    <row r="33" spans="1:22" ht="15.75" thickBot="1">
       <c r="A33" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5467,33 +5658,39 @@
       <c r="F33" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H33" s="26">
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="N33" s="26">
         <f t="shared" si="1"/>
         <v>44959</v>
       </c>
-      <c r="I33">
+      <c r="O33">
         <v>13.76912650928467</v>
       </c>
-      <c r="L33" t="str">
+      <c r="R33" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M33" t="s">
+      <c r="S33" t="s">
         <v>261</v>
       </c>
-      <c r="N33" s="31" t="str">
+      <c r="T33" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingEstablishDate</v>
       </c>
-      <c r="O33" s="33">
-        <f>P33</f>
+      <c r="U33" s="33">
+        <f>V33</f>
         <v>44951</v>
       </c>
-      <c r="P33" s="44">
+      <c r="V33" s="44">
         <v>44951</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.75" thickBot="1">
+    <row r="34" spans="1:22" ht="15.75" thickBot="1">
       <c r="A34" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5512,34 +5709,40 @@
       <c r="F34" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H34" s="26">
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="N34" s="26">
         <f t="shared" si="1"/>
         <v>44960</v>
       </c>
-      <c r="I34">
+      <c r="O34">
         <v>23.549644512826927</v>
       </c>
-      <c r="K34">
+      <c r="Q34">
         <v>3</v>
       </c>
-      <c r="L34" t="str">
+      <c r="R34" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M34" t="s">
+      <c r="S34" t="s">
         <v>262</v>
       </c>
-      <c r="N34" s="31" t="str">
+      <c r="T34" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingEstablishStage</v>
       </c>
-      <c r="O34" s="32" t="str">
-        <f>IF(P34="",VLOOKUP(O$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K34,FALSE),P34)</f>
+      <c r="U34" s="32" t="str">
+        <f>IF(V34="",VLOOKUP(U$27,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q34,FALSE),V34)</f>
         <v>Seed</v>
       </c>
-      <c r="P34" s="43"/>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" thickBot="1">
+      <c r="V34" s="43"/>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" thickBot="1">
       <c r="A35" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5558,27 +5761,33 @@
       <c r="F35" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L35" t="str">
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="R35" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M35" t="s">
+      <c r="S35" t="s">
         <v>263</v>
       </c>
-      <c r="N35" s="31" t="str">
+      <c r="T35" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingHarvestDate</v>
       </c>
-      <c r="O35" s="33">
-        <f>P35</f>
+      <c r="U35" s="33">
+        <f>V35</f>
         <v>44959</v>
       </c>
-      <c r="P35" s="44">
-        <f>H33</f>
+      <c r="V35" s="44">
+        <f>N33</f>
         <v>44959</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:22">
       <c r="A36" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5597,27 +5806,33 @@
       <c r="F36" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K36">
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="Q36">
         <v>5</v>
       </c>
-      <c r="L36" t="str">
+      <c r="R36" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M36" t="s">
+      <c r="S36" t="s">
         <v>264</v>
       </c>
-      <c r="N36" s="31" t="str">
+      <c r="T36" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingHarvestStage</v>
       </c>
-      <c r="O36" s="32" t="str">
-        <f>IF(P36="",VLOOKUP(O$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$K36,FALSE),P36)</f>
+      <c r="U36" s="32" t="str">
+        <f>IF(V36="",VLOOKUP(U$3,CropCoefficients!$K$3:$AF$78,'NBalance Test'!$Q36,FALSE),V36)</f>
         <v>EarlyReproductive</v>
       </c>
-      <c r="P36" s="43"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="V36" s="43"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5636,24 +5851,30 @@
       <c r="F37" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L37" t="str">
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="R37" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M37" t="s">
+      <c r="S37" t="s">
         <v>265</v>
       </c>
-      <c r="N37" s="31" t="str">
+      <c r="T37" s="31" t="str">
         <f t="shared" si="5"/>
         <v>FollowingResidueTreatment</v>
       </c>
-      <c r="O37" s="32" t="str">
-        <f>IF(P37="",W2,P37)</f>
+      <c r="U37" s="32" t="str">
+        <f>IF(V37="",AC2,V37)</f>
         <v>None</v>
       </c>
-      <c r="P37" s="43"/>
-    </row>
-    <row r="38" spans="1:16" ht="15.75" thickBot="1">
+      <c r="V37" s="43"/>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" thickBot="1">
       <c r="A38" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5672,24 +5893,30 @@
       <c r="F38" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L38" t="str">
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="R38" t="str">
         <f t="shared" si="6"/>
         <v>Following</v>
       </c>
-      <c r="M38" t="s">
+      <c r="S38" t="s">
         <v>266</v>
       </c>
-      <c r="N38" s="34" t="str">
+      <c r="T38" s="34" t="str">
         <f t="shared" si="5"/>
         <v>FollowingEstablishN</v>
       </c>
-      <c r="O38" s="35">
-        <f>IF(P38="",0,P38)</f>
-        <v>0</v>
-      </c>
-      <c r="P38" s="43"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="U38" s="35">
+        <f>IF(V38="",0,V38)</f>
+        <v>0</v>
+      </c>
+      <c r="V38" s="43"/>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5708,15 +5935,21 @@
       <c r="F39" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G39" s="27"/>
-      <c r="N39" t="s">
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="27"/>
+      <c r="T39" t="s">
         <v>281</v>
       </c>
-      <c r="O39">
+      <c r="U39">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:22">
       <c r="A40" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5735,14 +5968,20 @@
       <c r="F40" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N40" t="s">
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="T40" t="s">
         <v>282</v>
       </c>
-      <c r="O40">
+      <c r="U40">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:22">
       <c r="A41" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5761,14 +6000,20 @@
       <c r="F41" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N41" t="s">
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="T41" t="s">
         <v>283</v>
       </c>
-      <c r="O41">
+      <c r="U41">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:22">
       <c r="A42" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5787,14 +6032,20 @@
       <c r="F42" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N42" t="s">
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="T42" t="s">
         <v>284</v>
       </c>
-      <c r="O42">
+      <c r="U42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:22">
       <c r="A43" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5813,14 +6064,20 @@
       <c r="F43" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N43" t="s">
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="T43" t="s">
         <v>266</v>
       </c>
-      <c r="O43">
+      <c r="U43">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:22">
       <c r="A44" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5839,14 +6096,20 @@
       <c r="F44" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N44" t="s">
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="T44" t="s">
         <v>285</v>
       </c>
-      <c r="O44">
+      <c r="U44">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:22">
       <c r="A45" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5865,8 +6128,14 @@
       <c r="F45" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5885,8 +6154,14 @@
       <c r="F46" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5905,8 +6180,14 @@
       <c r="F47" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5925,8 +6206,14 @@
       <c r="F48" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5945,8 +6232,14 @@
       <c r="F49" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5965,8 +6258,14 @@
       <c r="F50" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -5985,8 +6284,14 @@
       <c r="F51" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6005,8 +6310,14 @@
       <c r="F52" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6025,8 +6336,14 @@
       <c r="F53" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6045,8 +6362,14 @@
       <c r="F54" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6065,8 +6388,14 @@
       <c r="F55" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6085,8 +6414,14 @@
       <c r="F56" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6105,8 +6440,14 @@
       <c r="F57" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6125,8 +6466,14 @@
       <c r="F58" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6145,8 +6492,14 @@
       <c r="F59" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6165,8 +6518,14 @@
       <c r="F60" s="46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="28" t="e">
         <v>#N/A</v>
       </c>
@@ -6185,25 +6544,31 @@
       <c r="F61" s="46" t="e">
         <v>#N/A</v>
       </c>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O25:P25 O37:P37 O13:P13" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
-      <formula1>$W$2:$W$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U25:V25 U13:V13 U37:V37" xr:uid="{3DE26B06-4750-44B0-83A7-1227F7B54B47}">
+      <formula1>$AC$2:$AC$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P24 P36 P12" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
-      <formula1>$V$2:$V$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V24 V12 V36" xr:uid="{06B45905-6E1B-443D-B1AD-A919DC745A0E}">
+      <formula1>$AB$2:$AB$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P22 P34 P10" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
-      <formula1>$U$2:$U$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V22 V10 V34" xr:uid="{DC0257CB-3CD1-4F7D-9B68-276D2BCCE56B}">
+      <formula1>$AA$2:$AA$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P17 P29 P5" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
-      <formula1>$X$2:$X$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V17 V5 V29" xr:uid="{4075E367-9DF1-477A-911B-4E740AEED4E4}">
+      <formula1>$AD$2:$AD$4</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P18:P20 P30:P32 P6:P8" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:V20 V30:V32 V6:V8" xr:uid="{B2D348D7-0423-4C32-BE28-8CA7100F800E}">
       <formula1>100</formula1>
     </dataValidation>
   </dataValidations>
@@ -6217,19 +6582,19 @@
           <x14:formula1>
             <xm:f>CropCoefficients!$F$3:$F$78</xm:f>
           </x14:formula1>
-          <xm:sqref>J1</xm:sqref>
+          <xm:sqref>P1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3A6DE27-0EE4-4266-A7F4-377B95F78D99}">
           <x14:formula1>
             <xm:f>CropCoefficients!$B$3:$B$78</xm:f>
           </x14:formula1>
-          <xm:sqref>K3 K15 K27</xm:sqref>
+          <xm:sqref>Q3 Q15 Q27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFFB7881-7C85-4FD9-826D-70611F88B0E7}">
           <x14:formula1>
             <xm:f>CropCoefficients!$K$3:$K$78</xm:f>
           </x14:formula1>
-          <xm:sqref>O15:P15 O27:P27 O3:P3</xm:sqref>
+          <xm:sqref>U15:V15 U27:V27 U3:V3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6241,8 +6606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6871C5-A1CC-4FCE-AC7A-C84D2E0677C6}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D35:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6771,31 +7136,31 @@
         <v>44947</v>
       </c>
       <c r="C36">
-        <v>0.33522855275841695</v>
+        <v>0.32826590267958394</v>
       </c>
       <c r="D36">
-        <v>0.46093926004282321</v>
+        <v>0.45136561618442778</v>
       </c>
       <c r="E36">
-        <v>7.699780821169889</v>
+        <v>7.5398574521716917</v>
       </c>
       <c r="F36">
-        <v>0.85553120235221003</v>
+        <v>0.83776193913018815</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36">
-        <v>9.3514798363233407</v>
+        <v>9.1572509101658923</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>6.1117457438044233E-2</v>
+        <v>5.3835246346392154E-2</v>
       </c>
       <c r="K36">
-        <v>8.0314105887464238E-2</v>
+        <v>7.5548054211533114E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -6803,31 +7168,31 @@
         <v>44948</v>
       </c>
       <c r="C37">
-        <v>0.51082902926001172</v>
+        <v>0.48808460900452805</v>
       </c>
       <c r="D37">
-        <v>0.70238991523251593</v>
+        <v>0.67111633738122589</v>
       </c>
       <c r="E37">
-        <v>11.733104265815891</v>
+        <v>11.210693363072751</v>
       </c>
       <c r="F37">
-        <v>1.3036782517573218</v>
+        <v>1.2456325958969727</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>14.250001462065743</v>
+        <v>13.61552690535548</v>
       </c>
       <c r="I37">
-        <v>4.8985216257424025</v>
+        <v>4.4582759951895881</v>
       </c>
       <c r="J37">
-        <v>0.49688601323733578</v>
+        <v>0.42349796341566553</v>
       </c>
       <c r="K37">
-        <v>0.17660987768080746</v>
+        <v>0.16612937996243612</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -6835,31 +7200,31 @@
         <v>44949</v>
       </c>
       <c r="C38">
-        <v>0.6380181044769937</v>
+        <v>0.60191329863549692</v>
       </c>
       <c r="D38">
-        <v>0.87727489365586608</v>
+        <v>0.82763078562380821</v>
       </c>
       <c r="E38">
-        <v>14.654478337205948</v>
+        <v>13.82519607803407</v>
       </c>
       <c r="F38">
-        <v>1.6282753708006612</v>
+        <v>1.5361328975593416</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>17.798046706139466</v>
+        <v>16.790873059852718</v>
       </c>
       <c r="I38">
-        <v>3.5480452440737231</v>
+        <v>3.1753461544972374</v>
       </c>
       <c r="J38">
-        <v>0.80857015829254442</v>
+        <v>0.74241051060908547</v>
       </c>
       <c r="K38">
-        <v>0.22806804321122803</v>
+        <v>0.21453388171416449</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -6867,31 +7232,31 @@
         <v>44950</v>
       </c>
       <c r="C39">
-        <v>0.94753996287915065</v>
+        <v>0.87458541209486573</v>
       </c>
       <c r="D39">
-        <v>1.3028674489588317</v>
+        <v>1.2025549416304402</v>
       </c>
       <c r="E39">
-        <v>21.763808522380486</v>
+        <v>20.088133684053943</v>
       </c>
       <c r="F39">
-        <v>2.4182009469311661</v>
+        <v>2.2320148537837725</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>26.432416881149638</v>
+        <v>24.397288891563026</v>
       </c>
       <c r="I39">
-        <v>8.6343701750101722</v>
+        <v>7.6064158317103079</v>
       </c>
       <c r="J39">
-        <v>0.98321335826309841</v>
+        <v>0.97158441773664173</v>
       </c>
       <c r="K39">
-        <v>0.32117901920013953</v>
+        <v>0.30211940587545627</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -6899,31 +7264,31 @@
         <v>44951</v>
       </c>
       <c r="C40">
-        <v>1.063902167143687</v>
+        <v>0.97596911896507899</v>
       </c>
       <c r="D40">
-        <v>1.4628654798225691</v>
+        <v>1.3419575385769831</v>
       </c>
       <c r="E40">
-        <v>24.436502901581555</v>
+        <v>22.416790701229154</v>
       </c>
       <c r="F40">
-        <v>2.7151669890646177</v>
+        <v>2.4907545223587957</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>29.678437537612432</v>
+        <v>27.225471881130012</v>
       </c>
       <c r="I40">
-        <v>3.2460206564627931</v>
+        <v>2.8281829895669865</v>
       </c>
       <c r="J40">
-        <v>0.99226681948646744</v>
+        <v>0.98620667777240589</v>
       </c>
       <c r="K40">
-        <v>0.3489487209248201</v>
+        <v>0.32824117997917229</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -6931,31 +7296,31 @@
         <v>44952</v>
       </c>
       <c r="C41">
-        <v>1.4641520076038363</v>
+        <v>1.3217359777221946</v>
       </c>
       <c r="D41">
-        <v>2.0132090104552747</v>
+        <v>1.8173869693680174</v>
       </c>
       <c r="E41">
-        <v>33.629741424650618</v>
+        <v>30.358623238306656</v>
       </c>
       <c r="F41">
-        <v>3.7366379360722912</v>
+        <v>3.3731803598118515</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>40.843740378782016</v>
+        <v>36.870926545208718</v>
       </c>
       <c r="I41">
-        <v>11.165302841169584</v>
+        <v>9.6454546640787058</v>
       </c>
       <c r="J41">
-        <v>0.99914388713482938</v>
+        <v>0.99825010121612701</v>
       </c>
       <c r="K41">
-        <v>0.42712663218014496</v>
+        <v>0.40177980700363841</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -6963,31 +7328,31 @@
         <v>44953</v>
       </c>
       <c r="C42">
-        <v>1.9701271928745332</v>
+        <v>1.7550605016760175</v>
       </c>
       <c r="D42">
-        <v>2.7089248902024825</v>
+        <v>2.4132081898045237</v>
       </c>
       <c r="E42">
-        <v>45.251358961336926</v>
+        <v>40.311545897871021</v>
       </c>
       <c r="F42">
-        <v>5.0279287734818814</v>
+        <v>4.4790606553190031</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>54.958339817895826</v>
+        <v>48.958875244670566</v>
       </c>
       <c r="I42">
-        <v>14.11459943911381</v>
+        <v>12.087948699461847</v>
       </c>
       <c r="J42">
-        <v>0.99989856999543736</v>
+        <v>0.9997645107001577</v>
       </c>
       <c r="K42">
-        <v>0.5026844821313492</v>
+        <v>0.47285385409841441</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -6995,31 +7360,31 @@
         <v>44954</v>
       </c>
       <c r="C43">
-        <v>2.7828050302780944</v>
+        <v>2.4488471902102389</v>
       </c>
       <c r="D43">
-        <v>3.826356916632379</v>
+        <v>3.3671648865390775</v>
       </c>
       <c r="E43">
-        <v>63.917553039199966</v>
+        <v>56.246958900141408</v>
       </c>
       <c r="F43">
-        <v>7.1019503376888879</v>
+        <v>6.2496621000157146</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>77.628665323799339</v>
+        <v>68.312633076906451</v>
       </c>
       <c r="I43">
-        <v>22.670325505903513</v>
+        <v>19.353757832235885</v>
       </c>
       <c r="J43">
-        <v>0.99999271626123865</v>
+        <v>0.99998022615321358</v>
       </c>
       <c r="K43">
-        <v>0.5959485068923972</v>
+        <v>0.56058334471250559</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -7027,31 +7392,31 @@
         <v>44955</v>
       </c>
       <c r="C44">
-        <v>3.3028993915675144</v>
+        <v>2.8943128418798212</v>
       </c>
       <c r="D44">
-        <v>4.5414866634053324</v>
+        <v>3.9796801575847534</v>
       </c>
       <c r="E44">
-        <v>75.863470400066333</v>
+        <v>66.478748086927126</v>
       </c>
       <c r="F44">
-        <v>8.4292744888962634</v>
+        <v>7.3865275652141271</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>92.13713094393546</v>
+        <v>80.739268651605826</v>
       </c>
       <c r="I44">
-        <v>14.508465620136121</v>
+        <v>12.426635574699375</v>
       </c>
       <c r="J44">
-        <v>0.99999819521272737</v>
+        <v>0.99999467739480674</v>
       </c>
       <c r="K44">
-        <v>0.64535305368135432</v>
+        <v>0.60705609489586954</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -7059,31 +7424,31 @@
         <v>44956</v>
       </c>
       <c r="C45">
-        <v>4.4449302938747888</v>
+        <v>3.883658272780584</v>
       </c>
       <c r="D45">
-        <v>6.1117791540778326</v>
+        <v>5.3400301250733015</v>
       </c>
       <c r="E45">
-        <v>102.09449268743653</v>
+        <v>89.202775952929031</v>
       </c>
       <c r="F45">
-        <v>11.343832520826284</v>
+        <v>9.9114195503254496</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
       <c r="H45">
-        <v>123.99503465621545</v>
+        <v>108.33788390110836</v>
       </c>
       <c r="I45">
-        <v>31.857903712279992</v>
+        <v>27.598615249502529</v>
       </c>
       <c r="J45">
-        <v>0.99999987035220539</v>
+        <v>0.99999955297412213</v>
       </c>
       <c r="K45">
-        <v>0.73860147596266168</v>
+        <v>0.69477090892267568</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -7091,31 +7456,31 @@
         <v>44957</v>
       </c>
       <c r="C46">
-        <v>4.9313574074792328</v>
+        <v>4.3117699299026784</v>
       </c>
       <c r="D46">
-        <v>6.7806164352839451</v>
+        <v>5.928683653616182</v>
       </c>
       <c r="E46">
-        <v>113.26711545303863</v>
+        <v>99.035965577452146</v>
       </c>
       <c r="F46">
-        <v>12.58523505033763</v>
+        <v>11.003996175272464</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>137.56432434613944</v>
+        <v>120.28041533624346</v>
       </c>
       <c r="I46">
-        <v>13.569289689923991</v>
+        <v>11.942531435135109</v>
       </c>
       <c r="J46">
-        <v>0.99999995287276255</v>
+        <v>0.99999982744788474</v>
       </c>
       <c r="K46">
-        <v>0.7744355423380993</v>
+        <v>0.72847848692826955</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -7123,31 +7488,31 @@
         <v>44958</v>
       </c>
       <c r="C47">
-        <v>6.2185302216902407</v>
+        <v>5.4710632139814965</v>
       </c>
       <c r="D47">
-        <v>8.5504790548240788</v>
+        <v>7.5227119192245553</v>
       </c>
       <c r="E47">
-        <v>142.83186602944767</v>
+        <v>125.66348319613746</v>
       </c>
       <c r="F47">
-        <v>15.870207336605302</v>
+        <v>13.962609244015278</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47">
-        <v>173.4710826425673</v>
+        <v>152.61986757335882</v>
       </c>
       <c r="I47">
-        <v>35.906758296427853</v>
+        <v>32.339452237115353</v>
       </c>
       <c r="J47">
-        <v>0.99999999623016689</v>
+        <v>0.99999998396509482</v>
       </c>
       <c r="K47">
-        <v>0.86387532367869146</v>
+        <v>0.81261067485120564</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -7155,31 +7520,31 @@
         <v>44959</v>
       </c>
       <c r="C48">
-        <v>6.8764219213981645</v>
+        <v>6.0816390949054302</v>
       </c>
       <c r="D48">
-        <v>9.4550801419224744</v>
+        <v>8.3622537554949652</v>
       </c>
       <c r="E48">
-        <v>157.94281600711406</v>
+        <v>139.68764796110906</v>
       </c>
       <c r="F48">
-        <v>17.549201778568236</v>
+        <v>15.520849773456568</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
-        <v>191.82351984900293</v>
+        <v>169.65239058496607</v>
       </c>
       <c r="I48">
-        <v>18.352437206435638</v>
+        <v>17.032523011607253</v>
       </c>
       <c r="J48">
-        <v>0.99999999893033653</v>
+        <v>0.99999999509706305</v>
       </c>
       <c r="K48">
-        <v>0.90848106795902406</v>
+        <v>0.85456939617169458</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -7187,31 +7552,31 @@
         <v>44960</v>
       </c>
       <c r="C49">
-        <v>8.3236359770049315</v>
+        <v>7.4793779856040734</v>
       </c>
       <c r="D49">
-        <v>11.444999468381779</v>
+        <v>10.284144730205599</v>
       </c>
       <c r="E49">
-        <v>191.183513846832</v>
+        <v>171.79196310684353</v>
       </c>
       <c r="F49">
-        <v>21.242612649648006</v>
+        <v>19.087995900760397</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
-        <v>232.19476194186674</v>
+        <v>208.64348172341363</v>
       </c>
       <c r="I49">
-        <v>40.37124209286381</v>
+        <v>38.991091138447558</v>
       </c>
       <c r="J49">
-        <v>0.99999999993860578</v>
+        <v>0.99999999966658248</v>
       </c>
       <c r="K49">
-        <v>1.0096756976515484</v>
+        <v>0.94975886862425551</v>
       </c>
     </row>
     <row r="50" spans="2:11">
@@ -7219,31 +7584,31 @@
         <v>44961</v>
       </c>
       <c r="C50">
-        <v>9.2445077455772076</v>
+        <v>8.4168188368175141</v>
       </c>
       <c r="D50">
-        <v>12.711198150168658</v>
+        <v>11.573125900624081</v>
       </c>
       <c r="E50">
-        <v>212.33478728122648</v>
+        <v>193.32380765815228</v>
       </c>
       <c r="F50">
-        <v>23.592754142358501</v>
+        <v>21.480423073128037</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
       <c r="H50">
-        <v>257.88324731933085</v>
+        <v>234.79417546872193</v>
       </c>
       <c r="I50">
-        <v>25.688485377464104</v>
+        <v>26.150693745308303</v>
       </c>
       <c r="J50">
-        <v>0.99999999999172928</v>
+        <v>0.99999999994941002</v>
       </c>
       <c r="K50">
-        <v>1.0806589412892906</v>
+        <v>1.0165297786555361</v>
       </c>
     </row>
     <row r="51" spans="2:11">
@@ -7251,31 +7616,31 @@
         <v>44962</v>
       </c>
       <c r="C51">
-        <v>10.141371478468965</v>
+        <v>9.3751509436163669</v>
       </c>
       <c r="D51">
-        <v>13.944385782894825</v>
+        <v>12.890832547472501</v>
       </c>
       <c r="E51">
-        <v>232.93462614608401</v>
+        <v>215.33549823618836</v>
       </c>
       <c r="F51">
-        <v>25.881625127342673</v>
+        <v>23.926166470687601</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
       <c r="H51">
-        <v>282.90200853479053</v>
+        <v>261.52764819796488</v>
       </c>
       <c r="I51">
-        <v>25.018761215459676</v>
+        <v>26.733472729242948</v>
       </c>
       <c r="J51">
-        <v>0.99999999999912781</v>
+        <v>0.99999999999390354</v>
       </c>
       <c r="K51">
-        <v>1.1603155175697402</v>
+        <v>1.0914593228077525</v>
       </c>
     </row>
     <row r="52" spans="2:11">
@@ -7283,31 +7648,31 @@
         <v>44963</v>
       </c>
       <c r="C52">
-        <v>10.400099866147247</v>
+        <v>9.6614162956291114</v>
       </c>
       <c r="D52">
-        <v>14.300137315952462</v>
+        <v>13.284447406490028</v>
       </c>
       <c r="E52">
-        <v>238.87729380056956</v>
+        <v>221.91065554023115</v>
       </c>
       <c r="F52">
-        <v>26.541921533396625</v>
+        <v>24.656739504470135</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>290.11945251606591</v>
+        <v>269.51325874682044</v>
       </c>
       <c r="I52">
-        <v>7.2174439812753803</v>
+        <v>7.9856105488555613</v>
       </c>
       <c r="J52">
-        <v>0.99999999999958233</v>
+        <v>0.99999999999694933</v>
       </c>
       <c r="K52">
-        <v>1.1863773205536725</v>
+        <v>1.115974549403679</v>
       </c>
     </row>
     <row r="53" spans="2:11">
@@ -7315,31 +7680,31 @@
         <v>44964</v>
       </c>
       <c r="C53">
-        <v>10.779416313943202</v>
+        <v>10.090221512713546</v>
       </c>
       <c r="D53">
-        <v>14.821697431671897</v>
+        <v>13.874054579981122</v>
       </c>
       <c r="E53">
-        <v>247.58971846088284</v>
+        <v>231.75977537013921</v>
       </c>
       <c r="F53">
-        <v>27.509968717875878</v>
+        <v>25.751086152237701</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>300.70080092437382</v>
+        <v>281.47513761507156</v>
       </c>
       <c r="I53">
-        <v>10.581348408307917</v>
+        <v>11.961878868251119</v>
       </c>
       <c r="J53">
-        <v>0.99999999999987188</v>
+        <v>0.99999999999899702</v>
       </c>
       <c r="K53">
-        <v>1.2</v>
+        <v>1.1553615573806109</v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -7347,31 +7712,31 @@
         <v>44965</v>
       </c>
       <c r="C54">
-        <v>11.065390171261214</v>
+        <v>10.421396655229284</v>
       </c>
       <c r="D54">
-        <v>15.214911485484166</v>
+        <v>14.329420400940263</v>
       </c>
       <c r="E54">
-        <v>254.15818049615598</v>
+        <v>239.36645442479758</v>
       </c>
       <c r="F54">
-        <v>28.239797832906227</v>
+        <v>26.596272713866409</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>308.67827998580765</v>
+        <v>290.71354419483356</v>
       </c>
       <c r="I54">
-        <v>7.9774790614338258</v>
+        <v>9.2384065797619996</v>
       </c>
       <c r="J54">
-        <v>0.9999999999999527</v>
+        <v>0.99999999999960765</v>
       </c>
       <c r="K54">
-        <v>1.2</v>
+        <v>1.1886039617155066</v>
       </c>
     </row>
     <row r="55" spans="2:11">
@@ -7379,28 +7744,28 @@
         <v>44966</v>
       </c>
       <c r="C55">
-        <v>11.685163262837966</v>
+        <v>11.166380440125588</v>
       </c>
       <c r="D55">
-        <v>16.067099486402199</v>
+        <v>15.35377310517268</v>
       </c>
       <c r="E55">
-        <v>268.39359369330947</v>
+        <v>256.47780073413452</v>
       </c>
       <c r="F55">
-        <v>29.821510410367726</v>
+        <v>28.497533414903845</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>325.96736685291739</v>
+        <v>311.4954876943367</v>
       </c>
       <c r="I55">
-        <v>17.289086867109745</v>
+        <v>20.781943499503143</v>
       </c>
       <c r="J55">
-        <v>0.99960599385063065</v>
+        <v>0.9999999999999678</v>
       </c>
       <c r="K55">
         <v>1.2</v>
@@ -7411,28 +7776,28 @@
         <v>44967</v>
       </c>
       <c r="C56">
-        <v>12.101695800803148</v>
+        <v>11.692727695360439</v>
       </c>
       <c r="D56">
-        <v>16.639831726104326</v>
+        <v>16.077500581120599</v>
       </c>
       <c r="E56">
-        <v>277.96082542469725</v>
+        <v>268.56733925281003</v>
       </c>
       <c r="F56">
-        <v>30.884536158299703</v>
+        <v>29.840815472534455</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>337.58688910990446</v>
+        <v>326.17838300182558</v>
       </c>
       <c r="I56">
-        <v>11.619522256987068</v>
+        <v>14.682895307488877</v>
       </c>
       <c r="J56">
-        <v>0.85679685776854186</v>
+        <v>0.99738015904888566</v>
       </c>
       <c r="K56">
         <v>1.2</v>
@@ -7443,28 +7808,28 @@
         <v>44968</v>
       </c>
       <c r="C57">
-        <v>12.49690247240852</v>
+        <v>12.217902966359345</v>
       </c>
       <c r="D57">
-        <v>17.183240899561714</v>
+        <v>16.799616578744097</v>
       </c>
       <c r="E57">
-        <v>287.03822866313317</v>
+        <v>280.6299587585662</v>
       </c>
       <c r="F57">
-        <v>31.893136518125917</v>
+        <v>31.181106528729583</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>348.61150855322938</v>
+        <v>340.8285848323992</v>
       </c>
       <c r="I57">
-        <v>11.024619443324923</v>
+        <v>14.650201830573621</v>
       </c>
       <c r="J57">
-        <v>0.65421244754302488</v>
+        <v>0.80681764407083278</v>
       </c>
       <c r="K57">
         <v>1.2</v>
@@ -7475,28 +7840,28 @@
         <v>44969</v>
       </c>
       <c r="C58">
-        <v>12.665233887387556</v>
+        <v>12.452025304349887</v>
       </c>
       <c r="D58">
-        <v>17.414696595157888</v>
+        <v>17.121534793481093</v>
       </c>
       <c r="E58">
-        <v>290.90459085093289</v>
+        <v>286.00745620928643</v>
       </c>
       <c r="F58">
-        <v>32.322732316770328</v>
+        <v>31.778606245476279</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>353.30725365024875</v>
+        <v>347.35962255259375</v>
       </c>
       <c r="I58">
-        <v>4.695745097019369</v>
+        <v>6.5310377201945471</v>
       </c>
       <c r="J58">
-        <v>0.52256405645422088</v>
+        <v>0.68298161704994975</v>
       </c>
       <c r="K58">
         <v>1.2</v>
@@ -7507,28 +7872,28 @@
         <v>44970</v>
       </c>
       <c r="C59">
-        <v>12.808284813701666</v>
+        <v>12.657982785372736</v>
       </c>
       <c r="D59">
-        <v>17.611391618839786</v>
+        <v>17.404726329887506</v>
       </c>
       <c r="E59">
-        <v>294.19029181471012</v>
+        <v>290.73804210152997</v>
       </c>
       <c r="F59">
-        <v>32.687810201634463</v>
+        <v>32.304226900170008</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>357.29777844888605</v>
+        <v>353.10497811696024</v>
       </c>
       <c r="I59">
-        <v>3.9905247986372956</v>
+        <v>5.7453555643664913</v>
       </c>
       <c r="J59">
-        <v>0.3591352725761835</v>
+        <v>0.52925112988692158</v>
       </c>
       <c r="K59">
         <v>1.2</v>
@@ -7539,28 +7904,28 @@
         <v>44971</v>
       </c>
       <c r="C60">
-        <v>12.878405504849862</v>
+        <v>12.762144586383007</v>
       </c>
       <c r="D60">
-        <v>17.707807569168558</v>
+        <v>17.547948806276633</v>
       </c>
       <c r="E60">
-        <v>295.80087643952021</v>
+        <v>293.13050846848466</v>
       </c>
       <c r="F60">
-        <v>32.866764048835584</v>
+        <v>32.570056496498303</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>359.25385356237422</v>
+        <v>356.01065835764263</v>
       </c>
       <c r="I60">
-        <v>1.9560751134881684</v>
+        <v>2.9056802406823863</v>
       </c>
       <c r="J60">
-        <v>0.24282282182010295</v>
+        <v>0.41984096789733027</v>
       </c>
       <c r="K60">
         <v>1.2</v>
@@ -7571,28 +7936,28 @@
         <v>44972</v>
       </c>
       <c r="C61">
-        <v>12.957499478723086</v>
+        <v>12.883318601532229</v>
       </c>
       <c r="D61">
-        <v>17.816561783244239</v>
+        <v>17.71456307710681</v>
       </c>
       <c r="E61">
-        <v>297.61756615192081</v>
+        <v>295.91372412894333</v>
       </c>
       <c r="F61">
-        <v>33.068618461324547</v>
+        <v>32.879302680993717</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>361.46024587521276</v>
+        <v>359.39090848857614</v>
       </c>
       <c r="I61">
-        <v>2.2063923128385454</v>
+        <v>3.3802501309335184</v>
       </c>
       <c r="J61">
-        <v>4.4347630833892593E-2</v>
+        <v>0.2331438202097158</v>
       </c>
       <c r="K61">
         <v>1.2</v>
@@ -7603,28 +7968,28 @@
         <v>44973</v>
       </c>
       <c r="C62">
-        <v>12.997050336896374</v>
+        <v>12.946076762605795</v>
       </c>
       <c r="D62">
-        <v>17.870944213232512</v>
+        <v>17.800855548582966</v>
       </c>
       <c r="E62">
-        <v>298.52599992558856</v>
+        <v>297.35520064110182</v>
       </c>
       <c r="F62">
-        <v>33.169555547287622</v>
+        <v>33.039466737900213</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>362.56355002300506</v>
+        <v>361.14159969019079</v>
       </c>
       <c r="I62">
-        <v>1.1033041477923007</v>
+        <v>1.750691201614643</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>8.0441853961365939E-2</v>
       </c>
       <c r="K62">
         <v>1.2</v>
@@ -7635,25 +8000,25 @@
         <v>44974</v>
       </c>
       <c r="C63">
-        <v>13.026556156235843</v>
+        <v>12.994427297901929</v>
       </c>
       <c r="D63">
-        <v>17.911514714824282</v>
+        <v>17.86733753461515</v>
       </c>
       <c r="E63">
-        <v>299.20371171354196</v>
+        <v>298.46575199868488</v>
       </c>
       <c r="F63">
-        <v>33.244856857060235</v>
+        <v>33.162861333187223</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>363.38663944166234</v>
+        <v>362.4903781643892</v>
       </c>
       <c r="I63">
-        <v>0.82308941865727547</v>
+        <v>1.3487784741984115</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -7667,25 +8032,25 @@
         <v>44975</v>
       </c>
       <c r="C64">
-        <v>13.042393735799077</v>
+        <v>13.021253506266081</v>
       </c>
       <c r="D64">
-        <v>17.933291386723727</v>
+        <v>17.904223571115857</v>
       </c>
       <c r="E64">
-        <v>299.56748111913504</v>
+        <v>299.08191647204899</v>
       </c>
       <c r="F64">
-        <v>33.285275679903897</v>
+        <v>33.231324052449892</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>363.82844192156176</v>
+        <v>363.23871760188086</v>
       </c>
       <c r="I64">
-        <v>0.44180247989942245</v>
+        <v>0.74833943749166565</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -7699,25 +8064,25 @@
         <v>44976</v>
       </c>
       <c r="C65">
-        <v>13.054235569720101</v>
+        <v>13.042003028798327</v>
       </c>
       <c r="D65">
-        <v>17.949573908365135</v>
+        <v>17.932754164597693</v>
       </c>
       <c r="E65">
-        <v>299.83947324200852</v>
+        <v>299.55850706771156</v>
       </c>
       <c r="F65">
-        <v>33.315497026889844</v>
+        <v>33.28427856307907</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>364.15877974698361</v>
+        <v>363.81754282418666</v>
       </c>
       <c r="I65">
-        <v>0.33033782542185008</v>
+        <v>0.57882522230579525</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -7731,25 +8096,25 @@
         <v>44977</v>
       </c>
       <c r="C66">
-        <v>13.058838051481922</v>
+        <v>13.050338820683718</v>
       </c>
       <c r="D66">
-        <v>17.95590232078764</v>
+        <v>17.944215878440108</v>
       </c>
       <c r="E66">
-        <v>299.94518649497542</v>
+        <v>299.74996978757912</v>
       </c>
       <c r="F66">
-        <v>33.327242943886155</v>
+        <v>33.305552198619907</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>364.28716981113115</v>
+        <v>364.05007668532284</v>
       </c>
       <c r="I66">
-        <v>0.1283900641475384</v>
+        <v>0.2325338611361758</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -7759,35 +8124,35 @@
       </c>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K67" t="e">
-        <v>#N/A</v>
+      <c r="B67" s="28">
+        <v>44978</v>
+      </c>
+      <c r="C67">
+        <v>13.058838051481922</v>
+      </c>
+      <c r="D67">
+        <v>17.95590232078764</v>
+      </c>
+      <c r="E67">
+        <v>299.94518649497542</v>
+      </c>
+      <c r="F67">
+        <v>33.327242943886155</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>364.28716981113115</v>
+      </c>
+      <c r="I67">
+        <v>0.23709312580831465</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -7830,8 +8195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4474A41F-DE8A-4797-B435-AE89636818A9}">
   <dimension ref="A1:BE78"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E59" sqref="A1:AF78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>